<commit_message>
[Surface mode] - Correct coordination when Flip screen
</commit_message>
<xml_diff>
--- a/UserInterface/Scripts/DSX_CoordinationClear.xlsx
+++ b/UserInterface/Scripts/DSX_CoordinationClear.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ducth\Downloads\DSX_Projects_T6_ALL\UserInterface\Scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7DC0737-86B6-4557-B3BA-08201CC9B2C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCA8849C-929B-4FBA-A336-88E5D965D75F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3853,9 +3853,9 @@
   <dimension ref="A1:W218"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A199" zoomScale="103" zoomScaleNormal="103" workbookViewId="0">
-      <pane ySplit="6290" topLeftCell="A163" activePane="bottomLeft"/>
+      <pane ySplit="6290" topLeftCell="A209" activePane="bottomLeft"/>
       <selection activeCell="H215" sqref="H215"/>
-      <selection pane="bottomLeft" activeCell="H176" sqref="H176"/>
+      <selection pane="bottomLeft" activeCell="A231" sqref="A231"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -19053,8 +19053,8 @@
         <v>160</v>
       </c>
       <c r="M167" s="52">
-        <f t="shared" si="282"/>
-        <v>71</v>
+        <f>D167</f>
+        <v>47</v>
       </c>
       <c r="N167">
         <f t="shared" si="272"/>
@@ -19082,7 +19082,7 @@
       </c>
       <c r="T167" t="str">
         <f t="shared" si="275"/>
-        <v>static const CooGUI_tds Pos_GPS_Icon_Flipped = {160,71,128,15,64,105,192,120};</v>
+        <v>static const CooGUI_tds Pos_GPS_Icon_Flipped = {160,47,128,15,64,105,192,120};</v>
       </c>
       <c r="U167" t="str">
         <f t="shared" si="276"/>
@@ -19142,16 +19142,16 @@
         <v>160</v>
       </c>
       <c r="M168" s="52">
-        <f t="shared" si="282"/>
-        <v>84</v>
+        <f>D168</f>
+        <v>60</v>
       </c>
       <c r="N168">
         <f t="shared" si="272"/>
         <v>0</v>
       </c>
       <c r="O168">
-        <f t="shared" ref="O168:O173" si="291">F168 + $D$1</f>
-        <v>84</v>
+        <f>F168</f>
+        <v>60</v>
       </c>
       <c r="P168">
         <f t="shared" si="218"/>
@@ -19167,11 +19167,11 @@
       </c>
       <c r="S168" s="20">
         <f>O168+Q168</f>
-        <v>112</v>
+        <v>88</v>
       </c>
       <c r="T168" t="str">
         <f t="shared" si="275"/>
-        <v>static const CooGUI_tds Pos_GPS_Page_Txt_00_Flipped = {160,84,0,84,320,28,320,112};</v>
+        <v>static const CooGUI_tds Pos_GPS_Page_Txt_00_Flipped = {160,60,0,60,320,28,320,88};</v>
       </c>
       <c r="U168" t="str">
         <f t="shared" si="276"/>
@@ -19191,7 +19191,7 @@
         <v>158</v>
       </c>
       <c r="B169" t="str">
-        <f t="shared" ref="B169:B174" si="292">CONCATENATE(A169, "_Normal")</f>
+        <f t="shared" ref="B169:B174" si="291">CONCATENATE(A169, "_Normal")</f>
         <v>Pos_GPS_Page_Txt_01_Normal</v>
       </c>
       <c r="C169" s="22">
@@ -19210,71 +19210,71 @@
         <v>88</v>
       </c>
       <c r="G169" s="23">
-        <f t="shared" ref="G169:H173" si="293">G168</f>
+        <f t="shared" ref="G169:H173" si="292">G168</f>
         <v>320</v>
       </c>
       <c r="H169" s="23">
-        <f t="shared" si="293"/>
+        <f t="shared" si="292"/>
         <v>28</v>
       </c>
       <c r="I169" s="20">
-        <f t="shared" ref="I169:I174" si="294">E169+G169</f>
+        <f t="shared" ref="I169:I174" si="293">E169+G169</f>
         <v>320</v>
       </c>
       <c r="J169" s="20">
-        <f t="shared" ref="J169:J174" si="295">F169+H169</f>
+        <f t="shared" ref="J169:J174" si="294">F169+H169</f>
         <v>116</v>
       </c>
       <c r="K169" t="str">
-        <f t="shared" ref="K169:K174" si="296">CONCATENATE("static const CooGUI_tds ",A169, "_Normal = {", C169, ",", D169, ",", E169, ",", F169, ",",G169, ",", H169,",",  I169, ",", J169, "};")</f>
+        <f t="shared" ref="K169:K174" si="295">CONCATENATE("static const CooGUI_tds ",A169, "_Normal = {", C169, ",", D169, ",", E169, ",", F169, ",",G169, ",", H169,",",  I169, ",", J169, "};")</f>
         <v>static const CooGUI_tds Pos_GPS_Page_Txt_01_Normal = {160,88,0,88,320,28,320,116};</v>
       </c>
       <c r="L169">
-        <f t="shared" ref="L169:L174" si="297">C169</f>
+        <f t="shared" ref="L169:L174" si="296">C169</f>
         <v>160</v>
       </c>
       <c r="M169" s="52">
-        <f t="shared" si="282"/>
-        <v>112</v>
+        <f t="shared" ref="M169:M173" si="297">D169</f>
+        <v>88</v>
       </c>
       <c r="N169">
         <f t="shared" ref="N169:N174" si="298">E169</f>
         <v>0</v>
       </c>
       <c r="O169">
-        <f t="shared" si="291"/>
-        <v>112</v>
+        <f t="shared" ref="O169:O173" si="299">F169</f>
+        <v>88</v>
       </c>
       <c r="P169">
-        <f t="shared" ref="P169:P174" si="299">G169</f>
+        <f t="shared" ref="P169:P174" si="300">G169</f>
         <v>320</v>
       </c>
       <c r="Q169">
-        <f t="shared" ref="Q169:Q174" si="300">H169</f>
+        <f t="shared" ref="Q169:Q174" si="301">H169</f>
         <v>28</v>
       </c>
       <c r="R169" s="20">
-        <f t="shared" ref="R169:R174" si="301">N169+P169</f>
+        <f t="shared" ref="R169:R174" si="302">N169+P169</f>
         <v>320</v>
       </c>
       <c r="S169" s="20">
-        <f t="shared" ref="S169:S174" si="302">O169+Q169</f>
-        <v>140</v>
+        <f t="shared" ref="S169:S174" si="303">O169+Q169</f>
+        <v>116</v>
       </c>
       <c r="T169" t="str">
-        <f t="shared" ref="T169:T174" si="303">CONCATENATE("static const CooGUI_tds ",A169, "_Flipped = {", L169, ",", M169, ",", N169, ",", O169, ",",P169, ",", Q169,",",  R169, ",", S169, "};")</f>
-        <v>static const CooGUI_tds Pos_GPS_Page_Txt_01_Flipped = {160,112,0,112,320,28,320,140};</v>
+        <f t="shared" ref="T169:T174" si="304">CONCATENATE("static const CooGUI_tds ",A169, "_Flipped = {", L169, ",", M169, ",", N169, ",", O169, ",",P169, ",", Q169,",",  R169, ",", S169, "};")</f>
+        <v>static const CooGUI_tds Pos_GPS_Page_Txt_01_Flipped = {160,88,0,88,320,28,320,116};</v>
       </c>
       <c r="U169" t="str">
-        <f t="shared" ref="U169:U174" si="304">CONCATENATE("const CooGUI_tds* ",A169, ";")</f>
+        <f t="shared" ref="U169:U174" si="305">CONCATENATE("const CooGUI_tds* ",A169, ";")</f>
         <v>const CooGUI_tds* Pos_GPS_Page_Txt_01;</v>
       </c>
       <c r="V169">
-        <f t="shared" ref="V169:V174" si="305">(G169*H169)/1024</f>
+        <f t="shared" ref="V169:V174" si="306">(G169*H169)/1024</f>
         <v>8.75</v>
       </c>
       <c r="W169" t="str">
-        <f t="shared" ref="W169:W174" si="306">CONCATENATE(A169, " = &amp;", B169,";")</f>
+        <f t="shared" ref="W169:W174" si="307">CONCATENATE(A169, " = &amp;", B169,";")</f>
         <v>Pos_GPS_Page_Txt_01 = &amp;Pos_GPS_Page_Txt_01_Normal;</v>
       </c>
     </row>
@@ -19283,7 +19283,7 @@
         <v>159</v>
       </c>
       <c r="B170" t="str">
-        <f t="shared" si="292"/>
+        <f t="shared" si="291"/>
         <v>Pos_GPS_Page_Txt_02_Normal</v>
       </c>
       <c r="C170" s="22">
@@ -19302,71 +19302,71 @@
         <v>116</v>
       </c>
       <c r="G170" s="23">
+        <f t="shared" si="292"/>
+        <v>320</v>
+      </c>
+      <c r="H170" s="23">
+        <f t="shared" si="292"/>
+        <v>28</v>
+      </c>
+      <c r="I170" s="20">
         <f t="shared" si="293"/>
         <v>320</v>
       </c>
-      <c r="H170" s="23">
-        <f t="shared" si="293"/>
-        <v>28</v>
-      </c>
-      <c r="I170" s="20">
+      <c r="J170" s="20">
         <f t="shared" si="294"/>
-        <v>320</v>
-      </c>
-      <c r="J170" s="20">
+        <v>144</v>
+      </c>
+      <c r="K170" t="str">
         <f t="shared" si="295"/>
-        <v>144</v>
-      </c>
-      <c r="K170" t="str">
+        <v>static const CooGUI_tds Pos_GPS_Page_Txt_02_Normal = {160,116,0,116,320,28,320,144};</v>
+      </c>
+      <c r="L170">
         <f t="shared" si="296"/>
-        <v>static const CooGUI_tds Pos_GPS_Page_Txt_02_Normal = {160,116,0,116,320,28,320,144};</v>
-      </c>
-      <c r="L170">
+        <v>160</v>
+      </c>
+      <c r="M170" s="52">
         <f t="shared" si="297"/>
-        <v>160</v>
-      </c>
-      <c r="M170" s="52">
-        <f t="shared" si="282"/>
-        <v>140</v>
+        <v>116</v>
       </c>
       <c r="N170">
         <f t="shared" si="298"/>
         <v>0</v>
       </c>
       <c r="O170">
-        <f t="shared" si="291"/>
-        <v>140</v>
+        <f t="shared" si="299"/>
+        <v>116</v>
       </c>
       <c r="P170">
-        <f t="shared" si="299"/>
+        <f t="shared" si="300"/>
         <v>320</v>
       </c>
       <c r="Q170">
-        <f t="shared" si="300"/>
+        <f t="shared" si="301"/>
         <v>28</v>
       </c>
       <c r="R170" s="20">
-        <f t="shared" si="301"/>
+        <f t="shared" si="302"/>
         <v>320</v>
       </c>
       <c r="S170" s="20">
-        <f t="shared" si="302"/>
-        <v>168</v>
+        <f t="shared" si="303"/>
+        <v>144</v>
       </c>
       <c r="T170" t="str">
-        <f t="shared" si="303"/>
-        <v>static const CooGUI_tds Pos_GPS_Page_Txt_02_Flipped = {160,140,0,140,320,28,320,168};</v>
+        <f t="shared" si="304"/>
+        <v>static const CooGUI_tds Pos_GPS_Page_Txt_02_Flipped = {160,116,0,116,320,28,320,144};</v>
       </c>
       <c r="U170" t="str">
-        <f t="shared" si="304"/>
+        <f t="shared" si="305"/>
         <v>const CooGUI_tds* Pos_GPS_Page_Txt_02;</v>
       </c>
       <c r="V170">
-        <f t="shared" si="305"/>
+        <f t="shared" si="306"/>
         <v>8.75</v>
       </c>
       <c r="W170" t="str">
-        <f t="shared" si="306"/>
+        <f t="shared" si="307"/>
         <v>Pos_GPS_Page_Txt_02 = &amp;Pos_GPS_Page_Txt_02_Normal;</v>
       </c>
     </row>
@@ -19375,7 +19375,7 @@
         <v>160</v>
       </c>
       <c r="B171" t="str">
-        <f t="shared" si="292"/>
+        <f t="shared" si="291"/>
         <v>Pos_GPS_Page_Txt_03_Normal</v>
       </c>
       <c r="C171" s="22">
@@ -19394,71 +19394,71 @@
         <v>144</v>
       </c>
       <c r="G171" s="23">
+        <f t="shared" si="292"/>
+        <v>320</v>
+      </c>
+      <c r="H171" s="23">
+        <f t="shared" si="292"/>
+        <v>28</v>
+      </c>
+      <c r="I171" s="20">
         <f t="shared" si="293"/>
         <v>320</v>
       </c>
-      <c r="H171" s="23">
-        <f t="shared" si="293"/>
-        <v>28</v>
-      </c>
-      <c r="I171" s="20">
+      <c r="J171" s="20">
         <f t="shared" si="294"/>
-        <v>320</v>
-      </c>
-      <c r="J171" s="20">
+        <v>172</v>
+      </c>
+      <c r="K171" t="str">
         <f t="shared" si="295"/>
-        <v>172</v>
-      </c>
-      <c r="K171" t="str">
+        <v>static const CooGUI_tds Pos_GPS_Page_Txt_03_Normal = {160,144,0,144,320,28,320,172};</v>
+      </c>
+      <c r="L171">
         <f t="shared" si="296"/>
-        <v>static const CooGUI_tds Pos_GPS_Page_Txt_03_Normal = {160,144,0,144,320,28,320,172};</v>
-      </c>
-      <c r="L171">
+        <v>160</v>
+      </c>
+      <c r="M171" s="52">
         <f t="shared" si="297"/>
-        <v>160</v>
-      </c>
-      <c r="M171" s="52">
-        <f t="shared" si="282"/>
-        <v>168</v>
+        <v>144</v>
       </c>
       <c r="N171">
         <f t="shared" si="298"/>
         <v>0</v>
       </c>
       <c r="O171">
-        <f t="shared" si="291"/>
-        <v>168</v>
+        <f t="shared" si="299"/>
+        <v>144</v>
       </c>
       <c r="P171">
-        <f t="shared" si="299"/>
+        <f t="shared" si="300"/>
         <v>320</v>
       </c>
       <c r="Q171">
-        <f t="shared" si="300"/>
+        <f t="shared" si="301"/>
         <v>28</v>
       </c>
       <c r="R171" s="20">
-        <f t="shared" si="301"/>
+        <f t="shared" si="302"/>
         <v>320</v>
       </c>
       <c r="S171" s="20">
-        <f t="shared" si="302"/>
-        <v>196</v>
+        <f t="shared" si="303"/>
+        <v>172</v>
       </c>
       <c r="T171" t="str">
-        <f t="shared" si="303"/>
-        <v>static const CooGUI_tds Pos_GPS_Page_Txt_03_Flipped = {160,168,0,168,320,28,320,196};</v>
+        <f t="shared" si="304"/>
+        <v>static const CooGUI_tds Pos_GPS_Page_Txt_03_Flipped = {160,144,0,144,320,28,320,172};</v>
       </c>
       <c r="U171" t="str">
-        <f t="shared" si="304"/>
+        <f t="shared" si="305"/>
         <v>const CooGUI_tds* Pos_GPS_Page_Txt_03;</v>
       </c>
       <c r="V171">
-        <f t="shared" si="305"/>
+        <f t="shared" si="306"/>
         <v>8.75</v>
       </c>
       <c r="W171" t="str">
-        <f t="shared" si="306"/>
+        <f t="shared" si="307"/>
         <v>Pos_GPS_Page_Txt_03 = &amp;Pos_GPS_Page_Txt_03_Normal;</v>
       </c>
     </row>
@@ -19467,7 +19467,7 @@
         <v>161</v>
       </c>
       <c r="B172" t="str">
-        <f t="shared" si="292"/>
+        <f t="shared" si="291"/>
         <v>Pos_GPS_Page_Txt_04_Normal</v>
       </c>
       <c r="C172" s="22">
@@ -19486,71 +19486,71 @@
         <v>172</v>
       </c>
       <c r="G172" s="23">
+        <f t="shared" si="292"/>
+        <v>320</v>
+      </c>
+      <c r="H172" s="23">
+        <f t="shared" si="292"/>
+        <v>28</v>
+      </c>
+      <c r="I172" s="20">
         <f t="shared" si="293"/>
         <v>320</v>
       </c>
-      <c r="H172" s="23">
-        <f t="shared" si="293"/>
-        <v>28</v>
-      </c>
-      <c r="I172" s="20">
+      <c r="J172" s="20">
         <f t="shared" si="294"/>
-        <v>320</v>
-      </c>
-      <c r="J172" s="20">
+        <v>200</v>
+      </c>
+      <c r="K172" t="str">
         <f t="shared" si="295"/>
-        <v>200</v>
-      </c>
-      <c r="K172" t="str">
+        <v>static const CooGUI_tds Pos_GPS_Page_Txt_04_Normal = {160,172,0,172,320,28,320,200};</v>
+      </c>
+      <c r="L172">
         <f t="shared" si="296"/>
-        <v>static const CooGUI_tds Pos_GPS_Page_Txt_04_Normal = {160,172,0,172,320,28,320,200};</v>
-      </c>
-      <c r="L172">
+        <v>160</v>
+      </c>
+      <c r="M172" s="52">
         <f t="shared" si="297"/>
-        <v>160</v>
-      </c>
-      <c r="M172" s="52">
-        <f t="shared" si="282"/>
-        <v>196</v>
+        <v>172</v>
       </c>
       <c r="N172">
         <f t="shared" si="298"/>
         <v>0</v>
       </c>
       <c r="O172">
-        <f t="shared" si="291"/>
-        <v>196</v>
+        <f t="shared" si="299"/>
+        <v>172</v>
       </c>
       <c r="P172">
-        <f t="shared" si="299"/>
+        <f t="shared" si="300"/>
         <v>320</v>
       </c>
       <c r="Q172">
-        <f t="shared" si="300"/>
+        <f t="shared" si="301"/>
         <v>28</v>
       </c>
       <c r="R172" s="20">
-        <f t="shared" si="301"/>
+        <f t="shared" si="302"/>
         <v>320</v>
       </c>
       <c r="S172" s="20">
-        <f t="shared" si="302"/>
-        <v>224</v>
+        <f t="shared" si="303"/>
+        <v>200</v>
       </c>
       <c r="T172" t="str">
-        <f t="shared" si="303"/>
-        <v>static const CooGUI_tds Pos_GPS_Page_Txt_04_Flipped = {160,196,0,196,320,28,320,224};</v>
+        <f t="shared" si="304"/>
+        <v>static const CooGUI_tds Pos_GPS_Page_Txt_04_Flipped = {160,172,0,172,320,28,320,200};</v>
       </c>
       <c r="U172" t="str">
-        <f t="shared" si="304"/>
+        <f t="shared" si="305"/>
         <v>const CooGUI_tds* Pos_GPS_Page_Txt_04;</v>
       </c>
       <c r="V172">
-        <f t="shared" si="305"/>
+        <f t="shared" si="306"/>
         <v>8.75</v>
       </c>
       <c r="W172" t="str">
-        <f t="shared" si="306"/>
+        <f t="shared" si="307"/>
         <v>Pos_GPS_Page_Txt_04 = &amp;Pos_GPS_Page_Txt_04_Normal;</v>
       </c>
     </row>
@@ -19559,7 +19559,7 @@
         <v>162</v>
       </c>
       <c r="B173" t="str">
-        <f t="shared" si="292"/>
+        <f t="shared" si="291"/>
         <v>Pos_GPS_Page_Txt_05_Normal</v>
       </c>
       <c r="C173" s="22">
@@ -19578,71 +19578,71 @@
         <v>200</v>
       </c>
       <c r="G173" s="23">
+        <f t="shared" si="292"/>
+        <v>320</v>
+      </c>
+      <c r="H173" s="23">
+        <f t="shared" si="292"/>
+        <v>28</v>
+      </c>
+      <c r="I173" s="20">
         <f t="shared" si="293"/>
         <v>320</v>
       </c>
-      <c r="H173" s="23">
-        <f t="shared" si="293"/>
-        <v>28</v>
-      </c>
-      <c r="I173" s="20">
+      <c r="J173" s="20">
         <f t="shared" si="294"/>
-        <v>320</v>
-      </c>
-      <c r="J173" s="20">
+        <v>228</v>
+      </c>
+      <c r="K173" t="str">
         <f t="shared" si="295"/>
-        <v>228</v>
-      </c>
-      <c r="K173" t="str">
+        <v>static const CooGUI_tds Pos_GPS_Page_Txt_05_Normal = {160,200,0,200,320,28,320,228};</v>
+      </c>
+      <c r="L173">
         <f t="shared" si="296"/>
-        <v>static const CooGUI_tds Pos_GPS_Page_Txt_05_Normal = {160,200,0,200,320,28,320,228};</v>
-      </c>
-      <c r="L173">
+        <v>160</v>
+      </c>
+      <c r="M173" s="52">
         <f t="shared" si="297"/>
-        <v>160</v>
-      </c>
-      <c r="M173" s="52">
-        <f t="shared" si="282"/>
-        <v>224</v>
+        <v>200</v>
       </c>
       <c r="N173">
         <f t="shared" si="298"/>
         <v>0</v>
       </c>
       <c r="O173">
-        <f t="shared" si="291"/>
-        <v>224</v>
+        <f t="shared" si="299"/>
+        <v>200</v>
       </c>
       <c r="P173">
-        <f t="shared" si="299"/>
+        <f t="shared" si="300"/>
         <v>320</v>
       </c>
       <c r="Q173">
-        <f t="shared" si="300"/>
+        <f t="shared" si="301"/>
         <v>28</v>
       </c>
       <c r="R173" s="20">
-        <f t="shared" si="301"/>
+        <f t="shared" si="302"/>
         <v>320</v>
       </c>
       <c r="S173" s="20">
-        <f t="shared" si="302"/>
-        <v>252</v>
+        <f t="shared" si="303"/>
+        <v>228</v>
       </c>
       <c r="T173" t="str">
-        <f t="shared" si="303"/>
-        <v>static const CooGUI_tds Pos_GPS_Page_Txt_05_Flipped = {160,224,0,224,320,28,320,252};</v>
+        <f t="shared" si="304"/>
+        <v>static const CooGUI_tds Pos_GPS_Page_Txt_05_Flipped = {160,200,0,200,320,28,320,228};</v>
       </c>
       <c r="U173" t="str">
-        <f t="shared" si="304"/>
+        <f t="shared" si="305"/>
         <v>const CooGUI_tds* Pos_GPS_Page_Txt_05;</v>
       </c>
       <c r="V173">
-        <f t="shared" si="305"/>
+        <f t="shared" si="306"/>
         <v>8.75</v>
       </c>
       <c r="W173" t="str">
-        <f t="shared" si="306"/>
+        <f t="shared" si="307"/>
         <v>Pos_GPS_Page_Txt_05 = &amp;Pos_GPS_Page_Txt_05_Normal;</v>
       </c>
     </row>
@@ -19651,7 +19651,7 @@
         <v>180</v>
       </c>
       <c r="B174" t="str">
-        <f t="shared" si="292"/>
+        <f t="shared" si="291"/>
         <v>Pos_Bluetooth_PasscodeTxt_Normal</v>
       </c>
       <c r="C174" s="22">
@@ -19675,24 +19675,24 @@
         <v>25</v>
       </c>
       <c r="I174" s="20">
+        <f t="shared" si="293"/>
+        <v>235</v>
+      </c>
+      <c r="J174" s="20">
         <f t="shared" si="294"/>
-        <v>235</v>
-      </c>
-      <c r="J174" s="20">
+        <v>140</v>
+      </c>
+      <c r="K174" t="str">
         <f t="shared" si="295"/>
-        <v>140</v>
-      </c>
-      <c r="K174" t="str">
+        <v>static const CooGUI_tds Pos_Bluetooth_PasscodeTxt_Normal = {160,115,85,115,150,25,235,140};</v>
+      </c>
+      <c r="L174">
         <f t="shared" si="296"/>
-        <v>static const CooGUI_tds Pos_Bluetooth_PasscodeTxt_Normal = {160,115,85,115,150,25,235,140};</v>
-      </c>
-      <c r="L174">
-        <f t="shared" si="297"/>
         <v>160</v>
       </c>
       <c r="M174" s="52">
-        <f t="shared" ref="M174:M189" si="307">D174 + $D$1</f>
-        <v>139</v>
+        <f>D174</f>
+        <v>115</v>
       </c>
       <c r="N174">
         <f t="shared" si="298"/>
@@ -19703,35 +19703,35 @@
         <v>115</v>
       </c>
       <c r="P174">
-        <f t="shared" si="299"/>
+        <f t="shared" si="300"/>
         <v>150</v>
       </c>
       <c r="Q174">
-        <f t="shared" si="300"/>
+        <f t="shared" si="301"/>
         <v>25</v>
       </c>
       <c r="R174" s="20">
-        <f t="shared" si="301"/>
+        <f t="shared" si="302"/>
         <v>235</v>
       </c>
       <c r="S174" s="20">
-        <f t="shared" si="302"/>
+        <f t="shared" si="303"/>
         <v>140</v>
       </c>
       <c r="T174" t="str">
-        <f t="shared" si="303"/>
-        <v>static const CooGUI_tds Pos_Bluetooth_PasscodeTxt_Flipped = {160,139,85,115,150,25,235,140};</v>
+        <f t="shared" si="304"/>
+        <v>static const CooGUI_tds Pos_Bluetooth_PasscodeTxt_Flipped = {160,115,85,115,150,25,235,140};</v>
       </c>
       <c r="U174" t="str">
-        <f t="shared" si="304"/>
+        <f t="shared" si="305"/>
         <v>const CooGUI_tds* Pos_Bluetooth_PasscodeTxt;</v>
       </c>
       <c r="V174">
-        <f t="shared" si="305"/>
+        <f t="shared" si="306"/>
         <v>3.662109375</v>
       </c>
       <c r="W174" t="str">
-        <f t="shared" si="306"/>
+        <f t="shared" si="307"/>
         <v>Pos_Bluetooth_PasscodeTxt = &amp;Pos_Bluetooth_PasscodeTxt_Normal;</v>
       </c>
     </row>
@@ -19782,47 +19782,47 @@
         <v>160</v>
       </c>
       <c r="M175" s="52">
-        <f t="shared" si="307"/>
-        <v>164</v>
+        <f>D175</f>
+        <v>140</v>
       </c>
       <c r="N175">
         <f t="shared" ref="N175:N189" si="314">E175</f>
         <v>85</v>
       </c>
       <c r="O175">
-        <f t="shared" si="308"/>
+        <f>F175</f>
         <v>140</v>
       </c>
       <c r="P175">
-        <f t="shared" ref="P175:P189" si="315">G175</f>
+        <f>G175</f>
         <v>150</v>
       </c>
       <c r="Q175">
-        <f t="shared" ref="Q175:Q189" si="316">H175</f>
+        <f t="shared" ref="Q175:Q189" si="315">H175</f>
         <v>60</v>
       </c>
       <c r="R175" s="20">
-        <f t="shared" ref="R175:R189" si="317">N175+P175</f>
+        <f t="shared" ref="R175:R189" si="316">N175+P175</f>
         <v>235</v>
       </c>
       <c r="S175" s="20">
-        <f t="shared" ref="S175:S189" si="318">O175+Q175</f>
+        <f t="shared" ref="S175:S189" si="317">O175+Q175</f>
         <v>200</v>
       </c>
       <c r="T175" t="str">
-        <f t="shared" ref="T175:T189" si="319">CONCATENATE("static const CooGUI_tds ",A175, "_Flipped = {", L175, ",", M175, ",", N175, ",", O175, ",",P175, ",", Q175,",",  R175, ",", S175, "};")</f>
-        <v>static const CooGUI_tds Pos_Bluetooth_PasscodeValue_Flipped = {160,164,85,140,150,60,235,200};</v>
+        <f t="shared" ref="T175:T189" si="318">CONCATENATE("static const CooGUI_tds ",A175, "_Flipped = {", L175, ",", M175, ",", N175, ",", O175, ",",P175, ",", Q175,",",  R175, ",", S175, "};")</f>
+        <v>static const CooGUI_tds Pos_Bluetooth_PasscodeValue_Flipped = {160,140,85,140,150,60,235,200};</v>
       </c>
       <c r="U175" t="str">
-        <f t="shared" ref="U175:U189" si="320">CONCATENATE("const CooGUI_tds* ",A175, ";")</f>
+        <f t="shared" ref="U175:U189" si="319">CONCATENATE("const CooGUI_tds* ",A175, ";")</f>
         <v>const CooGUI_tds* Pos_Bluetooth_PasscodeValue;</v>
       </c>
       <c r="V175">
-        <f t="shared" ref="V175:V189" si="321">(G175*H175)/1024</f>
+        <f t="shared" ref="V175:V189" si="320">(G175*H175)/1024</f>
         <v>8.7890625</v>
       </c>
       <c r="W175" t="str">
-        <f t="shared" ref="W175:W189" si="322">CONCATENATE(A175, " = &amp;", B175,";")</f>
+        <f t="shared" ref="W175:W189" si="321">CONCATENATE(A175, " = &amp;", B175,";")</f>
         <v>Pos_Bluetooth_PasscodeValue = &amp;Pos_Bluetooth_PasscodeValue_Normal;</v>
       </c>
     </row>
@@ -19831,7 +19831,7 @@
         <v>307</v>
       </c>
       <c r="B176" t="str">
-        <f t="shared" ref="B176" si="323">CONCATENATE(A176, "_Normal")</f>
+        <f t="shared" ref="B176" si="322">CONCATENATE(A176, "_Normal")</f>
         <v>Pos_Bluetooth_DownLoadData_01_Normal</v>
       </c>
       <c r="C176" s="22">
@@ -19843,7 +19843,7 @@
         <v>115</v>
       </c>
       <c r="E176" s="23">
-        <f t="shared" ref="E176" si="324">C176-G176/2</f>
+        <f t="shared" ref="E176" si="323">C176-G176/2</f>
         <v>0</v>
       </c>
       <c r="F176" s="23">
@@ -19857,63 +19857,63 @@
         <v>32</v>
       </c>
       <c r="I176" s="20">
-        <f t="shared" ref="I176" si="325">E176+G176</f>
+        <f t="shared" ref="I176" si="324">E176+G176</f>
         <v>320</v>
       </c>
       <c r="J176" s="20">
-        <f t="shared" ref="J176" si="326">F176+H176</f>
+        <f t="shared" ref="J176" si="325">F176+H176</f>
         <v>147</v>
       </c>
       <c r="K176" t="str">
-        <f t="shared" ref="K176" si="327">CONCATENATE("static const CooGUI_tds ",A176, "_Normal = {", C176, ",", D176, ",", E176, ",", F176, ",",G176, ",", H176,",",  I176, ",", J176, "};")</f>
+        <f t="shared" ref="K176" si="326">CONCATENATE("static const CooGUI_tds ",A176, "_Normal = {", C176, ",", D176, ",", E176, ",", F176, ",",G176, ",", H176,",",  I176, ",", J176, "};")</f>
         <v>static const CooGUI_tds Pos_Bluetooth_DownLoadData_01_Normal = {160,115,0,115,320,32,320,147};</v>
       </c>
       <c r="L176">
-        <f t="shared" ref="L176" si="328">C176</f>
+        <f t="shared" ref="L176" si="327">C176</f>
         <v>160</v>
       </c>
       <c r="M176" s="52">
-        <f t="shared" ref="M176" si="329">D176 + $D$1</f>
-        <v>139</v>
+        <f>D176</f>
+        <v>115</v>
       </c>
       <c r="N176">
-        <f t="shared" ref="N176" si="330">E176</f>
+        <f t="shared" ref="N176" si="328">E176</f>
         <v>0</v>
       </c>
       <c r="O176">
-        <f t="shared" ref="O176" si="331">F176</f>
+        <f>F176</f>
         <v>115</v>
       </c>
       <c r="P176">
-        <f t="shared" ref="P176" si="332">G176</f>
+        <f t="shared" ref="P176" si="329">G176</f>
         <v>320</v>
       </c>
       <c r="Q176">
-        <f t="shared" ref="Q176" si="333">H176</f>
+        <f t="shared" ref="Q176" si="330">H176</f>
         <v>32</v>
       </c>
       <c r="R176" s="20">
-        <f t="shared" ref="R176" si="334">N176+P176</f>
+        <f t="shared" ref="R176" si="331">N176+P176</f>
         <v>320</v>
       </c>
       <c r="S176" s="20">
-        <f t="shared" ref="S176" si="335">O176+Q176</f>
+        <f t="shared" ref="S176" si="332">O176+Q176</f>
         <v>147</v>
       </c>
       <c r="T176" t="str">
-        <f t="shared" ref="T176" si="336">CONCATENATE("static const CooGUI_tds ",A176, "_Flipped = {", L176, ",", M176, ",", N176, ",", O176, ",",P176, ",", Q176,",",  R176, ",", S176, "};")</f>
-        <v>static const CooGUI_tds Pos_Bluetooth_DownLoadData_01_Flipped = {160,139,0,115,320,32,320,147};</v>
+        <f t="shared" ref="T176" si="333">CONCATENATE("static const CooGUI_tds ",A176, "_Flipped = {", L176, ",", M176, ",", N176, ",", O176, ",",P176, ",", Q176,",",  R176, ",", S176, "};")</f>
+        <v>static const CooGUI_tds Pos_Bluetooth_DownLoadData_01_Flipped = {160,115,0,115,320,32,320,147};</v>
       </c>
       <c r="U176" t="str">
-        <f t="shared" ref="U176" si="337">CONCATENATE("const CooGUI_tds* ",A176, ";")</f>
+        <f t="shared" ref="U176" si="334">CONCATENATE("const CooGUI_tds* ",A176, ";")</f>
         <v>const CooGUI_tds* Pos_Bluetooth_DownLoadData_01;</v>
       </c>
       <c r="V176">
-        <f t="shared" ref="V176" si="338">(G176*H176)/1024</f>
+        <f t="shared" ref="V176" si="335">(G176*H176)/1024</f>
         <v>10</v>
       </c>
       <c r="W176" t="str">
-        <f t="shared" ref="W176" si="339">CONCATENATE(A176, " = &amp;", B176,";")</f>
+        <f t="shared" ref="W176" si="336">CONCATENATE(A176, " = &amp;", B176,";")</f>
         <v>Pos_Bluetooth_DownLoadData_01 = &amp;Pos_Bluetooth_DownLoadData_01_Normal;</v>
       </c>
     </row>
@@ -19922,7 +19922,7 @@
         <v>308</v>
       </c>
       <c r="B177" t="str">
-        <f t="shared" ref="B177" si="340">CONCATENATE(A177, "_Normal")</f>
+        <f t="shared" ref="B177" si="337">CONCATENATE(A177, "_Normal")</f>
         <v>Pos_Bluetooth_DownLoadData_02_Normal</v>
       </c>
       <c r="C177" s="22">
@@ -19950,63 +19950,63 @@
         <v>32</v>
       </c>
       <c r="I177" s="20">
-        <f t="shared" ref="I177" si="341">E177+G177</f>
+        <f t="shared" ref="I177" si="338">E177+G177</f>
         <v>320</v>
       </c>
       <c r="J177" s="20">
-        <f t="shared" ref="J177" si="342">F177+H177</f>
+        <f t="shared" ref="J177" si="339">F177+H177</f>
         <v>179</v>
       </c>
       <c r="K177" t="str">
-        <f t="shared" ref="K177" si="343">CONCATENATE("static const CooGUI_tds ",A177, "_Normal = {", C177, ",", D177, ",", E177, ",", F177, ",",G177, ",", H177,",",  I177, ",", J177, "};")</f>
+        <f t="shared" ref="K177" si="340">CONCATENATE("static const CooGUI_tds ",A177, "_Normal = {", C177, ",", D177, ",", E177, ",", F177, ",",G177, ",", H177,",",  I177, ",", J177, "};")</f>
         <v>static const CooGUI_tds Pos_Bluetooth_DownLoadData_02_Normal = {160,147,0,147,320,32,320,179};</v>
       </c>
       <c r="L177">
-        <f t="shared" ref="L177" si="344">C177</f>
+        <f t="shared" ref="L177" si="341">C177</f>
         <v>160</v>
       </c>
       <c r="M177" s="52">
-        <f t="shared" ref="M177" si="345">D177 + $D$1</f>
-        <v>171</v>
+        <f>D177</f>
+        <v>147</v>
       </c>
       <c r="N177">
-        <f t="shared" ref="N177" si="346">E177</f>
+        <f t="shared" ref="N177" si="342">E177</f>
         <v>0</v>
       </c>
       <c r="O177">
-        <f t="shared" ref="O177" si="347">F177</f>
+        <f t="shared" ref="O177" si="343">F177</f>
         <v>147</v>
       </c>
       <c r="P177">
-        <f t="shared" ref="P177" si="348">G177</f>
+        <f t="shared" ref="P177" si="344">G177</f>
         <v>320</v>
       </c>
       <c r="Q177">
-        <f t="shared" ref="Q177" si="349">H177</f>
+        <f t="shared" ref="Q177" si="345">H177</f>
         <v>32</v>
       </c>
       <c r="R177" s="20">
-        <f t="shared" ref="R177" si="350">N177+P177</f>
+        <f t="shared" ref="R177" si="346">N177+P177</f>
         <v>320</v>
       </c>
       <c r="S177" s="20">
-        <f t="shared" ref="S177" si="351">O177+Q177</f>
+        <f t="shared" ref="S177" si="347">O177+Q177</f>
         <v>179</v>
       </c>
       <c r="T177" t="str">
-        <f t="shared" ref="T177" si="352">CONCATENATE("static const CooGUI_tds ",A177, "_Flipped = {", L177, ",", M177, ",", N177, ",", O177, ",",P177, ",", Q177,",",  R177, ",", S177, "};")</f>
-        <v>static const CooGUI_tds Pos_Bluetooth_DownLoadData_02_Flipped = {160,171,0,147,320,32,320,179};</v>
+        <f t="shared" ref="T177" si="348">CONCATENATE("static const CooGUI_tds ",A177, "_Flipped = {", L177, ",", M177, ",", N177, ",", O177, ",",P177, ",", Q177,",",  R177, ",", S177, "};")</f>
+        <v>static const CooGUI_tds Pos_Bluetooth_DownLoadData_02_Flipped = {160,147,0,147,320,32,320,179};</v>
       </c>
       <c r="U177" t="str">
-        <f t="shared" ref="U177" si="353">CONCATENATE("const CooGUI_tds* ",A177, ";")</f>
+        <f t="shared" ref="U177" si="349">CONCATENATE("const CooGUI_tds* ",A177, ";")</f>
         <v>const CooGUI_tds* Pos_Bluetooth_DownLoadData_02;</v>
       </c>
       <c r="V177">
-        <f t="shared" ref="V177" si="354">(G177*H177)/1024</f>
+        <f t="shared" ref="V177" si="350">(G177*H177)/1024</f>
         <v>10</v>
       </c>
       <c r="W177" t="str">
-        <f t="shared" ref="W177" si="355">CONCATENATE(A177, " = &amp;", B177,";")</f>
+        <f t="shared" ref="W177" si="351">CONCATENATE(A177, " = &amp;", B177,";")</f>
         <v>Pos_Bluetooth_DownLoadData_02 = &amp;Pos_Bluetooth_DownLoadData_02_Normal;</v>
       </c>
     </row>
@@ -20055,7 +20055,7 @@
         <v>180</v>
       </c>
       <c r="M178" s="52">
-        <f t="shared" si="307"/>
+        <f t="shared" ref="M174:M189" si="352">D178 + $D$1</f>
         <v>24</v>
       </c>
       <c r="N178">
@@ -20067,35 +20067,35 @@
         <v>0</v>
       </c>
       <c r="P178">
+        <f t="shared" ref="P175:P189" si="353">G178</f>
+        <v>140</v>
+      </c>
+      <c r="Q178">
         <f t="shared" si="315"/>
-        <v>140</v>
-      </c>
-      <c r="Q178">
+        <v>23</v>
+      </c>
+      <c r="R178" s="20">
         <f t="shared" si="316"/>
+        <v>320</v>
+      </c>
+      <c r="S178" s="20">
+        <f t="shared" si="317"/>
         <v>23</v>
       </c>
-      <c r="R178" s="20">
-        <f t="shared" si="317"/>
-        <v>320</v>
-      </c>
-      <c r="S178" s="20">
+      <c r="T178" t="str">
         <f t="shared" si="318"/>
-        <v>23</v>
-      </c>
-      <c r="T178" t="str">
+        <v>static const CooGUI_tds Pos_Slates_Tittle_Flipped = {180,24,180,0,140,23,320,23};</v>
+      </c>
+      <c r="U178" t="str">
         <f t="shared" si="319"/>
-        <v>static const CooGUI_tds Pos_Slates_Tittle_Flipped = {180,24,180,0,140,23,320,23};</v>
-      </c>
-      <c r="U178" t="str">
+        <v>const CooGUI_tds* Pos_Slates_Tittle;</v>
+      </c>
+      <c r="V178">
         <f t="shared" si="320"/>
-        <v>const CooGUI_tds* Pos_Slates_Tittle;</v>
-      </c>
-      <c r="V178">
+        <v>3.14453125</v>
+      </c>
+      <c r="W178" t="str">
         <f t="shared" si="321"/>
-        <v>3.14453125</v>
-      </c>
-      <c r="W178" t="str">
-        <f t="shared" si="322"/>
         <v>Pos_Slates_Tittle = &amp;Pos_Slates_Tittle_Normal;</v>
       </c>
     </row>
@@ -20143,7 +20143,7 @@
         <v>0</v>
       </c>
       <c r="M179" s="52">
-        <f t="shared" si="307"/>
+        <f t="shared" si="352"/>
         <v>24</v>
       </c>
       <c r="N179">
@@ -20155,35 +20155,35 @@
         <v>120</v>
       </c>
       <c r="P179">
+        <f t="shared" si="353"/>
+        <v>260</v>
+      </c>
+      <c r="Q179">
         <f t="shared" si="315"/>
-        <v>260</v>
-      </c>
-      <c r="Q179">
+        <v>90</v>
+      </c>
+      <c r="R179" s="20">
         <f t="shared" si="316"/>
-        <v>90</v>
-      </c>
-      <c r="R179" s="20">
+        <v>285</v>
+      </c>
+      <c r="S179" s="20">
         <f t="shared" si="317"/>
-        <v>285</v>
-      </c>
-      <c r="S179" s="20">
+        <v>210</v>
+      </c>
+      <c r="T179" t="str">
         <f t="shared" si="318"/>
-        <v>210</v>
-      </c>
-      <c r="T179" t="str">
+        <v>static const CooGUI_tds Pos_SurfClearToUpdate_1_Flipped = {0,24,25,120,260,90,285,210};</v>
+      </c>
+      <c r="U179" t="str">
         <f t="shared" si="319"/>
-        <v>static const CooGUI_tds Pos_SurfClearToUpdate_1_Flipped = {0,24,25,120,260,90,285,210};</v>
-      </c>
-      <c r="U179" t="str">
+        <v>const CooGUI_tds* Pos_SurfClearToUpdate_1;</v>
+      </c>
+      <c r="V179">
         <f t="shared" si="320"/>
-        <v>const CooGUI_tds* Pos_SurfClearToUpdate_1;</v>
-      </c>
-      <c r="V179">
+        <v>22.8515625</v>
+      </c>
+      <c r="W179" t="str">
         <f t="shared" si="321"/>
-        <v>22.8515625</v>
-      </c>
-      <c r="W179" t="str">
-        <f t="shared" si="322"/>
         <v>Pos_SurfClearToUpdate_1 = &amp;Pos_SurfClearToUpdate_1_Normal;</v>
       </c>
     </row>
@@ -20231,7 +20231,7 @@
         <v>0</v>
       </c>
       <c r="M180" s="52">
-        <f t="shared" si="307"/>
+        <f t="shared" si="352"/>
         <v>24</v>
       </c>
       <c r="N180">
@@ -20243,35 +20243,35 @@
         <v>210</v>
       </c>
       <c r="P180">
+        <f t="shared" si="353"/>
+        <v>320</v>
+      </c>
+      <c r="Q180">
         <f t="shared" si="315"/>
+        <v>30</v>
+      </c>
+      <c r="R180" s="20">
+        <f t="shared" si="316"/>
         <v>320</v>
       </c>
-      <c r="Q180">
-        <f t="shared" si="316"/>
-        <v>30</v>
-      </c>
-      <c r="R180" s="20">
+      <c r="S180" s="20">
         <f t="shared" si="317"/>
-        <v>320</v>
-      </c>
-      <c r="S180" s="20">
+        <v>240</v>
+      </c>
+      <c r="T180" t="str">
         <f t="shared" si="318"/>
-        <v>240</v>
-      </c>
-      <c r="T180" t="str">
+        <v>static const CooGUI_tds Pos_SurfClearToUpdate_2_Flipped = {0,24,0,210,320,30,320,240};</v>
+      </c>
+      <c r="U180" t="str">
         <f t="shared" si="319"/>
-        <v>static const CooGUI_tds Pos_SurfClearToUpdate_2_Flipped = {0,24,0,210,320,30,320,240};</v>
-      </c>
-      <c r="U180" t="str">
+        <v>const CooGUI_tds* Pos_SurfClearToUpdate_2;</v>
+      </c>
+      <c r="V180">
         <f t="shared" si="320"/>
-        <v>const CooGUI_tds* Pos_SurfClearToUpdate_2;</v>
-      </c>
-      <c r="V180">
+        <v>9.375</v>
+      </c>
+      <c r="W180" t="str">
         <f t="shared" si="321"/>
-        <v>9.375</v>
-      </c>
-      <c r="W180" t="str">
-        <f t="shared" si="322"/>
         <v>Pos_SurfClearToUpdate_2 = &amp;Pos_SurfClearToUpdate_2_Normal;</v>
       </c>
     </row>
@@ -20306,11 +20306,11 @@
         <v>30</v>
       </c>
       <c r="I181" s="20">
-        <f t="shared" ref="I181:J184" si="356">E181+G181</f>
+        <f t="shared" ref="I181:J184" si="354">E181+G181</f>
         <v>294</v>
       </c>
       <c r="J181" s="20">
-        <f t="shared" si="356"/>
+        <f t="shared" si="354"/>
         <v>210</v>
       </c>
       <c r="K181" t="str">
@@ -20326,27 +20326,27 @@
         <v>24</v>
       </c>
       <c r="N181">
-        <f t="shared" ref="N181:Q184" si="357">E181</f>
+        <f t="shared" ref="N181:Q184" si="355">E181</f>
         <v>25</v>
       </c>
       <c r="O181">
-        <f t="shared" si="357"/>
+        <f t="shared" si="355"/>
         <v>180</v>
       </c>
       <c r="P181">
-        <f t="shared" si="357"/>
+        <f t="shared" si="355"/>
         <v>269</v>
       </c>
       <c r="Q181">
-        <f t="shared" si="357"/>
+        <f t="shared" si="355"/>
         <v>30</v>
       </c>
       <c r="R181" s="20">
-        <f t="shared" ref="R181:S184" si="358">N181+P181</f>
+        <f t="shared" ref="R181:S184" si="356">N181+P181</f>
         <v>294</v>
       </c>
       <c r="S181" s="20">
-        <f t="shared" si="358"/>
+        <f t="shared" si="356"/>
         <v>210</v>
       </c>
       <c r="T181" t="str">
@@ -20395,11 +20395,11 @@
         <v>30</v>
       </c>
       <c r="I182" s="20">
-        <f t="shared" si="356"/>
+        <f t="shared" si="354"/>
         <v>320</v>
       </c>
       <c r="J182" s="20">
-        <f t="shared" si="356"/>
+        <f t="shared" si="354"/>
         <v>240</v>
       </c>
       <c r="K182" t="str">
@@ -20415,27 +20415,27 @@
         <v>24</v>
       </c>
       <c r="N182">
-        <f t="shared" si="357"/>
+        <f t="shared" si="355"/>
         <v>25</v>
       </c>
       <c r="O182">
-        <f t="shared" si="357"/>
+        <f t="shared" si="355"/>
         <v>210</v>
       </c>
       <c r="P182">
-        <f t="shared" si="357"/>
+        <f t="shared" si="355"/>
         <v>295</v>
       </c>
       <c r="Q182">
-        <f t="shared" si="357"/>
+        <f t="shared" si="355"/>
         <v>30</v>
       </c>
       <c r="R182" s="20">
-        <f t="shared" si="358"/>
+        <f t="shared" si="356"/>
         <v>320</v>
       </c>
       <c r="S182" s="20">
-        <f t="shared" si="358"/>
+        <f t="shared" si="356"/>
         <v>240</v>
       </c>
       <c r="T182" t="str">
@@ -20485,11 +20485,11 @@
         <v>38</v>
       </c>
       <c r="I183" s="20">
-        <f t="shared" si="356"/>
+        <f t="shared" si="354"/>
         <v>25</v>
       </c>
       <c r="J183" s="20">
-        <f t="shared" si="356"/>
+        <f t="shared" si="354"/>
         <v>240</v>
       </c>
       <c r="K183" t="str">
@@ -20505,27 +20505,27 @@
         <v>24</v>
       </c>
       <c r="N183">
-        <f t="shared" si="357"/>
+        <f t="shared" si="355"/>
         <v>0</v>
       </c>
       <c r="O183">
-        <f t="shared" si="357"/>
+        <f t="shared" si="355"/>
         <v>202</v>
       </c>
       <c r="P183">
-        <f t="shared" si="357"/>
+        <f t="shared" si="355"/>
         <v>25</v>
       </c>
       <c r="Q183">
-        <f t="shared" si="357"/>
+        <f t="shared" si="355"/>
         <v>38</v>
       </c>
       <c r="R183" s="20">
-        <f t="shared" si="358"/>
+        <f t="shared" si="356"/>
         <v>25</v>
       </c>
       <c r="S183" s="20">
-        <f t="shared" si="358"/>
+        <f t="shared" si="356"/>
         <v>240</v>
       </c>
       <c r="T183" t="str">
@@ -20576,11 +20576,11 @@
         <v>30</v>
       </c>
       <c r="I184" s="20">
-        <f t="shared" si="356"/>
+        <f t="shared" si="354"/>
         <v>319</v>
       </c>
       <c r="J184" s="20">
-        <f t="shared" si="356"/>
+        <f t="shared" si="354"/>
         <v>240</v>
       </c>
       <c r="K184" t="str">
@@ -20596,27 +20596,27 @@
         <v>24</v>
       </c>
       <c r="N184">
-        <f t="shared" si="357"/>
+        <f t="shared" si="355"/>
         <v>294</v>
       </c>
       <c r="O184">
-        <f t="shared" si="357"/>
+        <f t="shared" si="355"/>
         <v>210</v>
       </c>
       <c r="P184">
-        <f t="shared" si="357"/>
+        <f t="shared" si="355"/>
         <v>25</v>
       </c>
       <c r="Q184">
-        <f t="shared" si="357"/>
+        <f t="shared" si="355"/>
         <v>30</v>
       </c>
       <c r="R184" s="20">
-        <f t="shared" si="358"/>
+        <f t="shared" si="356"/>
         <v>319</v>
       </c>
       <c r="S184" s="20">
-        <f t="shared" si="358"/>
+        <f t="shared" si="356"/>
         <v>240</v>
       </c>
       <c r="T184" t="str">
@@ -20682,7 +20682,7 @@
         <v>160</v>
       </c>
       <c r="M185" s="52">
-        <f t="shared" si="307"/>
+        <f t="shared" si="352"/>
         <v>24</v>
       </c>
       <c r="N185">
@@ -20694,35 +20694,35 @@
         <v>0</v>
       </c>
       <c r="P185">
+        <f t="shared" si="353"/>
+        <v>320</v>
+      </c>
+      <c r="Q185">
         <f t="shared" si="315"/>
+        <v>20</v>
+      </c>
+      <c r="R185" s="20">
+        <f t="shared" si="316"/>
         <v>320</v>
       </c>
-      <c r="Q185">
-        <f t="shared" si="316"/>
+      <c r="S185" s="20">
+        <f t="shared" si="317"/>
         <v>20</v>
       </c>
-      <c r="R185" s="20">
-        <f t="shared" si="317"/>
-        <v>320</v>
-      </c>
-      <c r="S185" s="20">
+      <c r="T185" t="str">
         <f t="shared" si="318"/>
-        <v>20</v>
-      </c>
-      <c r="T185" t="str">
+        <v>static const CooGUI_tds Pos_DiveMenu_DecoStop_PO2_Tittle_Flipped = {160,24,0,0,320,20,320,20};</v>
+      </c>
+      <c r="U185" t="str">
         <f t="shared" si="319"/>
-        <v>static const CooGUI_tds Pos_DiveMenu_DecoStop_PO2_Tittle_Flipped = {160,24,0,0,320,20,320,20};</v>
-      </c>
-      <c r="U185" t="str">
+        <v>const CooGUI_tds* Pos_DiveMenu_DecoStop_PO2_Tittle;</v>
+      </c>
+      <c r="V185">
         <f t="shared" si="320"/>
-        <v>const CooGUI_tds* Pos_DiveMenu_DecoStop_PO2_Tittle;</v>
-      </c>
-      <c r="V185">
+        <v>6.25</v>
+      </c>
+      <c r="W185" t="str">
         <f t="shared" si="321"/>
-        <v>6.25</v>
-      </c>
-      <c r="W185" t="str">
-        <f t="shared" si="322"/>
         <v>Pos_DiveMenu_DecoStop_PO2_Tittle = &amp;Pos_DiveMenu_DecoStop_PO2_Tittle_Normal;</v>
       </c>
     </row>
@@ -20774,7 +20774,7 @@
         <v>160</v>
       </c>
       <c r="M186" s="52">
-        <f t="shared" si="307"/>
+        <f t="shared" si="352"/>
         <v>38</v>
       </c>
       <c r="N186">
@@ -20786,35 +20786,35 @@
         <v>20</v>
       </c>
       <c r="P186">
+        <f t="shared" si="353"/>
+        <v>320</v>
+      </c>
+      <c r="Q186">
         <f t="shared" si="315"/>
+        <v>40</v>
+      </c>
+      <c r="R186" s="20">
+        <f t="shared" si="316"/>
         <v>320</v>
       </c>
-      <c r="Q186">
-        <f t="shared" si="316"/>
-        <v>40</v>
-      </c>
-      <c r="R186" s="20">
+      <c r="S186" s="20">
         <f t="shared" si="317"/>
-        <v>320</v>
-      </c>
-      <c r="S186" s="20">
+        <v>60</v>
+      </c>
+      <c r="T186" t="str">
         <f t="shared" si="318"/>
-        <v>60</v>
-      </c>
-      <c r="T186" t="str">
+        <v>static const CooGUI_tds Pos_DiveMenu_DecoStop_PO2_Value_Flipped = {160,38,0,20,320,40,320,60};</v>
+      </c>
+      <c r="U186" t="str">
         <f t="shared" si="319"/>
-        <v>static const CooGUI_tds Pos_DiveMenu_DecoStop_PO2_Value_Flipped = {160,38,0,20,320,40,320,60};</v>
-      </c>
-      <c r="U186" t="str">
+        <v>const CooGUI_tds* Pos_DiveMenu_DecoStop_PO2_Value;</v>
+      </c>
+      <c r="V186">
         <f t="shared" si="320"/>
-        <v>const CooGUI_tds* Pos_DiveMenu_DecoStop_PO2_Value;</v>
-      </c>
-      <c r="V186">
+        <v>12.5</v>
+      </c>
+      <c r="W186" t="str">
         <f t="shared" si="321"/>
-        <v>12.5</v>
-      </c>
-      <c r="W186" t="str">
-        <f t="shared" si="322"/>
         <v>Pos_DiveMenu_DecoStop_PO2_Value = &amp;Pos_DiveMenu_DecoStop_PO2_Value_Normal;</v>
       </c>
     </row>
@@ -20864,7 +20864,7 @@
         <v>0</v>
       </c>
       <c r="M187" s="52">
-        <f t="shared" si="307"/>
+        <f t="shared" si="352"/>
         <v>84</v>
       </c>
       <c r="N187">
@@ -20876,35 +20876,35 @@
         <v>60</v>
       </c>
       <c r="P187">
+        <f t="shared" si="353"/>
+        <v>320</v>
+      </c>
+      <c r="Q187">
         <f t="shared" si="315"/>
+        <v>26</v>
+      </c>
+      <c r="R187" s="20">
+        <f t="shared" si="316"/>
         <v>320</v>
       </c>
-      <c r="Q187">
-        <f t="shared" si="316"/>
-        <v>26</v>
-      </c>
-      <c r="R187" s="20">
+      <c r="S187" s="20">
         <f t="shared" si="317"/>
-        <v>320</v>
-      </c>
-      <c r="S187" s="20">
+        <v>86</v>
+      </c>
+      <c r="T187" t="str">
         <f t="shared" si="318"/>
-        <v>86</v>
-      </c>
-      <c r="T187" t="str">
+        <v>static const CooGUI_tds Pos_DiveMenu_DecoStop_List_Flipped = {0,84,0,60,320,26,320,86};</v>
+      </c>
+      <c r="U187" t="str">
         <f t="shared" si="319"/>
-        <v>static const CooGUI_tds Pos_DiveMenu_DecoStop_List_Flipped = {0,84,0,60,320,26,320,86};</v>
-      </c>
-      <c r="U187" t="str">
+        <v>const CooGUI_tds* Pos_DiveMenu_DecoStop_List;</v>
+      </c>
+      <c r="V187">
         <f t="shared" si="320"/>
-        <v>const CooGUI_tds* Pos_DiveMenu_DecoStop_List;</v>
-      </c>
-      <c r="V187">
+        <v>8.125</v>
+      </c>
+      <c r="W187" t="str">
         <f t="shared" si="321"/>
-        <v>8.125</v>
-      </c>
-      <c r="W187" t="str">
-        <f t="shared" si="322"/>
         <v>Pos_DiveMenu_DecoStop_List = &amp;Pos_DiveMenu_DecoStop_List_Normal;</v>
       </c>
     </row>
@@ -20955,7 +20955,7 @@
         <v>160</v>
       </c>
       <c r="M188" s="52">
-        <f t="shared" si="307"/>
+        <f t="shared" si="352"/>
         <v>124</v>
       </c>
       <c r="N188">
@@ -20967,35 +20967,35 @@
         <v>110</v>
       </c>
       <c r="P188">
+        <f t="shared" si="353"/>
+        <v>200</v>
+      </c>
+      <c r="Q188">
         <f t="shared" si="315"/>
-        <v>200</v>
-      </c>
-      <c r="Q188">
+        <v>54</v>
+      </c>
+      <c r="R188" s="20">
         <f t="shared" si="316"/>
-        <v>54</v>
-      </c>
-      <c r="R188" s="20">
+        <v>260</v>
+      </c>
+      <c r="S188" s="20">
         <f t="shared" si="317"/>
-        <v>260</v>
-      </c>
-      <c r="S188" s="20">
+        <v>164</v>
+      </c>
+      <c r="T188" t="str">
         <f t="shared" si="318"/>
-        <v>164</v>
-      </c>
-      <c r="T188" t="str">
+        <v>static const CooGUI_tds Pos_DiveMenu_DecoStop_NODECO_Flipped = {160,124,60,110,200,54,260,164};</v>
+      </c>
+      <c r="U188" t="str">
         <f t="shared" si="319"/>
-        <v>static const CooGUI_tds Pos_DiveMenu_DecoStop_NODECO_Flipped = {160,124,60,110,200,54,260,164};</v>
-      </c>
-      <c r="U188" t="str">
+        <v>const CooGUI_tds* Pos_DiveMenu_DecoStop_NODECO;</v>
+      </c>
+      <c r="V188">
         <f t="shared" si="320"/>
-        <v>const CooGUI_tds* Pos_DiveMenu_DecoStop_NODECO;</v>
-      </c>
-      <c r="V188">
+        <v>10.546875</v>
+      </c>
+      <c r="W188" t="str">
         <f t="shared" si="321"/>
-        <v>10.546875</v>
-      </c>
-      <c r="W188" t="str">
-        <f t="shared" si="322"/>
         <v>Pos_DiveMenu_DecoStop_NODECO = &amp;Pos_DiveMenu_DecoStop_NODECO_Normal;</v>
       </c>
     </row>
@@ -21046,7 +21046,7 @@
         <v>160</v>
       </c>
       <c r="M189" s="52">
-        <f t="shared" si="307"/>
+        <f t="shared" si="352"/>
         <v>224</v>
       </c>
       <c r="N189">
@@ -21058,35 +21058,35 @@
         <v>180</v>
       </c>
       <c r="P189">
+        <f t="shared" si="353"/>
+        <v>270</v>
+      </c>
+      <c r="Q189">
         <f t="shared" si="315"/>
-        <v>270</v>
-      </c>
-      <c r="Q189">
+        <v>60</v>
+      </c>
+      <c r="R189" s="20">
         <f t="shared" si="316"/>
-        <v>60</v>
-      </c>
-      <c r="R189" s="20">
+        <v>295</v>
+      </c>
+      <c r="S189" s="20">
         <f t="shared" si="317"/>
-        <v>295</v>
-      </c>
-      <c r="S189" s="20">
+        <v>240</v>
+      </c>
+      <c r="T189" t="str">
         <f t="shared" si="318"/>
-        <v>240</v>
-      </c>
-      <c r="T189" t="str">
+        <v>static const CooGUI_tds Pos_ALARM_BottomInOneLine_Flipped = {160,224,25,180,270,60,295,240};</v>
+      </c>
+      <c r="U189" t="str">
         <f t="shared" si="319"/>
-        <v>static const CooGUI_tds Pos_ALARM_BottomInOneLine_Flipped = {160,224,25,180,270,60,295,240};</v>
-      </c>
-      <c r="U189" t="str">
+        <v>const CooGUI_tds* Pos_ALARM_BottomInOneLine;</v>
+      </c>
+      <c r="V189">
         <f t="shared" si="320"/>
-        <v>const CooGUI_tds* Pos_ALARM_BottomInOneLine;</v>
-      </c>
-      <c r="V189">
+        <v>15.8203125</v>
+      </c>
+      <c r="W189" t="str">
         <f t="shared" si="321"/>
-        <v>15.8203125</v>
-      </c>
-      <c r="W189" t="str">
-        <f t="shared" si="322"/>
         <v>Pos_ALARM_BottomInOneLine = &amp;Pos_ALARM_BottomInOneLine_Normal;</v>
       </c>
     </row>
@@ -21095,11 +21095,11 @@
         <v>302</v>
       </c>
       <c r="B190" s="102" t="str">
-        <f t="shared" ref="B190" si="359">CONCATENATE(A190, "_Normal")</f>
+        <f t="shared" ref="B190" si="357">CONCATENATE(A190, "_Normal")</f>
         <v>Pos_ALARM_BottomInTwoLines_01_Normal</v>
       </c>
       <c r="C190" s="23">
-        <f t="shared" ref="C190" si="360">C189</f>
+        <f t="shared" ref="C190" si="358">C189</f>
         <v>160</v>
       </c>
       <c r="D190" s="23">
@@ -21123,63 +21123,63 @@
         <v>30</v>
       </c>
       <c r="I190" s="20">
-        <f t="shared" ref="I190" si="361">E190+G190</f>
+        <f t="shared" ref="I190" si="359">E190+G190</f>
         <v>295</v>
       </c>
       <c r="J190" s="20">
-        <f t="shared" ref="J190" si="362">F190+H190</f>
+        <f t="shared" ref="J190" si="360">F190+H190</f>
         <v>210</v>
       </c>
       <c r="K190" t="str">
-        <f t="shared" ref="K190" si="363">CONCATENATE("static const CooGUI_tds ",A190, "_Normal = {", C190, ",", D190, ",", E190, ",", F190, ",",G190, ",", H190,",",  I190, ",", J190, "};")</f>
+        <f t="shared" ref="K190" si="361">CONCATENATE("static const CooGUI_tds ",A190, "_Normal = {", C190, ",", D190, ",", E190, ",", F190, ",",G190, ",", H190,",",  I190, ",", J190, "};")</f>
         <v>static const CooGUI_tds Pos_ALARM_BottomInTwoLines_01_Normal = {160,185,25,180,270,30,295,210};</v>
       </c>
       <c r="L190">
-        <f t="shared" ref="L190" si="364">C190</f>
+        <f t="shared" ref="L190" si="362">C190</f>
         <v>160</v>
       </c>
       <c r="M190" s="52">
-        <f t="shared" ref="M190" si="365">D190 + $D$1</f>
+        <f t="shared" ref="M190" si="363">D190 + $D$1</f>
         <v>209</v>
       </c>
       <c r="N190">
-        <f t="shared" ref="N190" si="366">E190</f>
+        <f t="shared" ref="N190" si="364">E190</f>
         <v>25</v>
       </c>
       <c r="O190">
-        <f t="shared" ref="O190" si="367">F190</f>
+        <f t="shared" ref="O190" si="365">F190</f>
         <v>180</v>
       </c>
       <c r="P190">
-        <f t="shared" ref="P190" si="368">G190</f>
+        <f t="shared" ref="P190" si="366">G190</f>
         <v>270</v>
       </c>
       <c r="Q190">
-        <f t="shared" ref="Q190" si="369">H190</f>
+        <f t="shared" ref="Q190" si="367">H190</f>
         <v>30</v>
       </c>
       <c r="R190" s="20">
-        <f t="shared" ref="R190" si="370">N190+P190</f>
+        <f t="shared" ref="R190" si="368">N190+P190</f>
         <v>295</v>
       </c>
       <c r="S190" s="20">
-        <f t="shared" ref="S190" si="371">O190+Q190</f>
+        <f t="shared" ref="S190" si="369">O190+Q190</f>
         <v>210</v>
       </c>
       <c r="T190" t="str">
-        <f t="shared" ref="T190" si="372">CONCATENATE("static const CooGUI_tds ",A190, "_Flipped = {", L190, ",", M190, ",", N190, ",", O190, ",",P190, ",", Q190,",",  R190, ",", S190, "};")</f>
+        <f t="shared" ref="T190" si="370">CONCATENATE("static const CooGUI_tds ",A190, "_Flipped = {", L190, ",", M190, ",", N190, ",", O190, ",",P190, ",", Q190,",",  R190, ",", S190, "};")</f>
         <v>static const CooGUI_tds Pos_ALARM_BottomInTwoLines_01_Flipped = {160,209,25,180,270,30,295,210};</v>
       </c>
       <c r="U190" t="str">
-        <f t="shared" ref="U190" si="373">CONCATENATE("const CooGUI_tds* ",A190, ";")</f>
+        <f t="shared" ref="U190" si="371">CONCATENATE("const CooGUI_tds* ",A190, ";")</f>
         <v>const CooGUI_tds* Pos_ALARM_BottomInTwoLines_01;</v>
       </c>
       <c r="V190">
-        <f t="shared" ref="V190" si="374">(G190*H190)/1024</f>
+        <f t="shared" ref="V190" si="372">(G190*H190)/1024</f>
         <v>7.91015625</v>
       </c>
       <c r="W190" t="str">
-        <f t="shared" ref="W190" si="375">CONCATENATE(A190, " = &amp;", B190,";")</f>
+        <f t="shared" ref="W190" si="373">CONCATENATE(A190, " = &amp;", B190,";")</f>
         <v>Pos_ALARM_BottomInTwoLines_01 = &amp;Pos_ALARM_BottomInTwoLines_01_Normal;</v>
       </c>
     </row>
@@ -21188,11 +21188,11 @@
         <v>303</v>
       </c>
       <c r="B191" s="102" t="str">
-        <f t="shared" ref="B191" si="376">CONCATENATE(A191, "_Normal")</f>
+        <f t="shared" ref="B191" si="374">CONCATENATE(A191, "_Normal")</f>
         <v>Pos_ALARM_BottomInTwoLines_02_Normal</v>
       </c>
       <c r="C191" s="23">
-        <f t="shared" ref="C191" si="377">C190</f>
+        <f t="shared" ref="C191" si="375">C190</f>
         <v>160</v>
       </c>
       <c r="D191" s="23">
@@ -21216,63 +21216,63 @@
         <v>30</v>
       </c>
       <c r="I191" s="20">
-        <f t="shared" ref="I191" si="378">E191+G191</f>
+        <f t="shared" ref="I191" si="376">E191+G191</f>
         <v>295</v>
       </c>
       <c r="J191" s="20">
-        <f t="shared" ref="J191" si="379">F191+H191</f>
+        <f t="shared" ref="J191" si="377">F191+H191</f>
         <v>240</v>
       </c>
       <c r="K191" t="str">
-        <f t="shared" ref="K191" si="380">CONCATENATE("static const CooGUI_tds ",A191, "_Normal = {", C191, ",", D191, ",", E191, ",", F191, ",",G191, ",", H191,",",  I191, ",", J191, "};")</f>
+        <f t="shared" ref="K191" si="378">CONCATENATE("static const CooGUI_tds ",A191, "_Normal = {", C191, ",", D191, ",", E191, ",", F191, ",",G191, ",", H191,",",  I191, ",", J191, "};")</f>
         <v>static const CooGUI_tds Pos_ALARM_BottomInTwoLines_02_Normal = {160,210,25,210,270,30,295,240};</v>
       </c>
       <c r="L191">
-        <f t="shared" ref="L191" si="381">C191</f>
+        <f t="shared" ref="L191" si="379">C191</f>
         <v>160</v>
       </c>
       <c r="M191" s="52">
-        <f t="shared" ref="M191" si="382">D191 + $D$1</f>
+        <f t="shared" ref="M191" si="380">D191 + $D$1</f>
         <v>234</v>
       </c>
       <c r="N191">
-        <f t="shared" ref="N191" si="383">E191</f>
+        <f t="shared" ref="N191" si="381">E191</f>
         <v>25</v>
       </c>
       <c r="O191">
-        <f t="shared" ref="O191" si="384">F191</f>
+        <f t="shared" ref="O191" si="382">F191</f>
         <v>210</v>
       </c>
       <c r="P191">
-        <f t="shared" ref="P191" si="385">G191</f>
+        <f t="shared" ref="P191" si="383">G191</f>
         <v>270</v>
       </c>
       <c r="Q191">
-        <f t="shared" ref="Q191" si="386">H191</f>
+        <f t="shared" ref="Q191" si="384">H191</f>
         <v>30</v>
       </c>
       <c r="R191" s="20">
-        <f t="shared" ref="R191" si="387">N191+P191</f>
+        <f t="shared" ref="R191" si="385">N191+P191</f>
         <v>295</v>
       </c>
       <c r="S191" s="20">
-        <f t="shared" ref="S191" si="388">O191+Q191</f>
+        <f t="shared" ref="S191" si="386">O191+Q191</f>
         <v>240</v>
       </c>
       <c r="T191" t="str">
-        <f t="shared" ref="T191" si="389">CONCATENATE("static const CooGUI_tds ",A191, "_Flipped = {", L191, ",", M191, ",", N191, ",", O191, ",",P191, ",", Q191,",",  R191, ",", S191, "};")</f>
+        <f t="shared" ref="T191" si="387">CONCATENATE("static const CooGUI_tds ",A191, "_Flipped = {", L191, ",", M191, ",", N191, ",", O191, ",",P191, ",", Q191,",",  R191, ",", S191, "};")</f>
         <v>static const CooGUI_tds Pos_ALARM_BottomInTwoLines_02_Flipped = {160,234,25,210,270,30,295,240};</v>
       </c>
       <c r="U191" t="str">
-        <f t="shared" ref="U191" si="390">CONCATENATE("const CooGUI_tds* ",A191, ";")</f>
+        <f t="shared" ref="U191" si="388">CONCATENATE("const CooGUI_tds* ",A191, ";")</f>
         <v>const CooGUI_tds* Pos_ALARM_BottomInTwoLines_02;</v>
       </c>
       <c r="V191">
-        <f t="shared" ref="V191" si="391">(G191*H191)/1024</f>
+        <f t="shared" ref="V191" si="389">(G191*H191)/1024</f>
         <v>7.91015625</v>
       </c>
       <c r="W191" t="str">
-        <f t="shared" ref="W191" si="392">CONCATENATE(A191, " = &amp;", B191,";")</f>
+        <f t="shared" ref="W191" si="390">CONCATENATE(A191, " = &amp;", B191,";")</f>
         <v>Pos_ALARM_BottomInTwoLines_02 = &amp;Pos_ALARM_BottomInTwoLines_02_Normal;</v>
       </c>
     </row>
@@ -21281,7 +21281,7 @@
         <v>238</v>
       </c>
       <c r="B192" t="str">
-        <f t="shared" ref="B192:B200" si="393">CONCATENATE(A192, "_Normal")</f>
+        <f t="shared" ref="B192:B200" si="391">CONCATENATE(A192, "_Normal")</f>
         <v>Pos_ALARM_DoubleArrowUp_Normal</v>
       </c>
       <c r="C192" s="9">
@@ -21305,63 +21305,63 @@
         <v>40</v>
       </c>
       <c r="I192" s="20">
-        <f t="shared" ref="I192:J200" si="394">E192+G192</f>
+        <f t="shared" ref="I192:J200" si="392">E192+G192</f>
         <v>170</v>
       </c>
       <c r="J192" s="20">
-        <f t="shared" si="394"/>
+        <f t="shared" si="392"/>
         <v>55</v>
       </c>
       <c r="K192" t="str">
-        <f t="shared" ref="K192:K200" si="395">CONCATENATE("static const CooGUI_tds ",A192, "_Normal = {", C192, ",", D192, ",", E192, ",", F192, ",",G192, ",", H192,",",  I192, ",", J192, "};")</f>
+        <f t="shared" ref="K192:K200" si="393">CONCATENATE("static const CooGUI_tds ",A192, "_Normal = {", C192, ",", D192, ",", E192, ",", F192, ",",G192, ",", H192,",",  I192, ",", J192, "};")</f>
         <v>static const CooGUI_tds Pos_ALARM_DoubleArrowUp_Normal = {160,15,150,15,20,40,170,55};</v>
       </c>
       <c r="L192">
-        <f t="shared" ref="L192:L200" si="396">C192</f>
+        <f t="shared" ref="L192:L200" si="394">C192</f>
         <v>160</v>
       </c>
       <c r="M192" s="52">
-        <f t="shared" ref="M192:M200" si="397">D192 + $D$1</f>
+        <f t="shared" ref="M192:M200" si="395">D192 + $D$1</f>
         <v>39</v>
       </c>
       <c r="N192">
-        <f t="shared" ref="N192:Q200" si="398">E192</f>
+        <f t="shared" ref="N192:Q200" si="396">E192</f>
         <v>150</v>
       </c>
       <c r="O192">
-        <f t="shared" si="398"/>
+        <f t="shared" si="396"/>
         <v>15</v>
       </c>
       <c r="P192">
-        <f t="shared" si="398"/>
+        <f t="shared" si="396"/>
         <v>20</v>
       </c>
       <c r="Q192">
-        <f t="shared" si="398"/>
+        <f t="shared" si="396"/>
         <v>40</v>
       </c>
       <c r="R192" s="20">
-        <f t="shared" ref="R192:S200" si="399">N192+P192</f>
+        <f t="shared" ref="R192:S200" si="397">N192+P192</f>
         <v>170</v>
       </c>
       <c r="S192" s="20">
-        <f t="shared" si="399"/>
+        <f t="shared" si="397"/>
         <v>55</v>
       </c>
       <c r="T192" t="str">
-        <f t="shared" ref="T192:T200" si="400">CONCATENATE("static const CooGUI_tds ",A192, "_Flipped = {", L192, ",", M192, ",", N192, ",", O192, ",",P192, ",", Q192,",",  R192, ",", S192, "};")</f>
+        <f t="shared" ref="T192:T200" si="398">CONCATENATE("static const CooGUI_tds ",A192, "_Flipped = {", L192, ",", M192, ",", N192, ",", O192, ",",P192, ",", Q192,",",  R192, ",", S192, "};")</f>
         <v>static const CooGUI_tds Pos_ALARM_DoubleArrowUp_Flipped = {160,39,150,15,20,40,170,55};</v>
       </c>
       <c r="U192" t="str">
-        <f t="shared" ref="U192:U200" si="401">CONCATENATE("const CooGUI_tds* ",A192, ";")</f>
+        <f t="shared" ref="U192:U200" si="399">CONCATENATE("const CooGUI_tds* ",A192, ";")</f>
         <v>const CooGUI_tds* Pos_ALARM_DoubleArrowUp;</v>
       </c>
       <c r="V192">
-        <f t="shared" ref="V192:V200" si="402">(G192*H192)/1024</f>
+        <f t="shared" ref="V192:V200" si="400">(G192*H192)/1024</f>
         <v>0.78125</v>
       </c>
       <c r="W192" t="str">
-        <f t="shared" ref="W192:W200" si="403">CONCATENATE(A192, " = &amp;", B192,";")</f>
+        <f t="shared" ref="W192:W200" si="401">CONCATENATE(A192, " = &amp;", B192,";")</f>
         <v>Pos_ALARM_DoubleArrowUp = &amp;Pos_ALARM_DoubleArrowUp_Normal;</v>
       </c>
     </row>
@@ -21370,7 +21370,7 @@
         <v>263</v>
       </c>
       <c r="B193" t="str">
-        <f t="shared" si="393"/>
+        <f t="shared" si="391"/>
         <v>Pos_ALARM_SwitchTankArrow_Normal</v>
       </c>
       <c r="C193" s="9">
@@ -21397,63 +21397,63 @@
         <v>40</v>
       </c>
       <c r="I193" s="20">
+        <f t="shared" si="392"/>
+        <v>210</v>
+      </c>
+      <c r="J193" s="20">
+        <f t="shared" si="392"/>
+        <v>240</v>
+      </c>
+      <c r="K193" t="str">
+        <f t="shared" si="393"/>
+        <v>static const CooGUI_tds Pos_ALARM_SwitchTankArrow_Normal = {165,200,125,200,85,40,210,240};</v>
+      </c>
+      <c r="L193">
         <f t="shared" si="394"/>
+        <v>165</v>
+      </c>
+      <c r="M193" s="52">
+        <f t="shared" si="395"/>
+        <v>224</v>
+      </c>
+      <c r="N193">
+        <f t="shared" si="396"/>
+        <v>125</v>
+      </c>
+      <c r="O193">
+        <f t="shared" si="396"/>
+        <v>200</v>
+      </c>
+      <c r="P193">
+        <f t="shared" si="396"/>
+        <v>85</v>
+      </c>
+      <c r="Q193">
+        <f t="shared" si="396"/>
+        <v>40</v>
+      </c>
+      <c r="R193" s="20">
+        <f t="shared" si="397"/>
         <v>210</v>
       </c>
-      <c r="J193" s="20">
-        <f t="shared" si="394"/>
+      <c r="S193" s="20">
+        <f t="shared" si="397"/>
         <v>240</v>
       </c>
-      <c r="K193" t="str">
-        <f t="shared" si="395"/>
-        <v>static const CooGUI_tds Pos_ALARM_SwitchTankArrow_Normal = {165,200,125,200,85,40,210,240};</v>
-      </c>
-      <c r="L193">
-        <f t="shared" si="396"/>
-        <v>165</v>
-      </c>
-      <c r="M193" s="52">
-        <f t="shared" si="397"/>
-        <v>224</v>
-      </c>
-      <c r="N193">
+      <c r="T193" t="str">
         <f t="shared" si="398"/>
-        <v>125</v>
-      </c>
-      <c r="O193">
-        <f t="shared" si="398"/>
-        <v>200</v>
-      </c>
-      <c r="P193">
-        <f t="shared" si="398"/>
-        <v>85</v>
-      </c>
-      <c r="Q193">
-        <f t="shared" si="398"/>
-        <v>40</v>
-      </c>
-      <c r="R193" s="20">
+        <v>static const CooGUI_tds Pos_ALARM_SwitchTankArrow_Flipped = {165,224,125,200,85,40,210,240};</v>
+      </c>
+      <c r="U193" t="str">
         <f t="shared" si="399"/>
-        <v>210</v>
-      </c>
-      <c r="S193" s="20">
-        <f t="shared" si="399"/>
-        <v>240</v>
-      </c>
-      <c r="T193" t="str">
+        <v>const CooGUI_tds* Pos_ALARM_SwitchTankArrow;</v>
+      </c>
+      <c r="V193">
         <f t="shared" si="400"/>
-        <v>static const CooGUI_tds Pos_ALARM_SwitchTankArrow_Flipped = {165,224,125,200,85,40,210,240};</v>
-      </c>
-      <c r="U193" t="str">
+        <v>3.3203125</v>
+      </c>
+      <c r="W193" t="str">
         <f t="shared" si="401"/>
-        <v>const CooGUI_tds* Pos_ALARM_SwitchTankArrow;</v>
-      </c>
-      <c r="V193">
-        <f t="shared" si="402"/>
-        <v>3.3203125</v>
-      </c>
-      <c r="W193" t="str">
-        <f t="shared" si="403"/>
         <v>Pos_ALARM_SwitchTankArrow = &amp;Pos_ALARM_SwitchTankArrow_Normal;</v>
       </c>
     </row>
@@ -21462,7 +21462,7 @@
         <v>239</v>
       </c>
       <c r="B194" t="str">
-        <f t="shared" si="393"/>
+        <f t="shared" si="391"/>
         <v>Pos_ALARM_FullViolation_Normal</v>
       </c>
       <c r="C194" s="9">
@@ -21489,63 +21489,63 @@
         <v>60</v>
       </c>
       <c r="I194" s="20">
+        <f t="shared" si="392"/>
+        <v>295</v>
+      </c>
+      <c r="J194" s="20">
+        <f t="shared" si="392"/>
+        <v>120</v>
+      </c>
+      <c r="K194" t="str">
+        <f t="shared" si="393"/>
+        <v>static const CooGUI_tds Pos_ALARM_FullViolation_Normal = {160,70,28,60,267,60,295,120};</v>
+      </c>
+      <c r="L194">
         <f t="shared" si="394"/>
+        <v>160</v>
+      </c>
+      <c r="M194" s="52">
+        <f t="shared" si="395"/>
+        <v>94</v>
+      </c>
+      <c r="N194">
+        <f t="shared" si="396"/>
+        <v>28</v>
+      </c>
+      <c r="O194">
+        <f t="shared" si="396"/>
+        <v>60</v>
+      </c>
+      <c r="P194">
+        <f t="shared" si="396"/>
+        <v>267</v>
+      </c>
+      <c r="Q194">
+        <f t="shared" si="396"/>
+        <v>60</v>
+      </c>
+      <c r="R194" s="20">
+        <f t="shared" si="397"/>
         <v>295</v>
       </c>
-      <c r="J194" s="20">
-        <f t="shared" si="394"/>
+      <c r="S194" s="20">
+        <f t="shared" si="397"/>
         <v>120</v>
       </c>
-      <c r="K194" t="str">
-        <f t="shared" si="395"/>
-        <v>static const CooGUI_tds Pos_ALARM_FullViolation_Normal = {160,70,28,60,267,60,295,120};</v>
-      </c>
-      <c r="L194">
-        <f t="shared" si="396"/>
-        <v>160</v>
-      </c>
-      <c r="M194" s="52">
-        <f t="shared" si="397"/>
-        <v>94</v>
-      </c>
-      <c r="N194">
+      <c r="T194" t="str">
         <f t="shared" si="398"/>
-        <v>28</v>
-      </c>
-      <c r="O194">
-        <f t="shared" si="398"/>
-        <v>60</v>
-      </c>
-      <c r="P194">
-        <f t="shared" si="398"/>
-        <v>267</v>
-      </c>
-      <c r="Q194">
-        <f t="shared" si="398"/>
-        <v>60</v>
-      </c>
-      <c r="R194" s="20">
+        <v>static const CooGUI_tds Pos_ALARM_FullViolation_Flipped = {160,94,28,60,267,60,295,120};</v>
+      </c>
+      <c r="U194" t="str">
         <f t="shared" si="399"/>
-        <v>295</v>
-      </c>
-      <c r="S194" s="20">
-        <f t="shared" si="399"/>
-        <v>120</v>
-      </c>
-      <c r="T194" t="str">
+        <v>const CooGUI_tds* Pos_ALARM_FullViolation;</v>
+      </c>
+      <c r="V194">
         <f t="shared" si="400"/>
-        <v>static const CooGUI_tds Pos_ALARM_FullViolation_Flipped = {160,94,28,60,267,60,295,120};</v>
-      </c>
-      <c r="U194" t="str">
+        <v>15.64453125</v>
+      </c>
+      <c r="W194" t="str">
         <f t="shared" si="401"/>
-        <v>const CooGUI_tds* Pos_ALARM_FullViolation;</v>
-      </c>
-      <c r="V194">
-        <f t="shared" si="402"/>
-        <v>15.64453125</v>
-      </c>
-      <c r="W194" t="str">
-        <f t="shared" si="403"/>
         <v>Pos_ALARM_FullViolation = &amp;Pos_ALARM_FullViolation_Normal;</v>
       </c>
     </row>
@@ -21554,7 +21554,7 @@
         <v>295</v>
       </c>
       <c r="B195" t="str">
-        <f t="shared" ref="B195" si="404">CONCATENATE(A195, "_Normal")</f>
+        <f t="shared" ref="B195" si="402">CONCATENATE(A195, "_Normal")</f>
         <v>Pos_ALARM_BatteryLine0_Normal</v>
       </c>
       <c r="C195" s="50">
@@ -21582,63 +21582,63 @@
         <v>30</v>
       </c>
       <c r="I195" s="20">
-        <f t="shared" ref="I195" si="405">E195+G195</f>
+        <f t="shared" ref="I195" si="403">E195+G195</f>
         <v>295</v>
       </c>
       <c r="J195" s="20">
-        <f t="shared" ref="J195" si="406">F195+H195</f>
+        <f t="shared" ref="J195" si="404">F195+H195</f>
         <v>90</v>
       </c>
       <c r="K195" t="str">
-        <f t="shared" ref="K195" si="407">CONCATENATE("static const CooGUI_tds ",A195, "_Normal = {", C195, ",", D195, ",", E195, ",", F195, ",",G195, ",", H195,",",  I195, ",", J195, "};")</f>
+        <f t="shared" ref="K195" si="405">CONCATENATE("static const CooGUI_tds ",A195, "_Normal = {", C195, ",", D195, ",", E195, ",", F195, ",",G195, ",", H195,",",  I195, ",", J195, "};")</f>
         <v>static const CooGUI_tds Pos_ALARM_BatteryLine0_Normal = {160,67,28,60,267,30,295,90};</v>
       </c>
       <c r="L195">
-        <f t="shared" ref="L195" si="408">C195</f>
+        <f t="shared" ref="L195" si="406">C195</f>
         <v>160</v>
       </c>
       <c r="M195" s="52">
-        <f t="shared" ref="M195" si="409">D195 + $D$1</f>
+        <f t="shared" ref="M195" si="407">D195 + $D$1</f>
         <v>91</v>
       </c>
       <c r="N195">
-        <f t="shared" ref="N195" si="410">E195</f>
+        <f t="shared" ref="N195" si="408">E195</f>
         <v>28</v>
       </c>
       <c r="O195">
-        <f t="shared" ref="O195" si="411">F195</f>
+        <f t="shared" ref="O195" si="409">F195</f>
         <v>60</v>
       </c>
       <c r="P195">
-        <f t="shared" ref="P195" si="412">G195</f>
+        <f t="shared" ref="P195" si="410">G195</f>
         <v>267</v>
       </c>
       <c r="Q195">
-        <f t="shared" ref="Q195" si="413">H195</f>
+        <f t="shared" ref="Q195" si="411">H195</f>
         <v>30</v>
       </c>
       <c r="R195" s="20">
-        <f t="shared" ref="R195" si="414">N195+P195</f>
+        <f t="shared" ref="R195" si="412">N195+P195</f>
         <v>295</v>
       </c>
       <c r="S195" s="20">
-        <f t="shared" ref="S195" si="415">O195+Q195</f>
+        <f t="shared" ref="S195" si="413">O195+Q195</f>
         <v>90</v>
       </c>
       <c r="T195" t="str">
-        <f t="shared" ref="T195" si="416">CONCATENATE("static const CooGUI_tds ",A195, "_Flipped = {", L195, ",", M195, ",", N195, ",", O195, ",",P195, ",", Q195,",",  R195, ",", S195, "};")</f>
+        <f t="shared" ref="T195" si="414">CONCATENATE("static const CooGUI_tds ",A195, "_Flipped = {", L195, ",", M195, ",", N195, ",", O195, ",",P195, ",", Q195,",",  R195, ",", S195, "};")</f>
         <v>static const CooGUI_tds Pos_ALARM_BatteryLine0_Flipped = {160,91,28,60,267,30,295,90};</v>
       </c>
       <c r="U195" t="str">
-        <f t="shared" ref="U195" si="417">CONCATENATE("const CooGUI_tds* ",A195, ";")</f>
+        <f t="shared" ref="U195" si="415">CONCATENATE("const CooGUI_tds* ",A195, ";")</f>
         <v>const CooGUI_tds* Pos_ALARM_BatteryLine0;</v>
       </c>
       <c r="V195">
-        <f t="shared" ref="V195" si="418">(G195*H195)/1024</f>
+        <f t="shared" ref="V195" si="416">(G195*H195)/1024</f>
         <v>7.822265625</v>
       </c>
       <c r="W195" t="str">
-        <f t="shared" ref="W195" si="419">CONCATENATE(A195, " = &amp;", B195,";")</f>
+        <f t="shared" ref="W195" si="417">CONCATENATE(A195, " = &amp;", B195,";")</f>
         <v>Pos_ALARM_BatteryLine0 = &amp;Pos_ALARM_BatteryLine0_Normal;</v>
       </c>
     </row>
@@ -21647,7 +21647,7 @@
         <v>296</v>
       </c>
       <c r="B196" t="str">
-        <f t="shared" ref="B196" si="420">CONCATENATE(A196, "_Normal")</f>
+        <f t="shared" ref="B196" si="418">CONCATENATE(A196, "_Normal")</f>
         <v>Pos_ALARM_BatteryLine1_Normal</v>
       </c>
       <c r="C196" s="50">
@@ -21675,63 +21675,63 @@
         <v>30</v>
       </c>
       <c r="I196" s="20">
-        <f t="shared" ref="I196" si="421">E196+G196</f>
+        <f t="shared" ref="I196" si="419">E196+G196</f>
         <v>295</v>
       </c>
       <c r="J196" s="20">
-        <f t="shared" ref="J196" si="422">F196+H196</f>
+        <f t="shared" ref="J196" si="420">F196+H196</f>
         <v>120</v>
       </c>
       <c r="K196" t="str">
-        <f t="shared" ref="K196" si="423">CONCATENATE("static const CooGUI_tds ",A196, "_Normal = {", C196, ",", D196, ",", E196, ",", F196, ",",G196, ",", H196,",",  I196, ",", J196, "};")</f>
+        <f t="shared" ref="K196" si="421">CONCATENATE("static const CooGUI_tds ",A196, "_Normal = {", C196, ",", D196, ",", E196, ",", F196, ",",G196, ",", H196,",",  I196, ",", J196, "};")</f>
         <v>static const CooGUI_tds Pos_ALARM_BatteryLine1_Normal = {160,97,28,90,267,30,295,120};</v>
       </c>
       <c r="L196">
-        <f t="shared" ref="L196" si="424">C196</f>
+        <f t="shared" ref="L196" si="422">C196</f>
         <v>160</v>
       </c>
       <c r="M196" s="52">
-        <f t="shared" ref="M196" si="425">D196 + $D$1</f>
+        <f t="shared" ref="M196" si="423">D196 + $D$1</f>
         <v>121</v>
       </c>
       <c r="N196">
-        <f t="shared" ref="N196" si="426">E196</f>
+        <f t="shared" ref="N196" si="424">E196</f>
         <v>28</v>
       </c>
       <c r="O196">
-        <f t="shared" ref="O196" si="427">F196</f>
+        <f t="shared" ref="O196" si="425">F196</f>
         <v>90</v>
       </c>
       <c r="P196">
-        <f t="shared" ref="P196" si="428">G196</f>
+        <f t="shared" ref="P196" si="426">G196</f>
         <v>267</v>
       </c>
       <c r="Q196">
-        <f t="shared" ref="Q196" si="429">H196</f>
+        <f t="shared" ref="Q196" si="427">H196</f>
         <v>30</v>
       </c>
       <c r="R196" s="20">
-        <f t="shared" ref="R196" si="430">N196+P196</f>
+        <f t="shared" ref="R196" si="428">N196+P196</f>
         <v>295</v>
       </c>
       <c r="S196" s="20">
-        <f t="shared" ref="S196" si="431">O196+Q196</f>
+        <f t="shared" ref="S196" si="429">O196+Q196</f>
         <v>120</v>
       </c>
       <c r="T196" t="str">
-        <f t="shared" ref="T196" si="432">CONCATENATE("static const CooGUI_tds ",A196, "_Flipped = {", L196, ",", M196, ",", N196, ",", O196, ",",P196, ",", Q196,",",  R196, ",", S196, "};")</f>
+        <f t="shared" ref="T196" si="430">CONCATENATE("static const CooGUI_tds ",A196, "_Flipped = {", L196, ",", M196, ",", N196, ",", O196, ",",P196, ",", Q196,",",  R196, ",", S196, "};")</f>
         <v>static const CooGUI_tds Pos_ALARM_BatteryLine1_Flipped = {160,121,28,90,267,30,295,120};</v>
       </c>
       <c r="U196" t="str">
-        <f t="shared" ref="U196" si="433">CONCATENATE("const CooGUI_tds* ",A196, ";")</f>
+        <f t="shared" ref="U196" si="431">CONCATENATE("const CooGUI_tds* ",A196, ";")</f>
         <v>const CooGUI_tds* Pos_ALARM_BatteryLine1;</v>
       </c>
       <c r="V196">
-        <f t="shared" ref="V196" si="434">(G196*H196)/1024</f>
+        <f t="shared" ref="V196" si="432">(G196*H196)/1024</f>
         <v>7.822265625</v>
       </c>
       <c r="W196" t="str">
-        <f t="shared" ref="W196" si="435">CONCATENATE(A196, " = &amp;", B196,";")</f>
+        <f t="shared" ref="W196" si="433">CONCATENATE(A196, " = &amp;", B196,";")</f>
         <v>Pos_ALARM_BatteryLine1 = &amp;Pos_ALARM_BatteryLine1_Normal;</v>
       </c>
     </row>
@@ -21740,7 +21740,7 @@
         <v>224</v>
       </c>
       <c r="B197" t="str">
-        <f t="shared" si="393"/>
+        <f t="shared" si="391"/>
         <v>Pos_Depth_In_Menu_Normal</v>
       </c>
       <c r="C197" s="9">
@@ -21762,63 +21762,63 @@
         <v>25</v>
       </c>
       <c r="I197" s="20">
+        <f t="shared" si="392"/>
+        <v>293</v>
+      </c>
+      <c r="J197" s="20">
+        <f t="shared" si="392"/>
+        <v>25</v>
+      </c>
+      <c r="K197" t="str">
+        <f t="shared" si="393"/>
+        <v>static const CooGUI_tds Pos_Depth_In_Menu_Normal = {268,0,203,0,90,25,293,25};</v>
+      </c>
+      <c r="L197">
         <f t="shared" si="394"/>
+        <v>268</v>
+      </c>
+      <c r="M197" s="52">
+        <f t="shared" si="395"/>
+        <v>24</v>
+      </c>
+      <c r="N197">
+        <f t="shared" si="396"/>
+        <v>203</v>
+      </c>
+      <c r="O197">
+        <f t="shared" si="396"/>
+        <v>0</v>
+      </c>
+      <c r="P197">
+        <f t="shared" si="396"/>
+        <v>90</v>
+      </c>
+      <c r="Q197">
+        <f t="shared" si="396"/>
+        <v>25</v>
+      </c>
+      <c r="R197" s="20">
+        <f t="shared" si="397"/>
         <v>293</v>
       </c>
-      <c r="J197" s="20">
-        <f t="shared" si="394"/>
+      <c r="S197" s="20">
+        <f t="shared" si="397"/>
         <v>25</v>
       </c>
-      <c r="K197" t="str">
-        <f t="shared" si="395"/>
-        <v>static const CooGUI_tds Pos_Depth_In_Menu_Normal = {268,0,203,0,90,25,293,25};</v>
-      </c>
-      <c r="L197">
-        <f t="shared" si="396"/>
-        <v>268</v>
-      </c>
-      <c r="M197" s="52">
-        <f t="shared" si="397"/>
-        <v>24</v>
-      </c>
-      <c r="N197">
+      <c r="T197" t="str">
         <f t="shared" si="398"/>
-        <v>203</v>
-      </c>
-      <c r="O197">
-        <f t="shared" si="398"/>
-        <v>0</v>
-      </c>
-      <c r="P197">
-        <f t="shared" si="398"/>
-        <v>90</v>
-      </c>
-      <c r="Q197">
-        <f t="shared" si="398"/>
-        <v>25</v>
-      </c>
-      <c r="R197" s="20">
+        <v>static const CooGUI_tds Pos_Depth_In_Menu_Flipped = {268,24,203,0,90,25,293,25};</v>
+      </c>
+      <c r="U197" t="str">
         <f t="shared" si="399"/>
-        <v>293</v>
-      </c>
-      <c r="S197" s="20">
-        <f t="shared" si="399"/>
-        <v>25</v>
-      </c>
-      <c r="T197" t="str">
+        <v>const CooGUI_tds* Pos_Depth_In_Menu;</v>
+      </c>
+      <c r="V197">
         <f t="shared" si="400"/>
-        <v>static const CooGUI_tds Pos_Depth_In_Menu_Flipped = {268,24,203,0,90,25,293,25};</v>
-      </c>
-      <c r="U197" t="str">
+        <v>2.197265625</v>
+      </c>
+      <c r="W197" t="str">
         <f t="shared" si="401"/>
-        <v>const CooGUI_tds* Pos_Depth_In_Menu;</v>
-      </c>
-      <c r="V197">
-        <f t="shared" si="402"/>
-        <v>2.197265625</v>
-      </c>
-      <c r="W197" t="str">
-        <f t="shared" si="403"/>
         <v>Pos_Depth_In_Menu = &amp;Pos_Depth_In_Menu_Normal;</v>
       </c>
     </row>
@@ -21827,7 +21827,7 @@
         <v>221</v>
       </c>
       <c r="B198" t="str">
-        <f t="shared" si="393"/>
+        <f t="shared" si="391"/>
         <v>Pos_SetGFHighMenu_TTS_Text_Normal</v>
       </c>
       <c r="C198" s="26">
@@ -21852,63 +21852,63 @@
         <v>45</v>
       </c>
       <c r="I198" s="20">
+        <f t="shared" si="392"/>
+        <v>310</v>
+      </c>
+      <c r="J198" s="20">
+        <f t="shared" si="392"/>
+        <v>105</v>
+      </c>
+      <c r="K198" t="str">
+        <f t="shared" si="393"/>
+        <v>static const CooGUI_tds Pos_SetGFHighMenu_TTS_Text_Normal = {235,60,160,60,150,45,310,105};</v>
+      </c>
+      <c r="L198">
         <f t="shared" si="394"/>
+        <v>235</v>
+      </c>
+      <c r="M198" s="52">
+        <f t="shared" si="395"/>
+        <v>84</v>
+      </c>
+      <c r="N198">
+        <f t="shared" si="396"/>
+        <v>160</v>
+      </c>
+      <c r="O198">
+        <f t="shared" si="396"/>
+        <v>60</v>
+      </c>
+      <c r="P198">
+        <f t="shared" si="396"/>
+        <v>150</v>
+      </c>
+      <c r="Q198">
+        <f t="shared" si="396"/>
+        <v>45</v>
+      </c>
+      <c r="R198" s="20">
+        <f t="shared" si="397"/>
         <v>310</v>
       </c>
-      <c r="J198" s="20">
-        <f t="shared" si="394"/>
+      <c r="S198" s="20">
+        <f t="shared" si="397"/>
         <v>105</v>
       </c>
-      <c r="K198" t="str">
-        <f t="shared" si="395"/>
-        <v>static const CooGUI_tds Pos_SetGFHighMenu_TTS_Text_Normal = {235,60,160,60,150,45,310,105};</v>
-      </c>
-      <c r="L198">
-        <f t="shared" si="396"/>
-        <v>235</v>
-      </c>
-      <c r="M198" s="52">
-        <f t="shared" si="397"/>
-        <v>84</v>
-      </c>
-      <c r="N198">
+      <c r="T198" t="str">
         <f t="shared" si="398"/>
-        <v>160</v>
-      </c>
-      <c r="O198">
-        <f t="shared" si="398"/>
-        <v>60</v>
-      </c>
-      <c r="P198">
-        <f t="shared" si="398"/>
-        <v>150</v>
-      </c>
-      <c r="Q198">
-        <f t="shared" si="398"/>
-        <v>45</v>
-      </c>
-      <c r="R198" s="20">
+        <v>static const CooGUI_tds Pos_SetGFHighMenu_TTS_Text_Flipped = {235,84,160,60,150,45,310,105};</v>
+      </c>
+      <c r="U198" t="str">
         <f t="shared" si="399"/>
-        <v>310</v>
-      </c>
-      <c r="S198" s="20">
-        <f t="shared" si="399"/>
-        <v>105</v>
-      </c>
-      <c r="T198" t="str">
+        <v>const CooGUI_tds* Pos_SetGFHighMenu_TTS_Text;</v>
+      </c>
+      <c r="V198">
         <f t="shared" si="400"/>
-        <v>static const CooGUI_tds Pos_SetGFHighMenu_TTS_Text_Flipped = {235,84,160,60,150,45,310,105};</v>
-      </c>
-      <c r="U198" t="str">
+        <v>6.591796875</v>
+      </c>
+      <c r="W198" t="str">
         <f t="shared" si="401"/>
-        <v>const CooGUI_tds* Pos_SetGFHighMenu_TTS_Text;</v>
-      </c>
-      <c r="V198">
-        <f t="shared" si="402"/>
-        <v>6.591796875</v>
-      </c>
-      <c r="W198" t="str">
-        <f t="shared" si="403"/>
         <v>Pos_SetGFHighMenu_TTS_Text = &amp;Pos_SetGFHighMenu_TTS_Text_Normal;</v>
       </c>
     </row>
@@ -21917,7 +21917,7 @@
         <v>223</v>
       </c>
       <c r="B199" t="str">
-        <f t="shared" si="393"/>
+        <f t="shared" si="391"/>
         <v>Pos_SetGFHighMenu_MIN_Value_Normal</v>
       </c>
       <c r="C199" s="26">
@@ -21943,63 +21943,63 @@
         <v>45</v>
       </c>
       <c r="I199" s="20">
+        <f t="shared" si="392"/>
+        <v>210</v>
+      </c>
+      <c r="J199" s="20">
+        <f t="shared" si="392"/>
+        <v>150</v>
+      </c>
+      <c r="K199" t="str">
+        <f t="shared" si="393"/>
+        <v>static const CooGUI_tds Pos_SetGFHighMenu_MIN_Value_Normal = {210,105,160,105,50,45,210,150};</v>
+      </c>
+      <c r="L199">
         <f t="shared" si="394"/>
         <v>210</v>
       </c>
-      <c r="J199" s="20">
-        <f t="shared" si="394"/>
+      <c r="M199" s="52">
+        <f t="shared" si="395"/>
+        <v>129</v>
+      </c>
+      <c r="N199">
+        <f t="shared" si="396"/>
+        <v>160</v>
+      </c>
+      <c r="O199">
+        <f t="shared" si="396"/>
+        <v>105</v>
+      </c>
+      <c r="P199">
+        <f t="shared" si="396"/>
+        <v>50</v>
+      </c>
+      <c r="Q199">
+        <f t="shared" si="396"/>
+        <v>45</v>
+      </c>
+      <c r="R199" s="20">
+        <f t="shared" si="397"/>
+        <v>210</v>
+      </c>
+      <c r="S199" s="20">
+        <f t="shared" si="397"/>
         <v>150</v>
       </c>
-      <c r="K199" t="str">
-        <f t="shared" si="395"/>
-        <v>static const CooGUI_tds Pos_SetGFHighMenu_MIN_Value_Normal = {210,105,160,105,50,45,210,150};</v>
-      </c>
-      <c r="L199">
-        <f t="shared" si="396"/>
-        <v>210</v>
-      </c>
-      <c r="M199" s="52">
-        <f t="shared" si="397"/>
-        <v>129</v>
-      </c>
-      <c r="N199">
+      <c r="T199" t="str">
         <f t="shared" si="398"/>
-        <v>160</v>
-      </c>
-      <c r="O199">
-        <f t="shared" si="398"/>
-        <v>105</v>
-      </c>
-      <c r="P199">
-        <f t="shared" si="398"/>
-        <v>50</v>
-      </c>
-      <c r="Q199">
-        <f t="shared" si="398"/>
-        <v>45</v>
-      </c>
-      <c r="R199" s="20">
+        <v>static const CooGUI_tds Pos_SetGFHighMenu_MIN_Value_Flipped = {210,129,160,105,50,45,210,150};</v>
+      </c>
+      <c r="U199" t="str">
         <f t="shared" si="399"/>
-        <v>210</v>
-      </c>
-      <c r="S199" s="20">
-        <f t="shared" si="399"/>
-        <v>150</v>
-      </c>
-      <c r="T199" t="str">
+        <v>const CooGUI_tds* Pos_SetGFHighMenu_MIN_Value;</v>
+      </c>
+      <c r="V199">
         <f t="shared" si="400"/>
-        <v>static const CooGUI_tds Pos_SetGFHighMenu_MIN_Value_Flipped = {210,129,160,105,50,45,210,150};</v>
-      </c>
-      <c r="U199" t="str">
+        <v>2.197265625</v>
+      </c>
+      <c r="W199" t="str">
         <f t="shared" si="401"/>
-        <v>const CooGUI_tds* Pos_SetGFHighMenu_MIN_Value;</v>
-      </c>
-      <c r="V199">
-        <f t="shared" si="402"/>
-        <v>2.197265625</v>
-      </c>
-      <c r="W199" t="str">
-        <f t="shared" si="403"/>
         <v>Pos_SetGFHighMenu_MIN_Value = &amp;Pos_SetGFHighMenu_MIN_Value_Normal;</v>
       </c>
     </row>
@@ -22008,7 +22008,7 @@
         <v>222</v>
       </c>
       <c r="B200" t="str">
-        <f t="shared" si="393"/>
+        <f t="shared" si="391"/>
         <v>Pos_SetGFHighMenu_MIN_Text_Normal</v>
       </c>
       <c r="C200" s="26">
@@ -22036,63 +22036,63 @@
         <v>45</v>
       </c>
       <c r="I200" s="20">
+        <f t="shared" si="392"/>
+        <v>310</v>
+      </c>
+      <c r="J200" s="20">
+        <f t="shared" si="392"/>
+        <v>150</v>
+      </c>
+      <c r="K200" t="str">
+        <f t="shared" si="393"/>
+        <v>static const CooGUI_tds Pos_SetGFHighMenu_MIN_Text_Normal = {220,105,210,105,100,45,310,150};</v>
+      </c>
+      <c r="L200">
         <f t="shared" si="394"/>
+        <v>220</v>
+      </c>
+      <c r="M200" s="52">
+        <f t="shared" si="395"/>
+        <v>129</v>
+      </c>
+      <c r="N200">
+        <f t="shared" si="396"/>
+        <v>210</v>
+      </c>
+      <c r="O200">
+        <f t="shared" si="396"/>
+        <v>105</v>
+      </c>
+      <c r="P200">
+        <f t="shared" si="396"/>
+        <v>100</v>
+      </c>
+      <c r="Q200">
+        <f t="shared" si="396"/>
+        <v>45</v>
+      </c>
+      <c r="R200" s="20">
+        <f t="shared" si="397"/>
         <v>310</v>
       </c>
-      <c r="J200" s="20">
-        <f t="shared" si="394"/>
+      <c r="S200" s="20">
+        <f t="shared" si="397"/>
         <v>150</v>
       </c>
-      <c r="K200" t="str">
-        <f t="shared" si="395"/>
-        <v>static const CooGUI_tds Pos_SetGFHighMenu_MIN_Text_Normal = {220,105,210,105,100,45,310,150};</v>
-      </c>
-      <c r="L200">
-        <f t="shared" si="396"/>
-        <v>220</v>
-      </c>
-      <c r="M200" s="52">
-        <f t="shared" si="397"/>
-        <v>129</v>
-      </c>
-      <c r="N200">
+      <c r="T200" t="str">
         <f t="shared" si="398"/>
-        <v>210</v>
-      </c>
-      <c r="O200">
-        <f t="shared" si="398"/>
-        <v>105</v>
-      </c>
-      <c r="P200">
-        <f t="shared" si="398"/>
-        <v>100</v>
-      </c>
-      <c r="Q200">
-        <f t="shared" si="398"/>
-        <v>45</v>
-      </c>
-      <c r="R200" s="20">
+        <v>static const CooGUI_tds Pos_SetGFHighMenu_MIN_Text_Flipped = {220,129,210,105,100,45,310,150};</v>
+      </c>
+      <c r="U200" t="str">
         <f t="shared" si="399"/>
-        <v>310</v>
-      </c>
-      <c r="S200" s="20">
-        <f t="shared" si="399"/>
-        <v>150</v>
-      </c>
-      <c r="T200" t="str">
+        <v>const CooGUI_tds* Pos_SetGFHighMenu_MIN_Text;</v>
+      </c>
+      <c r="V200">
         <f t="shared" si="400"/>
-        <v>static const CooGUI_tds Pos_SetGFHighMenu_MIN_Text_Flipped = {220,129,210,105,100,45,310,150};</v>
-      </c>
-      <c r="U200" t="str">
+        <v>4.39453125</v>
+      </c>
+      <c r="W200" t="str">
         <f t="shared" si="401"/>
-        <v>const CooGUI_tds* Pos_SetGFHighMenu_MIN_Text;</v>
-      </c>
-      <c r="V200">
-        <f t="shared" si="402"/>
-        <v>4.39453125</v>
-      </c>
-      <c r="W200" t="str">
-        <f t="shared" si="403"/>
         <v>Pos_SetGFHighMenu_MIN_Text = &amp;Pos_SetGFHighMenu_MIN_Text_Normal;</v>
       </c>
     </row>
@@ -22101,7 +22101,7 @@
         <v>281</v>
       </c>
       <c r="B201" t="str">
-        <f t="shared" ref="B201" si="436">CONCATENATE(A201, "_Normal")</f>
+        <f t="shared" ref="B201" si="434">CONCATENATE(A201, "_Normal")</f>
         <v>Pos_DepthDiveTime_DepthTittle_Normal</v>
       </c>
       <c r="C201" s="9">
@@ -22126,63 +22126,63 @@
         <v>28</v>
       </c>
       <c r="I201" s="26">
-        <f t="shared" ref="I201" si="437">E201+G201</f>
+        <f t="shared" ref="I201" si="435">E201+G201</f>
         <v>295</v>
       </c>
       <c r="J201" s="26">
-        <f t="shared" ref="J201" si="438">F201+H201</f>
+        <f t="shared" ref="J201" si="436">F201+H201</f>
         <v>28</v>
       </c>
       <c r="K201" t="str">
-        <f t="shared" ref="K201" si="439">CONCATENATE("static const CooGUI_tds ",A201, "_Normal = {", C201, ",", D201, ",", E201, ",", F201, ",",G201, ",", H201,",",  I201, ",", J201, "};")</f>
+        <f t="shared" ref="K201" si="437">CONCATENATE("static const CooGUI_tds ",A201, "_Normal = {", C201, ",", D201, ",", E201, ",", F201, ",",G201, ",", H201,",",  I201, ",", J201, "};")</f>
         <v>static const CooGUI_tds Pos_DepthDiveTime_DepthTittle_Normal = {160,0,25,0,270,28,295,28};</v>
       </c>
       <c r="L201">
-        <f t="shared" ref="L201" si="440">C201</f>
+        <f t="shared" ref="L201" si="438">C201</f>
         <v>160</v>
       </c>
       <c r="M201" s="52">
-        <f t="shared" ref="M201" si="441">D201 + $D$1</f>
+        <f t="shared" ref="M201" si="439">D201 + $D$1</f>
         <v>24</v>
       </c>
       <c r="N201">
-        <f t="shared" ref="N201" si="442">E201</f>
+        <f t="shared" ref="N201" si="440">E201</f>
         <v>25</v>
       </c>
       <c r="O201">
-        <f t="shared" ref="O201" si="443">F201</f>
+        <f t="shared" ref="O201" si="441">F201</f>
         <v>0</v>
       </c>
       <c r="P201">
-        <f t="shared" ref="P201" si="444">G201</f>
+        <f t="shared" ref="P201" si="442">G201</f>
         <v>270</v>
       </c>
       <c r="Q201">
-        <f t="shared" ref="Q201" si="445">H201</f>
+        <f t="shared" ref="Q201" si="443">H201</f>
         <v>28</v>
       </c>
       <c r="R201" s="20">
-        <f t="shared" ref="R201" si="446">N201+P201</f>
+        <f t="shared" ref="R201" si="444">N201+P201</f>
         <v>295</v>
       </c>
       <c r="S201" s="20">
-        <f t="shared" ref="S201" si="447">O201+Q201</f>
+        <f t="shared" ref="S201" si="445">O201+Q201</f>
         <v>28</v>
       </c>
       <c r="T201" t="str">
-        <f t="shared" ref="T201" si="448">CONCATENATE("static const CooGUI_tds ",A201, "_Flipped = {", L201, ",", M201, ",", N201, ",", O201, ",",P201, ",", Q201,",",  R201, ",", S201, "};")</f>
+        <f t="shared" ref="T201" si="446">CONCATENATE("static const CooGUI_tds ",A201, "_Flipped = {", L201, ",", M201, ",", N201, ",", O201, ",",P201, ",", Q201,",",  R201, ",", S201, "};")</f>
         <v>static const CooGUI_tds Pos_DepthDiveTime_DepthTittle_Flipped = {160,24,25,0,270,28,295,28};</v>
       </c>
       <c r="U201" t="str">
-        <f t="shared" ref="U201" si="449">CONCATENATE("const CooGUI_tds* ",A201, ";")</f>
+        <f t="shared" ref="U201" si="447">CONCATENATE("const CooGUI_tds* ",A201, ";")</f>
         <v>const CooGUI_tds* Pos_DepthDiveTime_DepthTittle;</v>
       </c>
       <c r="V201">
-        <f t="shared" ref="V201" si="450">(G201*H201)/1024</f>
+        <f t="shared" ref="V201" si="448">(G201*H201)/1024</f>
         <v>7.3828125</v>
       </c>
       <c r="W201" t="str">
-        <f t="shared" ref="W201" si="451">CONCATENATE(A201, " = &amp;", B201,";")</f>
+        <f t="shared" ref="W201" si="449">CONCATENATE(A201, " = &amp;", B201,";")</f>
         <v>Pos_DepthDiveTime_DepthTittle = &amp;Pos_DepthDiveTime_DepthTittle_Normal;</v>
       </c>
     </row>
@@ -22191,7 +22191,7 @@
         <v>282</v>
       </c>
       <c r="B202" t="str">
-        <f t="shared" ref="B202:B206" si="452">CONCATENATE(A202, "_Normal")</f>
+        <f t="shared" ref="B202:B206" si="450">CONCATENATE(A202, "_Normal")</f>
         <v>Pos_DepthDiveTime_DepthImperial_Normal</v>
       </c>
       <c r="C202" s="26">
@@ -22218,63 +22218,63 @@
         <v>76</v>
       </c>
       <c r="I202" s="26">
-        <f t="shared" ref="I202:I206" si="453">E202+G202</f>
+        <f t="shared" ref="I202:I206" si="451">E202+G202</f>
         <v>255</v>
       </c>
       <c r="J202" s="26">
-        <f t="shared" ref="J202:J206" si="454">F202+H202</f>
+        <f t="shared" ref="J202:J206" si="452">F202+H202</f>
         <v>104</v>
       </c>
       <c r="K202" t="str">
-        <f t="shared" ref="K202:K206" si="455">CONCATENATE("static const CooGUI_tds ",A202, "_Normal = {", C202, ",", D202, ",", E202, ",", F202, ",",G202, ",", H202,",",  I202, ",", J202, "};")</f>
+        <f t="shared" ref="K202:K206" si="453">CONCATENATE("static const CooGUI_tds ",A202, "_Normal = {", C202, ",", D202, ",", E202, ",", F202, ",",G202, ",", H202,",",  I202, ",", J202, "};")</f>
         <v>static const CooGUI_tds Pos_DepthDiveTime_DepthImperial_Normal = {160,10,25,28,230,76,255,104};</v>
       </c>
       <c r="L202">
-        <f t="shared" ref="L202:L206" si="456">C202</f>
+        <f t="shared" ref="L202:L206" si="454">C202</f>
         <v>160</v>
       </c>
       <c r="M202" s="52">
-        <f t="shared" ref="M202:M206" si="457">D202 + $D$1</f>
+        <f t="shared" ref="M202:M206" si="455">D202 + $D$1</f>
         <v>34</v>
       </c>
       <c r="N202">
-        <f t="shared" ref="N202:N206" si="458">E202</f>
+        <f t="shared" ref="N202:N206" si="456">E202</f>
         <v>25</v>
       </c>
       <c r="O202">
-        <f t="shared" ref="O202:O206" si="459">F202</f>
+        <f t="shared" ref="O202:O206" si="457">F202</f>
         <v>28</v>
       </c>
       <c r="P202">
-        <f t="shared" ref="P202:P206" si="460">G202</f>
+        <f t="shared" ref="P202:P206" si="458">G202</f>
         <v>230</v>
       </c>
       <c r="Q202">
-        <f t="shared" ref="Q202:Q206" si="461">H202</f>
+        <f t="shared" ref="Q202:Q206" si="459">H202</f>
         <v>76</v>
       </c>
       <c r="R202" s="20">
-        <f t="shared" ref="R202:R206" si="462">N202+P202</f>
+        <f t="shared" ref="R202:R206" si="460">N202+P202</f>
         <v>255</v>
       </c>
       <c r="S202" s="20">
-        <f t="shared" ref="S202:S206" si="463">O202+Q202</f>
+        <f t="shared" ref="S202:S206" si="461">O202+Q202</f>
         <v>104</v>
       </c>
       <c r="T202" t="str">
-        <f t="shared" ref="T202:T206" si="464">CONCATENATE("static const CooGUI_tds ",A202, "_Flipped = {", L202, ",", M202, ",", N202, ",", O202, ",",P202, ",", Q202,",",  R202, ",", S202, "};")</f>
+        <f t="shared" ref="T202:T206" si="462">CONCATENATE("static const CooGUI_tds ",A202, "_Flipped = {", L202, ",", M202, ",", N202, ",", O202, ",",P202, ",", Q202,",",  R202, ",", S202, "};")</f>
         <v>static const CooGUI_tds Pos_DepthDiveTime_DepthImperial_Flipped = {160,34,25,28,230,76,255,104};</v>
       </c>
       <c r="U202" t="str">
-        <f t="shared" ref="U202:U206" si="465">CONCATENATE("const CooGUI_tds* ",A202, ";")</f>
+        <f t="shared" ref="U202:U206" si="463">CONCATENATE("const CooGUI_tds* ",A202, ";")</f>
         <v>const CooGUI_tds* Pos_DepthDiveTime_DepthImperial;</v>
       </c>
       <c r="V202">
-        <f t="shared" ref="V202:V206" si="466">(G202*H202)/1024</f>
+        <f t="shared" ref="V202:V206" si="464">(G202*H202)/1024</f>
         <v>17.0703125</v>
       </c>
       <c r="W202" t="str">
-        <f t="shared" ref="W202:W206" si="467">CONCATENATE(A202, " = &amp;", B202,";")</f>
+        <f t="shared" ref="W202:W206" si="465">CONCATENATE(A202, " = &amp;", B202,";")</f>
         <v>Pos_DepthDiveTime_DepthImperial = &amp;Pos_DepthDiveTime_DepthImperial_Normal;</v>
       </c>
     </row>
@@ -22283,7 +22283,7 @@
         <v>286</v>
       </c>
       <c r="B203" t="str">
-        <f t="shared" ref="B203" si="468">CONCATENATE(A203, "_Normal")</f>
+        <f t="shared" ref="B203" si="466">CONCATENATE(A203, "_Normal")</f>
         <v>Pos_DepthDiveTime_DepthMetricDecimal_Normal</v>
       </c>
       <c r="C203" s="9">
@@ -22309,63 +22309,63 @@
         <v>76</v>
       </c>
       <c r="I203" s="26">
-        <f t="shared" ref="I203:I204" si="469">E203+G203</f>
+        <f t="shared" ref="I203:I204" si="467">E203+G203</f>
         <v>165</v>
       </c>
       <c r="J203" s="26">
-        <f t="shared" ref="J203:J204" si="470">F203+H203</f>
+        <f t="shared" ref="J203:J204" si="468">F203+H203</f>
         <v>104</v>
       </c>
       <c r="K203" t="str">
-        <f t="shared" ref="K203" si="471">CONCATENATE("static const CooGUI_tds ",A203, "_Normal = {", C203, ",", D203, ",", E203, ",", F203, ",",G203, ",", H203,",",  I203, ",", J203, "};")</f>
+        <f t="shared" ref="K203" si="469">CONCATENATE("static const CooGUI_tds ",A203, "_Normal = {", C203, ",", D203, ",", E203, ",", F203, ",",G203, ",", H203,",",  I203, ",", J203, "};")</f>
         <v>static const CooGUI_tds Pos_DepthDiveTime_DepthMetricDecimal_Normal = {165,10,25,28,140,76,165,104};</v>
       </c>
       <c r="L203">
-        <f t="shared" ref="L203" si="472">C203</f>
+        <f t="shared" ref="L203" si="470">C203</f>
         <v>165</v>
       </c>
       <c r="M203" s="52">
-        <f t="shared" ref="M203" si="473">D203 + $D$1</f>
+        <f t="shared" ref="M203" si="471">D203 + $D$1</f>
         <v>34</v>
       </c>
       <c r="N203">
-        <f t="shared" ref="N203" si="474">E203</f>
+        <f t="shared" ref="N203" si="472">E203</f>
         <v>25</v>
       </c>
       <c r="O203">
-        <f t="shared" ref="O203" si="475">F203</f>
+        <f t="shared" ref="O203" si="473">F203</f>
         <v>28</v>
       </c>
       <c r="P203">
-        <f t="shared" ref="P203" si="476">G203</f>
+        <f t="shared" ref="P203" si="474">G203</f>
         <v>140</v>
       </c>
       <c r="Q203">
-        <f t="shared" ref="Q203" si="477">H203</f>
+        <f t="shared" ref="Q203" si="475">H203</f>
         <v>76</v>
       </c>
       <c r="R203" s="20">
-        <f t="shared" ref="R203" si="478">N203+P203</f>
+        <f t="shared" ref="R203" si="476">N203+P203</f>
         <v>165</v>
       </c>
       <c r="S203" s="20">
-        <f t="shared" ref="S203" si="479">O203+Q203</f>
+        <f t="shared" ref="S203" si="477">O203+Q203</f>
         <v>104</v>
       </c>
       <c r="T203" t="str">
-        <f t="shared" ref="T203" si="480">CONCATENATE("static const CooGUI_tds ",A203, "_Flipped = {", L203, ",", M203, ",", N203, ",", O203, ",",P203, ",", Q203,",",  R203, ",", S203, "};")</f>
+        <f t="shared" ref="T203" si="478">CONCATENATE("static const CooGUI_tds ",A203, "_Flipped = {", L203, ",", M203, ",", N203, ",", O203, ",",P203, ",", Q203,",",  R203, ",", S203, "};")</f>
         <v>static const CooGUI_tds Pos_DepthDiveTime_DepthMetricDecimal_Flipped = {165,34,25,28,140,76,165,104};</v>
       </c>
       <c r="U203" t="str">
-        <f t="shared" ref="U203" si="481">CONCATENATE("const CooGUI_tds* ",A203, ";")</f>
+        <f t="shared" ref="U203" si="479">CONCATENATE("const CooGUI_tds* ",A203, ";")</f>
         <v>const CooGUI_tds* Pos_DepthDiveTime_DepthMetricDecimal;</v>
       </c>
       <c r="V203">
-        <f t="shared" ref="V203" si="482">(G203*H203)/1024</f>
+        <f t="shared" ref="V203" si="480">(G203*H203)/1024</f>
         <v>10.390625</v>
       </c>
       <c r="W203" t="str">
-        <f t="shared" ref="W203" si="483">CONCATENATE(A203, " = &amp;", B203,";")</f>
+        <f t="shared" ref="W203" si="481">CONCATENATE(A203, " = &amp;", B203,";")</f>
         <v>Pos_DepthDiveTime_DepthMetricDecimal = &amp;Pos_DepthDiveTime_DepthMetricDecimal_Normal;</v>
       </c>
     </row>
@@ -22374,7 +22374,7 @@
         <v>287</v>
       </c>
       <c r="B204" t="str">
-        <f t="shared" ref="B204" si="484">CONCATENATE(A204, "_Normal")</f>
+        <f t="shared" ref="B204" si="482">CONCATENATE(A204, "_Normal")</f>
         <v>Pos_DepthDiveTime_DepthMetricFloat_Normal</v>
       </c>
       <c r="C204" s="26">
@@ -22402,63 +22402,63 @@
         <v>76</v>
       </c>
       <c r="I204" s="26">
-        <f t="shared" si="469"/>
+        <f t="shared" si="467"/>
         <v>255</v>
       </c>
       <c r="J204" s="26">
-        <f t="shared" si="470"/>
+        <f t="shared" si="468"/>
         <v>104</v>
       </c>
       <c r="K204" t="str">
-        <f t="shared" ref="K204" si="485">CONCATENATE("static const CooGUI_tds ",A204, "_Normal = {", C204, ",", D204, ",", E204, ",", F204, ",",G204, ",", H204,",",  I204, ",", J204, "};")</f>
+        <f t="shared" ref="K204" si="483">CONCATENATE("static const CooGUI_tds ",A204, "_Normal = {", C204, ",", D204, ",", E204, ",", F204, ",",G204, ",", H204,",",  I204, ",", J204, "};")</f>
         <v>static const CooGUI_tds Pos_DepthDiveTime_DepthMetricFloat_Normal = {165,31,165,28,90,76,255,104};</v>
       </c>
       <c r="L204">
-        <f t="shared" ref="L204" si="486">C204</f>
+        <f t="shared" ref="L204" si="484">C204</f>
         <v>165</v>
       </c>
       <c r="M204" s="52">
-        <f t="shared" ref="M204" si="487">D204 + $D$1</f>
+        <f t="shared" ref="M204" si="485">D204 + $D$1</f>
         <v>55</v>
       </c>
       <c r="N204">
-        <f t="shared" ref="N204" si="488">E204</f>
+        <f t="shared" ref="N204" si="486">E204</f>
         <v>165</v>
       </c>
       <c r="O204">
-        <f t="shared" ref="O204" si="489">F204</f>
+        <f t="shared" ref="O204" si="487">F204</f>
         <v>28</v>
       </c>
       <c r="P204">
-        <f t="shared" ref="P204" si="490">G204</f>
+        <f t="shared" ref="P204" si="488">G204</f>
         <v>90</v>
       </c>
       <c r="Q204">
-        <f t="shared" ref="Q204" si="491">H204</f>
+        <f t="shared" ref="Q204" si="489">H204</f>
         <v>76</v>
       </c>
       <c r="R204" s="20">
-        <f t="shared" ref="R204" si="492">N204+P204</f>
+        <f t="shared" ref="R204" si="490">N204+P204</f>
         <v>255</v>
       </c>
       <c r="S204" s="20">
-        <f t="shared" ref="S204" si="493">O204+Q204</f>
+        <f t="shared" ref="S204" si="491">O204+Q204</f>
         <v>104</v>
       </c>
       <c r="T204" t="str">
-        <f t="shared" ref="T204" si="494">CONCATENATE("static const CooGUI_tds ",A204, "_Flipped = {", L204, ",", M204, ",", N204, ",", O204, ",",P204, ",", Q204,",",  R204, ",", S204, "};")</f>
+        <f t="shared" ref="T204" si="492">CONCATENATE("static const CooGUI_tds ",A204, "_Flipped = {", L204, ",", M204, ",", N204, ",", O204, ",",P204, ",", Q204,",",  R204, ",", S204, "};")</f>
         <v>static const CooGUI_tds Pos_DepthDiveTime_DepthMetricFloat_Flipped = {165,55,165,28,90,76,255,104};</v>
       </c>
       <c r="U204" t="str">
-        <f t="shared" ref="U204" si="495">CONCATENATE("const CooGUI_tds* ",A204, ";")</f>
+        <f t="shared" ref="U204" si="493">CONCATENATE("const CooGUI_tds* ",A204, ";")</f>
         <v>const CooGUI_tds* Pos_DepthDiveTime_DepthMetricFloat;</v>
       </c>
       <c r="V204">
-        <f t="shared" ref="V204" si="496">(G204*H204)/1024</f>
+        <f t="shared" ref="V204" si="494">(G204*H204)/1024</f>
         <v>6.6796875</v>
       </c>
       <c r="W204" t="str">
-        <f t="shared" ref="W204" si="497">CONCATENATE(A204, " = &amp;", B204,";")</f>
+        <f t="shared" ref="W204" si="495">CONCATENATE(A204, " = &amp;", B204,";")</f>
         <v>Pos_DepthDiveTime_DepthMetricFloat = &amp;Pos_DepthDiveTime_DepthMetricFloat_Normal;</v>
       </c>
     </row>
@@ -22467,7 +22467,7 @@
         <v>292</v>
       </c>
       <c r="B205" t="str">
-        <f t="shared" ref="B205" si="498">CONCATENATE(A205, "_Normal")</f>
+        <f t="shared" ref="B205" si="496">CONCATENATE(A205, "_Normal")</f>
         <v>Pos_DepthDiveTime_AlarmArrowOnRight_Normal</v>
       </c>
       <c r="C205" s="26">
@@ -22492,63 +22492,63 @@
         <v>60</v>
       </c>
       <c r="I205" s="26">
-        <f t="shared" ref="I205" si="499">E205+G205</f>
+        <f t="shared" ref="I205" si="497">E205+G205</f>
         <v>295</v>
       </c>
       <c r="J205" s="26">
-        <f t="shared" ref="J205" si="500">F205+H205</f>
+        <f t="shared" ref="J205" si="498">F205+H205</f>
         <v>60</v>
       </c>
       <c r="K205" t="str">
-        <f t="shared" ref="K205" si="501">CONCATENATE("static const CooGUI_tds ",A205, "_Normal = {", C205, ",", D205, ",", E205, ",", F205, ",",G205, ",", H205,",",  I205, ",", J205, "};")</f>
+        <f t="shared" ref="K205" si="499">CONCATENATE("static const CooGUI_tds ",A205, "_Normal = {", C205, ",", D205, ",", E205, ",", F205, ",",G205, ",", H205,",",  I205, ",", J205, "};")</f>
         <v>static const CooGUI_tds Pos_DepthDiveTime_AlarmArrowOnRight_Normal = {275,0,255,0,40,60,295,60};</v>
       </c>
       <c r="L205">
-        <f t="shared" ref="L205" si="502">C205</f>
+        <f t="shared" ref="L205" si="500">C205</f>
         <v>275</v>
       </c>
       <c r="M205" s="52">
-        <f t="shared" ref="M205" si="503">D205 + $D$1</f>
+        <f t="shared" ref="M205" si="501">D205 + $D$1</f>
         <v>24</v>
       </c>
       <c r="N205">
-        <f t="shared" ref="N205" si="504">E205</f>
+        <f t="shared" ref="N205" si="502">E205</f>
         <v>255</v>
       </c>
       <c r="O205">
-        <f t="shared" ref="O205" si="505">F205</f>
+        <f t="shared" ref="O205" si="503">F205</f>
         <v>0</v>
       </c>
       <c r="P205">
-        <f t="shared" ref="P205" si="506">G205</f>
+        <f t="shared" ref="P205" si="504">G205</f>
         <v>40</v>
       </c>
       <c r="Q205">
-        <f t="shared" ref="Q205" si="507">H205</f>
+        <f t="shared" ref="Q205" si="505">H205</f>
         <v>60</v>
       </c>
       <c r="R205" s="20">
-        <f t="shared" ref="R205" si="508">N205+P205</f>
+        <f t="shared" ref="R205" si="506">N205+P205</f>
         <v>295</v>
       </c>
       <c r="S205" s="20">
-        <f t="shared" ref="S205" si="509">O205+Q205</f>
+        <f t="shared" ref="S205" si="507">O205+Q205</f>
         <v>60</v>
       </c>
       <c r="T205" t="str">
-        <f t="shared" ref="T205" si="510">CONCATENATE("static const CooGUI_tds ",A205, "_Flipped = {", L205, ",", M205, ",", N205, ",", O205, ",",P205, ",", Q205,",",  R205, ",", S205, "};")</f>
+        <f t="shared" ref="T205" si="508">CONCATENATE("static const CooGUI_tds ",A205, "_Flipped = {", L205, ",", M205, ",", N205, ",", O205, ",",P205, ",", Q205,",",  R205, ",", S205, "};")</f>
         <v>static const CooGUI_tds Pos_DepthDiveTime_AlarmArrowOnRight_Flipped = {275,24,255,0,40,60,295,60};</v>
       </c>
       <c r="U205" t="str">
-        <f t="shared" ref="U205" si="511">CONCATENATE("const CooGUI_tds* ",A205, ";")</f>
+        <f t="shared" ref="U205" si="509">CONCATENATE("const CooGUI_tds* ",A205, ";")</f>
         <v>const CooGUI_tds* Pos_DepthDiveTime_AlarmArrowOnRight;</v>
       </c>
       <c r="V205">
-        <f t="shared" ref="V205" si="512">(G205*H205)/1024</f>
+        <f t="shared" ref="V205" si="510">(G205*H205)/1024</f>
         <v>2.34375</v>
       </c>
       <c r="W205" t="str">
-        <f t="shared" ref="W205" si="513">CONCATENATE(A205, " = &amp;", B205,";")</f>
+        <f t="shared" ref="W205" si="511">CONCATENATE(A205, " = &amp;", B205,";")</f>
         <v>Pos_DepthDiveTime_AlarmArrowOnRight = &amp;Pos_DepthDiveTime_AlarmArrowOnRight_Normal;</v>
       </c>
     </row>
@@ -22557,7 +22557,7 @@
         <v>283</v>
       </c>
       <c r="B206" s="99" t="str">
-        <f t="shared" si="452"/>
+        <f t="shared" si="450"/>
         <v>Pos_DepthDiveTime_CenterDiveTimeTittle_Normal</v>
       </c>
       <c r="C206" s="26">
@@ -22585,63 +22585,63 @@
         <v>28</v>
       </c>
       <c r="I206" s="26">
+        <f t="shared" si="451"/>
+        <v>295</v>
+      </c>
+      <c r="J206" s="26">
+        <f t="shared" si="452"/>
+        <v>132</v>
+      </c>
+      <c r="K206" t="str">
         <f t="shared" si="453"/>
+        <v>static const CooGUI_tds Pos_DepthDiveTime_CenterDiveTimeTittle_Normal = {160,104,25,104,270,28,295,132};</v>
+      </c>
+      <c r="L206">
+        <f t="shared" si="454"/>
+        <v>160</v>
+      </c>
+      <c r="M206" s="52">
+        <f t="shared" si="455"/>
+        <v>128</v>
+      </c>
+      <c r="N206">
+        <f t="shared" si="456"/>
+        <v>25</v>
+      </c>
+      <c r="O206">
+        <f t="shared" si="457"/>
+        <v>104</v>
+      </c>
+      <c r="P206">
+        <f t="shared" si="458"/>
+        <v>270</v>
+      </c>
+      <c r="Q206">
+        <f t="shared" si="459"/>
+        <v>28</v>
+      </c>
+      <c r="R206" s="20">
+        <f t="shared" si="460"/>
         <v>295</v>
       </c>
-      <c r="J206" s="26">
-        <f t="shared" si="454"/>
+      <c r="S206" s="20">
+        <f t="shared" si="461"/>
         <v>132</v>
       </c>
-      <c r="K206" t="str">
-        <f t="shared" si="455"/>
-        <v>static const CooGUI_tds Pos_DepthDiveTime_CenterDiveTimeTittle_Normal = {160,104,25,104,270,28,295,132};</v>
-      </c>
-      <c r="L206">
-        <f t="shared" si="456"/>
-        <v>160</v>
-      </c>
-      <c r="M206" s="52">
-        <f t="shared" si="457"/>
-        <v>128</v>
-      </c>
-      <c r="N206">
-        <f t="shared" si="458"/>
-        <v>25</v>
-      </c>
-      <c r="O206">
-        <f t="shared" si="459"/>
-        <v>104</v>
-      </c>
-      <c r="P206">
-        <f t="shared" si="460"/>
-        <v>270</v>
-      </c>
-      <c r="Q206">
-        <f t="shared" si="461"/>
-        <v>28</v>
-      </c>
-      <c r="R206" s="20">
+      <c r="T206" t="str">
         <f t="shared" si="462"/>
-        <v>295</v>
-      </c>
-      <c r="S206" s="20">
+        <v>static const CooGUI_tds Pos_DepthDiveTime_CenterDiveTimeTittle_Flipped = {160,128,25,104,270,28,295,132};</v>
+      </c>
+      <c r="U206" t="str">
         <f t="shared" si="463"/>
-        <v>132</v>
-      </c>
-      <c r="T206" t="str">
+        <v>const CooGUI_tds* Pos_DepthDiveTime_CenterDiveTimeTittle;</v>
+      </c>
+      <c r="V206">
         <f t="shared" si="464"/>
-        <v>static const CooGUI_tds Pos_DepthDiveTime_CenterDiveTimeTittle_Flipped = {160,128,25,104,270,28,295,132};</v>
-      </c>
-      <c r="U206" t="str">
+        <v>7.3828125</v>
+      </c>
+      <c r="W206" t="str">
         <f t="shared" si="465"/>
-        <v>const CooGUI_tds* Pos_DepthDiveTime_CenterDiveTimeTittle;</v>
-      </c>
-      <c r="V206">
-        <f t="shared" si="466"/>
-        <v>7.3828125</v>
-      </c>
-      <c r="W206" t="str">
-        <f t="shared" si="467"/>
         <v>Pos_DepthDiveTime_CenterDiveTimeTittle = &amp;Pos_DepthDiveTime_CenterDiveTimeTittle_Normal;</v>
       </c>
     </row>
@@ -22650,11 +22650,11 @@
         <v>284</v>
       </c>
       <c r="B207" s="99" t="str">
-        <f t="shared" ref="B207" si="514">CONCATENATE(A207, "_Normal")</f>
+        <f t="shared" ref="B207" si="512">CONCATENATE(A207, "_Normal")</f>
         <v>Pos_DepthDiveTime_CenterDiveTimeValue_Normal</v>
       </c>
       <c r="C207" s="26">
-        <f t="shared" ref="C207" si="515">C206</f>
+        <f t="shared" ref="C207" si="513">C206</f>
         <v>160</v>
       </c>
       <c r="D207" s="26">
@@ -22678,63 +22678,63 @@
         <v>76</v>
       </c>
       <c r="I207" s="26">
-        <f t="shared" ref="I207" si="516">E207+G207</f>
+        <f t="shared" ref="I207" si="514">E207+G207</f>
         <v>295</v>
       </c>
       <c r="J207" s="26">
-        <f t="shared" ref="J207" si="517">F207+H207</f>
+        <f t="shared" ref="J207" si="515">F207+H207</f>
         <v>208</v>
       </c>
       <c r="K207" t="str">
-        <f t="shared" ref="K207" si="518">CONCATENATE("static const CooGUI_tds ",A207, "_Normal = {", C207, ",", D207, ",", E207, ",", F207, ",",G207, ",", H207,",",  I207, ",", J207, "};")</f>
+        <f t="shared" ref="K207" si="516">CONCATENATE("static const CooGUI_tds ",A207, "_Normal = {", C207, ",", D207, ",", E207, ",", F207, ",",G207, ",", H207,",",  I207, ",", J207, "};")</f>
         <v>static const CooGUI_tds Pos_DepthDiveTime_CenterDiveTimeValue_Normal = {160,114,25,132,270,76,295,208};</v>
       </c>
       <c r="L207">
-        <f t="shared" ref="L207" si="519">C207</f>
+        <f t="shared" ref="L207" si="517">C207</f>
         <v>160</v>
       </c>
       <c r="M207" s="52">
-        <f t="shared" ref="M207" si="520">D207 + $D$1</f>
+        <f t="shared" ref="M207" si="518">D207 + $D$1</f>
         <v>138</v>
       </c>
       <c r="N207">
-        <f t="shared" ref="N207" si="521">E207</f>
+        <f t="shared" ref="N207" si="519">E207</f>
         <v>25</v>
       </c>
       <c r="O207">
-        <f t="shared" ref="O207" si="522">F207</f>
+        <f t="shared" ref="O207" si="520">F207</f>
         <v>132</v>
       </c>
       <c r="P207">
-        <f t="shared" ref="P207" si="523">G207</f>
+        <f t="shared" ref="P207" si="521">G207</f>
         <v>270</v>
       </c>
       <c r="Q207">
-        <f t="shared" ref="Q207" si="524">H207</f>
+        <f t="shared" ref="Q207" si="522">H207</f>
         <v>76</v>
       </c>
       <c r="R207" s="20">
-        <f t="shared" ref="R207" si="525">N207+P207</f>
+        <f t="shared" ref="R207" si="523">N207+P207</f>
         <v>295</v>
       </c>
       <c r="S207" s="20">
-        <f t="shared" ref="S207" si="526">O207+Q207</f>
+        <f t="shared" ref="S207" si="524">O207+Q207</f>
         <v>208</v>
       </c>
       <c r="T207" t="str">
-        <f t="shared" ref="T207" si="527">CONCATENATE("static const CooGUI_tds ",A207, "_Flipped = {", L207, ",", M207, ",", N207, ",", O207, ",",P207, ",", Q207,",",  R207, ",", S207, "};")</f>
+        <f t="shared" ref="T207" si="525">CONCATENATE("static const CooGUI_tds ",A207, "_Flipped = {", L207, ",", M207, ",", N207, ",", O207, ",",P207, ",", Q207,",",  R207, ",", S207, "};")</f>
         <v>static const CooGUI_tds Pos_DepthDiveTime_CenterDiveTimeValue_Flipped = {160,138,25,132,270,76,295,208};</v>
       </c>
       <c r="U207" t="str">
-        <f t="shared" ref="U207" si="528">CONCATENATE("const CooGUI_tds* ",A207, ";")</f>
+        <f t="shared" ref="U207" si="526">CONCATENATE("const CooGUI_tds* ",A207, ";")</f>
         <v>const CooGUI_tds* Pos_DepthDiveTime_CenterDiveTimeValue;</v>
       </c>
       <c r="V207">
-        <f t="shared" ref="V207" si="529">(G207*H207)/1024</f>
+        <f t="shared" ref="V207" si="527">(G207*H207)/1024</f>
         <v>20.0390625</v>
       </c>
       <c r="W207" t="str">
-        <f t="shared" ref="W207" si="530">CONCATENATE(A207, " = &amp;", B207,";")</f>
+        <f t="shared" ref="W207" si="528">CONCATENATE(A207, " = &amp;", B207,";")</f>
         <v>Pos_DepthDiveTime_CenterDiveTimeValue = &amp;Pos_DepthDiveTime_CenterDiveTimeValue_Normal;</v>
       </c>
     </row>
@@ -22743,7 +22743,7 @@
         <v>288</v>
       </c>
       <c r="B208" s="98" t="str">
-        <f t="shared" ref="B208" si="531">CONCATENATE(A208, "_Normal")</f>
+        <f t="shared" ref="B208" si="529">CONCATENATE(A208, "_Normal")</f>
         <v>Pos_DepthDiveTime_DiveTimeLeftTittle_Normal</v>
       </c>
       <c r="C208" s="26">
@@ -22770,63 +22770,63 @@
         <v>28</v>
       </c>
       <c r="I208" s="26">
-        <f t="shared" ref="I208" si="532">E208+G208</f>
+        <f t="shared" ref="I208" si="530">E208+G208</f>
         <v>160</v>
       </c>
       <c r="J208" s="26">
-        <f t="shared" ref="J208" si="533">F208+H208</f>
+        <f t="shared" ref="J208" si="531">F208+H208</f>
         <v>132</v>
       </c>
       <c r="K208" t="str">
-        <f t="shared" ref="K208" si="534">CONCATENATE("static const CooGUI_tds ",A208, "_Normal = {", C208, ",", D208, ",", E208, ",", F208, ",",G208, ",", H208,",",  I208, ",", J208, "};")</f>
+        <f t="shared" ref="K208" si="532">CONCATENATE("static const CooGUI_tds ",A208, "_Normal = {", C208, ",", D208, ",", E208, ",", F208, ",",G208, ",", H208,",",  I208, ",", J208, "};")</f>
         <v>static const CooGUI_tds Pos_DepthDiveTime_DiveTimeLeftTittle_Normal = {93,104,25,104,135,28,160,132};</v>
       </c>
       <c r="L208">
-        <f t="shared" ref="L208" si="535">C208</f>
+        <f t="shared" ref="L208" si="533">C208</f>
         <v>93</v>
       </c>
       <c r="M208" s="52">
-        <f t="shared" ref="M208" si="536">D208 + $D$1</f>
+        <f t="shared" ref="M208" si="534">D208 + $D$1</f>
         <v>128</v>
       </c>
       <c r="N208">
-        <f t="shared" ref="N208" si="537">E208</f>
+        <f t="shared" ref="N208" si="535">E208</f>
         <v>25</v>
       </c>
       <c r="O208">
-        <f t="shared" ref="O208" si="538">F208</f>
+        <f t="shared" ref="O208" si="536">F208</f>
         <v>104</v>
       </c>
       <c r="P208">
-        <f t="shared" ref="P208" si="539">G208</f>
+        <f t="shared" ref="P208" si="537">G208</f>
         <v>135</v>
       </c>
       <c r="Q208">
-        <f t="shared" ref="Q208" si="540">H208</f>
+        <f t="shared" ref="Q208" si="538">H208</f>
         <v>28</v>
       </c>
       <c r="R208" s="20">
-        <f t="shared" ref="R208" si="541">N208+P208</f>
+        <f t="shared" ref="R208" si="539">N208+P208</f>
         <v>160</v>
       </c>
       <c r="S208" s="20">
-        <f t="shared" ref="S208" si="542">O208+Q208</f>
+        <f t="shared" ref="S208" si="540">O208+Q208</f>
         <v>132</v>
       </c>
       <c r="T208" t="str">
-        <f t="shared" ref="T208" si="543">CONCATENATE("static const CooGUI_tds ",A208, "_Flipped = {", L208, ",", M208, ",", N208, ",", O208, ",",P208, ",", Q208,",",  R208, ",", S208, "};")</f>
+        <f t="shared" ref="T208" si="541">CONCATENATE("static const CooGUI_tds ",A208, "_Flipped = {", L208, ",", M208, ",", N208, ",", O208, ",",P208, ",", Q208,",",  R208, ",", S208, "};")</f>
         <v>static const CooGUI_tds Pos_DepthDiveTime_DiveTimeLeftTittle_Flipped = {93,128,25,104,135,28,160,132};</v>
       </c>
       <c r="U208" t="str">
-        <f t="shared" ref="U208" si="544">CONCATENATE("const CooGUI_tds* ",A208, ";")</f>
+        <f t="shared" ref="U208" si="542">CONCATENATE("const CooGUI_tds* ",A208, ";")</f>
         <v>const CooGUI_tds* Pos_DepthDiveTime_DiveTimeLeftTittle;</v>
       </c>
       <c r="V208">
-        <f t="shared" ref="V208" si="545">(G208*H208)/1024</f>
+        <f t="shared" ref="V208" si="543">(G208*H208)/1024</f>
         <v>3.69140625</v>
       </c>
       <c r="W208" t="str">
-        <f t="shared" ref="W208" si="546">CONCATENATE(A208, " = &amp;", B208,";")</f>
+        <f t="shared" ref="W208" si="544">CONCATENATE(A208, " = &amp;", B208,";")</f>
         <v>Pos_DepthDiveTime_DiveTimeLeftTittle = &amp;Pos_DepthDiveTime_DiveTimeLeftTittle_Normal;</v>
       </c>
     </row>
@@ -22835,7 +22835,7 @@
         <v>289</v>
       </c>
       <c r="B209" s="98" t="str">
-        <f t="shared" ref="B209" si="547">CONCATENATE(A209, "_Normal")</f>
+        <f t="shared" ref="B209" si="545">CONCATENATE(A209, "_Normal")</f>
         <v>Pos_DepthDiveTime_DiveTimeLeftValue_Normal</v>
       </c>
       <c r="C209" s="26">
@@ -22863,63 +22863,63 @@
         <v>76</v>
       </c>
       <c r="I209" s="26">
-        <f t="shared" ref="I209" si="548">E209+G209</f>
+        <f t="shared" ref="I209" si="546">E209+G209</f>
         <v>160</v>
       </c>
       <c r="J209" s="26">
-        <f t="shared" ref="J209" si="549">F209+H209</f>
+        <f t="shared" ref="J209" si="547">F209+H209</f>
         <v>208</v>
       </c>
       <c r="K209" t="str">
-        <f t="shared" ref="K209" si="550">CONCATENATE("static const CooGUI_tds ",A209, "_Normal = {", C209, ",", D209, ",", E209, ",", F209, ",",G209, ",", H209,",",  I209, ",", J209, "};")</f>
+        <f t="shared" ref="K209" si="548">CONCATENATE("static const CooGUI_tds ",A209, "_Normal = {", C209, ",", D209, ",", E209, ",", F209, ",",G209, ",", H209,",",  I209, ",", J209, "};")</f>
         <v>static const CooGUI_tds Pos_DepthDiveTime_DiveTimeLeftValue_Normal = {93,114,25,132,135,76,160,208};</v>
       </c>
       <c r="L209">
-        <f t="shared" ref="L209" si="551">C209</f>
+        <f t="shared" ref="L209" si="549">C209</f>
         <v>93</v>
       </c>
       <c r="M209" s="52">
-        <f t="shared" ref="M209" si="552">D209 + $D$1</f>
+        <f t="shared" ref="M209" si="550">D209 + $D$1</f>
         <v>138</v>
       </c>
       <c r="N209">
-        <f t="shared" ref="N209" si="553">E209</f>
+        <f t="shared" ref="N209" si="551">E209</f>
         <v>25</v>
       </c>
       <c r="O209">
-        <f t="shared" ref="O209" si="554">F209</f>
+        <f t="shared" ref="O209" si="552">F209</f>
         <v>132</v>
       </c>
       <c r="P209">
-        <f t="shared" ref="P209" si="555">G209</f>
+        <f t="shared" ref="P209" si="553">G209</f>
         <v>135</v>
       </c>
       <c r="Q209">
-        <f t="shared" ref="Q209" si="556">H209</f>
+        <f t="shared" ref="Q209" si="554">H209</f>
         <v>76</v>
       </c>
       <c r="R209" s="20">
-        <f t="shared" ref="R209" si="557">N209+P209</f>
+        <f t="shared" ref="R209" si="555">N209+P209</f>
         <v>160</v>
       </c>
       <c r="S209" s="20">
-        <f t="shared" ref="S209" si="558">O209+Q209</f>
+        <f t="shared" ref="S209" si="556">O209+Q209</f>
         <v>208</v>
       </c>
       <c r="T209" t="str">
-        <f t="shared" ref="T209" si="559">CONCATENATE("static const CooGUI_tds ",A209, "_Flipped = {", L209, ",", M209, ",", N209, ",", O209, ",",P209, ",", Q209,",",  R209, ",", S209, "};")</f>
+        <f t="shared" ref="T209" si="557">CONCATENATE("static const CooGUI_tds ",A209, "_Flipped = {", L209, ",", M209, ",", N209, ",", O209, ",",P209, ",", Q209,",",  R209, ",", S209, "};")</f>
         <v>static const CooGUI_tds Pos_DepthDiveTime_DiveTimeLeftValue_Flipped = {93,138,25,132,135,76,160,208};</v>
       </c>
       <c r="U209" t="str">
-        <f t="shared" ref="U209" si="560">CONCATENATE("const CooGUI_tds* ",A209, ";")</f>
+        <f t="shared" ref="U209" si="558">CONCATENATE("const CooGUI_tds* ",A209, ";")</f>
         <v>const CooGUI_tds* Pos_DepthDiveTime_DiveTimeLeftValue;</v>
       </c>
       <c r="V209">
-        <f t="shared" ref="V209" si="561">(G209*H209)/1024</f>
+        <f t="shared" ref="V209" si="559">(G209*H209)/1024</f>
         <v>10.01953125</v>
       </c>
       <c r="W209" t="str">
-        <f t="shared" ref="W209" si="562">CONCATENATE(A209, " = &amp;", B209,";")</f>
+        <f t="shared" ref="W209" si="560">CONCATENATE(A209, " = &amp;", B209,";")</f>
         <v>Pos_DepthDiveTime_DiveTimeLeftValue = &amp;Pos_DepthDiveTime_DiveTimeLeftValue_Normal;</v>
       </c>
     </row>
@@ -22928,7 +22928,7 @@
         <v>290</v>
       </c>
       <c r="B210" s="98" t="str">
-        <f t="shared" ref="B210" si="563">CONCATENATE(A210, "_Normal")</f>
+        <f t="shared" ref="B210" si="561">CONCATENATE(A210, "_Normal")</f>
         <v>Pos_DepthDiveTime_TankPressRightTittle_Normal</v>
       </c>
       <c r="C210" s="26">
@@ -22956,63 +22956,63 @@
         <v>28</v>
       </c>
       <c r="I210" s="26">
-        <f t="shared" ref="I210" si="564">E210+G210</f>
+        <f t="shared" ref="I210" si="562">E210+G210</f>
         <v>293</v>
       </c>
       <c r="J210" s="26">
-        <f t="shared" ref="J210" si="565">F210+H210</f>
+        <f t="shared" ref="J210" si="563">F210+H210</f>
         <v>132</v>
       </c>
       <c r="K210" t="str">
-        <f t="shared" ref="K210" si="566">CONCATENATE("static const CooGUI_tds ",A210, "_Normal = {", C210, ",", D210, ",", E210, ",", F210, ",",G210, ",", H210,",",  I210, ",", J210, "};")</f>
+        <f t="shared" ref="K210" si="564">CONCATENATE("static const CooGUI_tds ",A210, "_Normal = {", C210, ",", D210, ",", E210, ",", F210, ",",G210, ",", H210,",",  I210, ",", J210, "};")</f>
         <v>static const CooGUI_tds Pos_DepthDiveTime_TankPressRightTittle_Normal = {227,104,160,104,133,28,293,132};</v>
       </c>
       <c r="L210">
-        <f t="shared" ref="L210" si="567">C210</f>
+        <f t="shared" ref="L210" si="565">C210</f>
         <v>227</v>
       </c>
       <c r="M210" s="52">
-        <f t="shared" ref="M210" si="568">D210 + $D$1</f>
+        <f t="shared" ref="M210" si="566">D210 + $D$1</f>
         <v>128</v>
       </c>
       <c r="N210">
-        <f t="shared" ref="N210" si="569">E210</f>
+        <f t="shared" ref="N210" si="567">E210</f>
         <v>160</v>
       </c>
       <c r="O210">
-        <f t="shared" ref="O210" si="570">F210</f>
+        <f t="shared" ref="O210" si="568">F210</f>
         <v>104</v>
       </c>
       <c r="P210">
-        <f t="shared" ref="P210" si="571">G210</f>
+        <f t="shared" ref="P210" si="569">G210</f>
         <v>133</v>
       </c>
       <c r="Q210">
-        <f t="shared" ref="Q210" si="572">H210</f>
+        <f t="shared" ref="Q210" si="570">H210</f>
         <v>28</v>
       </c>
       <c r="R210" s="20">
-        <f t="shared" ref="R210" si="573">N210+P210</f>
+        <f t="shared" ref="R210" si="571">N210+P210</f>
         <v>293</v>
       </c>
       <c r="S210" s="20">
-        <f t="shared" ref="S210" si="574">O210+Q210</f>
+        <f t="shared" ref="S210" si="572">O210+Q210</f>
         <v>132</v>
       </c>
       <c r="T210" t="str">
-        <f t="shared" ref="T210" si="575">CONCATENATE("static const CooGUI_tds ",A210, "_Flipped = {", L210, ",", M210, ",", N210, ",", O210, ",",P210, ",", Q210,",",  R210, ",", S210, "};")</f>
+        <f t="shared" ref="T210" si="573">CONCATENATE("static const CooGUI_tds ",A210, "_Flipped = {", L210, ",", M210, ",", N210, ",", O210, ",",P210, ",", Q210,",",  R210, ",", S210, "};")</f>
         <v>static const CooGUI_tds Pos_DepthDiveTime_TankPressRightTittle_Flipped = {227,128,160,104,133,28,293,132};</v>
       </c>
       <c r="U210" t="str">
-        <f t="shared" ref="U210" si="576">CONCATENATE("const CooGUI_tds* ",A210, ";")</f>
+        <f t="shared" ref="U210" si="574">CONCATENATE("const CooGUI_tds* ",A210, ";")</f>
         <v>const CooGUI_tds* Pos_DepthDiveTime_TankPressRightTittle;</v>
       </c>
       <c r="V210">
-        <f t="shared" ref="V210" si="577">(G210*H210)/1024</f>
+        <f t="shared" ref="V210" si="575">(G210*H210)/1024</f>
         <v>3.63671875</v>
       </c>
       <c r="W210" t="str">
-        <f t="shared" ref="W210" si="578">CONCATENATE(A210, " = &amp;", B210,";")</f>
+        <f t="shared" ref="W210" si="576">CONCATENATE(A210, " = &amp;", B210,";")</f>
         <v>Pos_DepthDiveTime_TankPressRightTittle = &amp;Pos_DepthDiveTime_TankPressRightTittle_Normal;</v>
       </c>
     </row>
@@ -23021,7 +23021,7 @@
         <v>291</v>
       </c>
       <c r="B211" s="98" t="str">
-        <f t="shared" ref="B211" si="579">CONCATENATE(A211, "_Normal")</f>
+        <f t="shared" ref="B211" si="577">CONCATENATE(A211, "_Normal")</f>
         <v>Pos_DepthDiveTime_TankPressRightValue_Normal</v>
       </c>
       <c r="C211" s="26">
@@ -23049,63 +23049,63 @@
         <v>76</v>
       </c>
       <c r="I211" s="26">
-        <f t="shared" ref="I211" si="580">E211+G211</f>
+        <f t="shared" ref="I211" si="578">E211+G211</f>
         <v>293</v>
       </c>
       <c r="J211" s="26">
-        <f t="shared" ref="J211" si="581">F211+H211</f>
+        <f t="shared" ref="J211" si="579">F211+H211</f>
         <v>208</v>
       </c>
       <c r="K211" t="str">
-        <f t="shared" ref="K211" si="582">CONCATENATE("static const CooGUI_tds ",A211, "_Normal = {", C211, ",", D211, ",", E211, ",", F211, ",",G211, ",", H211,",",  I211, ",", J211, "};")</f>
+        <f t="shared" ref="K211" si="580">CONCATENATE("static const CooGUI_tds ",A211, "_Normal = {", C211, ",", D211, ",", E211, ",", F211, ",",G211, ",", H211,",",  I211, ",", J211, "};")</f>
         <v>static const CooGUI_tds Pos_DepthDiveTime_TankPressRightValue_Normal = {227,114,160,132,133,76,293,208};</v>
       </c>
       <c r="L211">
-        <f t="shared" ref="L211" si="583">C211</f>
+        <f t="shared" ref="L211" si="581">C211</f>
         <v>227</v>
       </c>
       <c r="M211" s="52">
-        <f t="shared" ref="M211" si="584">D211 + $D$1</f>
+        <f t="shared" ref="M211" si="582">D211 + $D$1</f>
         <v>138</v>
       </c>
       <c r="N211">
-        <f t="shared" ref="N211" si="585">E211</f>
+        <f t="shared" ref="N211" si="583">E211</f>
         <v>160</v>
       </c>
       <c r="O211">
-        <f t="shared" ref="O211" si="586">F211</f>
+        <f t="shared" ref="O211" si="584">F211</f>
         <v>132</v>
       </c>
       <c r="P211">
-        <f t="shared" ref="P211" si="587">G211</f>
+        <f t="shared" ref="P211" si="585">G211</f>
         <v>133</v>
       </c>
       <c r="Q211">
-        <f t="shared" ref="Q211" si="588">H211</f>
+        <f t="shared" ref="Q211" si="586">H211</f>
         <v>76</v>
       </c>
       <c r="R211" s="20">
-        <f t="shared" ref="R211" si="589">N211+P211</f>
+        <f t="shared" ref="R211" si="587">N211+P211</f>
         <v>293</v>
       </c>
       <c r="S211" s="20">
-        <f t="shared" ref="S211" si="590">O211+Q211</f>
+        <f t="shared" ref="S211" si="588">O211+Q211</f>
         <v>208</v>
       </c>
       <c r="T211" t="str">
-        <f t="shared" ref="T211" si="591">CONCATENATE("static const CooGUI_tds ",A211, "_Flipped = {", L211, ",", M211, ",", N211, ",", O211, ",",P211, ",", Q211,",",  R211, ",", S211, "};")</f>
+        <f t="shared" ref="T211" si="589">CONCATENATE("static const CooGUI_tds ",A211, "_Flipped = {", L211, ",", M211, ",", N211, ",", O211, ",",P211, ",", Q211,",",  R211, ",", S211, "};")</f>
         <v>static const CooGUI_tds Pos_DepthDiveTime_TankPressRightValue_Flipped = {227,138,160,132,133,76,293,208};</v>
       </c>
       <c r="U211" t="str">
-        <f t="shared" ref="U211" si="592">CONCATENATE("const CooGUI_tds* ",A211, ";")</f>
+        <f t="shared" ref="U211" si="590">CONCATENATE("const CooGUI_tds* ",A211, ";")</f>
         <v>const CooGUI_tds* Pos_DepthDiveTime_TankPressRightValue;</v>
       </c>
       <c r="V211">
-        <f t="shared" ref="V211" si="593">(G211*H211)/1024</f>
+        <f t="shared" ref="V211" si="591">(G211*H211)/1024</f>
         <v>9.87109375</v>
       </c>
       <c r="W211" t="str">
-        <f t="shared" ref="W211" si="594">CONCATENATE(A211, " = &amp;", B211,";")</f>
+        <f t="shared" ref="W211" si="592">CONCATENATE(A211, " = &amp;", B211,";")</f>
         <v>Pos_DepthDiveTime_TankPressRightValue = &amp;Pos_DepthDiveTime_TankPressRightValue_Normal;</v>
       </c>
     </row>
@@ -23114,7 +23114,7 @@
         <v>285</v>
       </c>
       <c r="B212" t="str">
-        <f t="shared" ref="B212" si="595">CONCATENATE(A212, "_Normal")</f>
+        <f t="shared" ref="B212" si="593">CONCATENATE(A212, "_Normal")</f>
         <v>Pos_DepthDiveTime_AlarmInBottom_Normal</v>
       </c>
       <c r="C212" s="26">
@@ -23142,63 +23142,63 @@
         <v>32</v>
       </c>
       <c r="I212" s="26">
-        <f t="shared" ref="I212" si="596">E212+G212</f>
+        <f t="shared" ref="I212" si="594">E212+G212</f>
         <v>295</v>
       </c>
       <c r="J212" s="26">
-        <f t="shared" ref="J212" si="597">F212+H212</f>
+        <f t="shared" ref="J212" si="595">F212+H212</f>
         <v>240</v>
       </c>
       <c r="K212" t="str">
-        <f t="shared" ref="K212" si="598">CONCATENATE("static const CooGUI_tds ",A212, "_Normal = {", C212, ",", D212, ",", E212, ",", F212, ",",G212, ",", H212,",",  I212, ",", J212, "};")</f>
+        <f t="shared" ref="K212" si="596">CONCATENATE("static const CooGUI_tds ",A212, "_Normal = {", C212, ",", D212, ",", E212, ",", F212, ",",G212, ",", H212,",",  I212, ",", J212, "};")</f>
         <v>static const CooGUI_tds Pos_DepthDiveTime_AlarmInBottom_Normal = {160,208,25,208,270,32,295,240};</v>
       </c>
       <c r="L212">
-        <f t="shared" ref="L212" si="599">C212</f>
+        <f t="shared" ref="L212" si="597">C212</f>
         <v>160</v>
       </c>
       <c r="M212" s="52">
-        <f t="shared" ref="M212" si="600">D212 + $D$1</f>
+        <f t="shared" ref="M212" si="598">D212 + $D$1</f>
         <v>232</v>
       </c>
       <c r="N212">
-        <f t="shared" ref="N212" si="601">E212</f>
+        <f t="shared" ref="N212" si="599">E212</f>
         <v>25</v>
       </c>
       <c r="O212">
-        <f t="shared" ref="O212" si="602">F212</f>
+        <f t="shared" ref="O212" si="600">F212</f>
         <v>208</v>
       </c>
       <c r="P212">
-        <f t="shared" ref="P212" si="603">G212</f>
+        <f t="shared" ref="P212" si="601">G212</f>
         <v>270</v>
       </c>
       <c r="Q212">
-        <f t="shared" ref="Q212" si="604">H212</f>
+        <f t="shared" ref="Q212" si="602">H212</f>
         <v>32</v>
       </c>
       <c r="R212" s="20">
-        <f t="shared" ref="R212" si="605">N212+P212</f>
+        <f t="shared" ref="R212" si="603">N212+P212</f>
         <v>295</v>
       </c>
       <c r="S212" s="20">
-        <f t="shared" ref="S212" si="606">O212+Q212</f>
+        <f t="shared" ref="S212" si="604">O212+Q212</f>
         <v>240</v>
       </c>
       <c r="T212" t="str">
-        <f t="shared" ref="T212" si="607">CONCATENATE("static const CooGUI_tds ",A212, "_Flipped = {", L212, ",", M212, ",", N212, ",", O212, ",",P212, ",", Q212,",",  R212, ",", S212, "};")</f>
+        <f t="shared" ref="T212" si="605">CONCATENATE("static const CooGUI_tds ",A212, "_Flipped = {", L212, ",", M212, ",", N212, ",", O212, ",",P212, ",", Q212,",",  R212, ",", S212, "};")</f>
         <v>static const CooGUI_tds Pos_DepthDiveTime_AlarmInBottom_Flipped = {160,232,25,208,270,32,295,240};</v>
       </c>
       <c r="U212" t="str">
-        <f t="shared" ref="U212" si="608">CONCATENATE("const CooGUI_tds* ",A212, ";")</f>
+        <f t="shared" ref="U212" si="606">CONCATENATE("const CooGUI_tds* ",A212, ";")</f>
         <v>const CooGUI_tds* Pos_DepthDiveTime_AlarmInBottom;</v>
       </c>
       <c r="V212">
-        <f t="shared" ref="V212" si="609">(G212*H212)/1024</f>
+        <f t="shared" ref="V212" si="607">(G212*H212)/1024</f>
         <v>8.4375</v>
       </c>
       <c r="W212" t="str">
-        <f t="shared" ref="W212" si="610">CONCATENATE(A212, " = &amp;", B212,";")</f>
+        <f t="shared" ref="W212" si="608">CONCATENATE(A212, " = &amp;", B212,";")</f>
         <v>Pos_DepthDiveTime_AlarmInBottom = &amp;Pos_DepthDiveTime_AlarmInBottom_Normal;</v>
       </c>
     </row>
@@ -23207,7 +23207,7 @@
         <v>293</v>
       </c>
       <c r="B213" t="str">
-        <f t="shared" ref="B213:B214" si="611">CONCATENATE(A213, "_Normal")</f>
+        <f t="shared" ref="B213:B214" si="609">CONCATENATE(A213, "_Normal")</f>
         <v>Pos_GasSwitch_BottomLine_1_Normal</v>
       </c>
       <c r="C213" s="26">
@@ -23231,63 +23231,63 @@
         <v>30</v>
       </c>
       <c r="I213" s="26">
-        <f t="shared" ref="I213:I214" si="612">E213+G213</f>
+        <f t="shared" ref="I213:I214" si="610">E213+G213</f>
         <v>320</v>
       </c>
       <c r="J213" s="26">
-        <f t="shared" ref="J213:J214" si="613">F213+H213</f>
+        <f t="shared" ref="J213:J214" si="611">F213+H213</f>
         <v>215</v>
       </c>
       <c r="K213" t="str">
-        <f t="shared" ref="K213:K214" si="614">CONCATENATE("static const CooGUI_tds ",A213, "_Normal = {", C213, ",", D213, ",", E213, ",", F213, ",",G213, ",", H213,",",  I213, ",", J213, "};")</f>
+        <f t="shared" ref="K213:K214" si="612">CONCATENATE("static const CooGUI_tds ",A213, "_Normal = {", C213, ",", D213, ",", E213, ",", F213, ",",G213, ",", H213,",",  I213, ",", J213, "};")</f>
         <v>static const CooGUI_tds Pos_GasSwitch_BottomLine_1_Normal = {160,185,0,185,320,30,320,215};</v>
       </c>
       <c r="L213">
-        <f t="shared" ref="L213:L214" si="615">C213</f>
+        <f t="shared" ref="L213:L214" si="613">C213</f>
         <v>160</v>
       </c>
       <c r="M213" s="52">
-        <f t="shared" ref="M213:M214" si="616">D213 + $D$1</f>
+        <f>D213 + $D$1</f>
         <v>209</v>
       </c>
       <c r="N213">
-        <f t="shared" ref="N213:N214" si="617">E213</f>
+        <f t="shared" ref="N213:N214" si="614">E213</f>
         <v>0</v>
       </c>
       <c r="O213">
-        <f t="shared" ref="O213:O214" si="618">F213</f>
+        <f t="shared" ref="O213:O214" si="615">F213</f>
         <v>185</v>
       </c>
       <c r="P213">
-        <f t="shared" ref="P213:P214" si="619">G213</f>
+        <f t="shared" ref="P213:P214" si="616">G213</f>
         <v>320</v>
       </c>
       <c r="Q213">
-        <f t="shared" ref="Q213:Q214" si="620">H213</f>
+        <f t="shared" ref="Q213:Q214" si="617">H213</f>
         <v>30</v>
       </c>
       <c r="R213" s="20">
-        <f t="shared" ref="R213:R214" si="621">N213+P213</f>
+        <f t="shared" ref="R213:R214" si="618">N213+P213</f>
         <v>320</v>
       </c>
       <c r="S213" s="20">
-        <f t="shared" ref="S213:S214" si="622">O213+Q213</f>
+        <f t="shared" ref="S213:S214" si="619">O213+Q213</f>
         <v>215</v>
       </c>
       <c r="T213" t="str">
-        <f t="shared" ref="T213:T214" si="623">CONCATENATE("static const CooGUI_tds ",A213, "_Flipped = {", L213, ",", M213, ",", N213, ",", O213, ",",P213, ",", Q213,",",  R213, ",", S213, "};")</f>
+        <f t="shared" ref="T213:T214" si="620">CONCATENATE("static const CooGUI_tds ",A213, "_Flipped = {", L213, ",", M213, ",", N213, ",", O213, ",",P213, ",", Q213,",",  R213, ",", S213, "};")</f>
         <v>static const CooGUI_tds Pos_GasSwitch_BottomLine_1_Flipped = {160,209,0,185,320,30,320,215};</v>
       </c>
       <c r="U213" t="str">
-        <f t="shared" ref="U213:U214" si="624">CONCATENATE("const CooGUI_tds* ",A213, ";")</f>
+        <f t="shared" ref="U213:U214" si="621">CONCATENATE("const CooGUI_tds* ",A213, ";")</f>
         <v>const CooGUI_tds* Pos_GasSwitch_BottomLine_1;</v>
       </c>
       <c r="V213">
-        <f t="shared" ref="V213:V214" si="625">(G213*H213)/1024</f>
+        <f t="shared" ref="V213:V214" si="622">(G213*H213)/1024</f>
         <v>9.375</v>
       </c>
       <c r="W213" t="str">
-        <f t="shared" ref="W213:W214" si="626">CONCATENATE(A213, " = &amp;", B213,";")</f>
+        <f t="shared" ref="W213:W214" si="623">CONCATENATE(A213, " = &amp;", B213,";")</f>
         <v>Pos_GasSwitch_BottomLine_1 = &amp;Pos_GasSwitch_BottomLine_1_Normal;</v>
       </c>
     </row>
@@ -23296,7 +23296,7 @@
         <v>294</v>
       </c>
       <c r="B214" t="str">
-        <f t="shared" si="611"/>
+        <f t="shared" si="609"/>
         <v>Pos_GasSwitch_BottomLine_2_Normal</v>
       </c>
       <c r="C214" s="26">
@@ -23322,63 +23322,63 @@
         <v>30</v>
       </c>
       <c r="I214" s="26">
+        <f t="shared" si="610"/>
+        <v>252</v>
+      </c>
+      <c r="J214" s="26">
+        <f t="shared" si="611"/>
+        <v>245</v>
+      </c>
+      <c r="K214" t="str">
         <f t="shared" si="612"/>
+        <v>static const CooGUI_tds Pos_GasSwitch_BottomLine_2_Normal = {160,210,32,215,220,30,252,245};</v>
+      </c>
+      <c r="L214">
+        <f t="shared" si="613"/>
+        <v>160</v>
+      </c>
+      <c r="M214" s="52">
+        <f t="shared" ref="M213:M218" si="624">D214 + $D$1</f>
+        <v>234</v>
+      </c>
+      <c r="N214">
+        <f t="shared" si="614"/>
+        <v>32</v>
+      </c>
+      <c r="O214">
+        <f t="shared" si="615"/>
+        <v>215</v>
+      </c>
+      <c r="P214">
+        <f t="shared" si="616"/>
+        <v>220</v>
+      </c>
+      <c r="Q214">
+        <f t="shared" si="617"/>
+        <v>30</v>
+      </c>
+      <c r="R214" s="20">
+        <f t="shared" si="618"/>
         <v>252</v>
       </c>
-      <c r="J214" s="26">
-        <f t="shared" si="613"/>
+      <c r="S214" s="20">
+        <f t="shared" si="619"/>
         <v>245</v>
       </c>
-      <c r="K214" t="str">
-        <f t="shared" si="614"/>
-        <v>static const CooGUI_tds Pos_GasSwitch_BottomLine_2_Normal = {160,210,32,215,220,30,252,245};</v>
-      </c>
-      <c r="L214">
-        <f t="shared" si="615"/>
-        <v>160</v>
-      </c>
-      <c r="M214" s="52">
-        <f t="shared" si="616"/>
-        <v>234</v>
-      </c>
-      <c r="N214">
-        <f t="shared" si="617"/>
-        <v>32</v>
-      </c>
-      <c r="O214">
-        <f t="shared" si="618"/>
-        <v>215</v>
-      </c>
-      <c r="P214">
-        <f t="shared" si="619"/>
-        <v>220</v>
-      </c>
-      <c r="Q214">
+      <c r="T214" t="str">
         <f t="shared" si="620"/>
-        <v>30</v>
-      </c>
-      <c r="R214" s="20">
+        <v>static const CooGUI_tds Pos_GasSwitch_BottomLine_2_Flipped = {160,234,32,215,220,30,252,245};</v>
+      </c>
+      <c r="U214" t="str">
         <f t="shared" si="621"/>
-        <v>252</v>
-      </c>
-      <c r="S214" s="20">
+        <v>const CooGUI_tds* Pos_GasSwitch_BottomLine_2;</v>
+      </c>
+      <c r="V214">
         <f t="shared" si="622"/>
-        <v>245</v>
-      </c>
-      <c r="T214" t="str">
+        <v>6.4453125</v>
+      </c>
+      <c r="W214" t="str">
         <f t="shared" si="623"/>
-        <v>static const CooGUI_tds Pos_GasSwitch_BottomLine_2_Flipped = {160,234,32,215,220,30,252,245};</v>
-      </c>
-      <c r="U214" t="str">
-        <f t="shared" si="624"/>
-        <v>const CooGUI_tds* Pos_GasSwitch_BottomLine_2;</v>
-      </c>
-      <c r="V214">
-        <f t="shared" si="625"/>
-        <v>6.4453125</v>
-      </c>
-      <c r="W214" t="str">
-        <f t="shared" si="626"/>
         <v>Pos_GasSwitch_BottomLine_2 = &amp;Pos_GasSwitch_BottomLine_2_Normal;</v>
       </c>
     </row>
@@ -23387,7 +23387,7 @@
         <v>297</v>
       </c>
       <c r="B215" t="str">
-        <f t="shared" ref="B215" si="627">CONCATENATE(A215, "_Normal")</f>
+        <f t="shared" ref="B215" si="625">CONCATENATE(A215, "_Normal")</f>
         <v>Pos_ErrorMsg_Line_0_Normal</v>
       </c>
       <c r="C215" s="26">
@@ -23411,7 +23411,7 @@
         <v>38</v>
       </c>
       <c r="I215" s="26">
-        <f t="shared" ref="I215" si="628">E215+G215</f>
+        <f t="shared" ref="I215" si="626">E215+G215</f>
         <v>320</v>
       </c>
       <c r="J215" s="26">
@@ -23419,55 +23419,55 @@
         <v>108</v>
       </c>
       <c r="K215" t="str">
-        <f t="shared" ref="K215" si="629">CONCATENATE("static const CooGUI_tds ",A215, "_Normal = {", C215, ",", D215, ",", E215, ",", F215, ",",G215, ",", H215,",",  I215, ",", J215, "};")</f>
+        <f t="shared" ref="K215" si="627">CONCATENATE("static const CooGUI_tds ",A215, "_Normal = {", C215, ",", D215, ",", E215, ",", F215, ",",G215, ",", H215,",",  I215, ",", J215, "};")</f>
         <v>static const CooGUI_tds Pos_ErrorMsg_Line_0_Normal = {160,65,0,70,320,38,320,108};</v>
       </c>
       <c r="L215">
-        <f t="shared" ref="L215" si="630">C215</f>
+        <f t="shared" ref="L215" si="628">C215</f>
         <v>160</v>
       </c>
       <c r="M215" s="52">
-        <f t="shared" ref="M215" si="631">D215 + $D$1</f>
+        <f t="shared" si="624"/>
         <v>89</v>
       </c>
       <c r="N215">
-        <f t="shared" ref="N215" si="632">E215</f>
+        <f t="shared" ref="N215" si="629">E215</f>
         <v>0</v>
       </c>
       <c r="O215">
-        <f t="shared" ref="O215" si="633">F215</f>
+        <f t="shared" ref="O215" si="630">F215</f>
         <v>70</v>
       </c>
       <c r="P215">
-        <f t="shared" ref="P215" si="634">G215</f>
+        <f t="shared" ref="P215" si="631">G215</f>
         <v>320</v>
       </c>
       <c r="Q215">
-        <f t="shared" ref="Q215" si="635">H215</f>
+        <f t="shared" ref="Q215" si="632">H215</f>
         <v>38</v>
       </c>
       <c r="R215" s="20">
-        <f t="shared" ref="R215" si="636">N215+P215</f>
+        <f t="shared" ref="R215" si="633">N215+P215</f>
         <v>320</v>
       </c>
       <c r="S215" s="20">
-        <f t="shared" ref="S215" si="637">O215+Q215</f>
+        <f t="shared" ref="S215" si="634">O215+Q215</f>
         <v>108</v>
       </c>
       <c r="T215" t="str">
-        <f t="shared" ref="T215" si="638">CONCATENATE("static const CooGUI_tds ",A215, "_Flipped = {", L215, ",", M215, ",", N215, ",", O215, ",",P215, ",", Q215,",",  R215, ",", S215, "};")</f>
+        <f t="shared" ref="T215" si="635">CONCATENATE("static const CooGUI_tds ",A215, "_Flipped = {", L215, ",", M215, ",", N215, ",", O215, ",",P215, ",", Q215,",",  R215, ",", S215, "};")</f>
         <v>static const CooGUI_tds Pos_ErrorMsg_Line_0_Flipped = {160,89,0,70,320,38,320,108};</v>
       </c>
       <c r="U215" t="str">
-        <f t="shared" ref="U215" si="639">CONCATENATE("const CooGUI_tds* ",A215, ";")</f>
+        <f t="shared" ref="U215" si="636">CONCATENATE("const CooGUI_tds* ",A215, ";")</f>
         <v>const CooGUI_tds* Pos_ErrorMsg_Line_0;</v>
       </c>
       <c r="V215">
-        <f t="shared" ref="V215" si="640">(G215*H215)/1024</f>
+        <f t="shared" ref="V215" si="637">(G215*H215)/1024</f>
         <v>11.875</v>
       </c>
       <c r="W215" t="str">
-        <f t="shared" ref="W215" si="641">CONCATENATE(A215, " = &amp;", B215,";")</f>
+        <f t="shared" ref="W215" si="638">CONCATENATE(A215, " = &amp;", B215,";")</f>
         <v>Pos_ErrorMsg_Line_0 = &amp;Pos_ErrorMsg_Line_0_Normal;</v>
       </c>
     </row>
@@ -23476,7 +23476,7 @@
         <v>298</v>
       </c>
       <c r="B216" t="str">
-        <f t="shared" ref="B216:B217" si="642">CONCATENATE(A216, "_Normal")</f>
+        <f t="shared" ref="B216:B217" si="639">CONCATENATE(A216, "_Normal")</f>
         <v>Pos_ErrorMsg_Line_1_Normal</v>
       </c>
       <c r="C216" s="26">
@@ -23500,67 +23500,67 @@
         <v>320</v>
       </c>
       <c r="H216" s="50">
-        <f t="shared" ref="H216:H217" si="643">H215</f>
+        <f t="shared" ref="H216:H217" si="640">H215</f>
         <v>38</v>
       </c>
       <c r="I216" s="26">
-        <f t="shared" ref="I216:I217" si="644">E216+G216</f>
+        <f t="shared" ref="I216:I217" si="641">E216+G216</f>
         <v>320</v>
       </c>
       <c r="J216" s="26">
-        <f t="shared" ref="J216:J217" si="645">F216+H216</f>
+        <f t="shared" ref="J216:J217" si="642">F216+H216</f>
         <v>146</v>
       </c>
       <c r="K216" t="str">
-        <f t="shared" ref="K216:K217" si="646">CONCATENATE("static const CooGUI_tds ",A216, "_Normal = {", C216, ",", D216, ",", E216, ",", F216, ",",G216, ",", H216,",",  I216, ",", J216, "};")</f>
+        <f t="shared" ref="K216:K217" si="643">CONCATENATE("static const CooGUI_tds ",A216, "_Normal = {", C216, ",", D216, ",", E216, ",", F216, ",",G216, ",", H216,",",  I216, ",", J216, "};")</f>
         <v>static const CooGUI_tds Pos_ErrorMsg_Line_1_Normal = {160,103,0,108,320,38,320,146};</v>
       </c>
       <c r="L216">
-        <f t="shared" ref="L216:L217" si="647">C216</f>
+        <f t="shared" ref="L216:L217" si="644">C216</f>
         <v>160</v>
       </c>
       <c r="M216" s="52">
-        <f t="shared" ref="M216:M217" si="648">D216 + $D$1</f>
+        <f t="shared" si="624"/>
         <v>127</v>
       </c>
       <c r="N216">
-        <f t="shared" ref="N216:N217" si="649">E216</f>
+        <f t="shared" ref="N216:N217" si="645">E216</f>
         <v>0</v>
       </c>
       <c r="O216">
-        <f t="shared" ref="O216:O217" si="650">F216</f>
+        <f t="shared" ref="O216:O217" si="646">F216</f>
         <v>108</v>
       </c>
       <c r="P216">
-        <f t="shared" ref="P216:P217" si="651">G216</f>
+        <f t="shared" ref="P216:P217" si="647">G216</f>
         <v>320</v>
       </c>
       <c r="Q216">
-        <f t="shared" ref="Q216:Q217" si="652">H216</f>
+        <f t="shared" ref="Q216:Q217" si="648">H216</f>
         <v>38</v>
       </c>
       <c r="R216" s="20">
-        <f t="shared" ref="R216:R217" si="653">N216+P216</f>
+        <f t="shared" ref="R216:R217" si="649">N216+P216</f>
         <v>320</v>
       </c>
       <c r="S216" s="20">
-        <f t="shared" ref="S216:S217" si="654">O216+Q216</f>
+        <f t="shared" ref="S216:S217" si="650">O216+Q216</f>
         <v>146</v>
       </c>
       <c r="T216" t="str">
-        <f t="shared" ref="T216:T217" si="655">CONCATENATE("static const CooGUI_tds ",A216, "_Flipped = {", L216, ",", M216, ",", N216, ",", O216, ",",P216, ",", Q216,",",  R216, ",", S216, "};")</f>
+        <f t="shared" ref="T216:T217" si="651">CONCATENATE("static const CooGUI_tds ",A216, "_Flipped = {", L216, ",", M216, ",", N216, ",", O216, ",",P216, ",", Q216,",",  R216, ",", S216, "};")</f>
         <v>static const CooGUI_tds Pos_ErrorMsg_Line_1_Flipped = {160,127,0,108,320,38,320,146};</v>
       </c>
       <c r="U216" t="str">
-        <f t="shared" ref="U216:U217" si="656">CONCATENATE("const CooGUI_tds* ",A216, ";")</f>
+        <f t="shared" ref="U216:U217" si="652">CONCATENATE("const CooGUI_tds* ",A216, ";")</f>
         <v>const CooGUI_tds* Pos_ErrorMsg_Line_1;</v>
       </c>
       <c r="V216">
-        <f t="shared" ref="V216:V217" si="657">(G216*H216)/1024</f>
+        <f t="shared" ref="V216:V217" si="653">(G216*H216)/1024</f>
         <v>11.875</v>
       </c>
       <c r="W216" t="str">
-        <f t="shared" ref="W216:W217" si="658">CONCATENATE(A216, " = &amp;", B216,";")</f>
+        <f t="shared" ref="W216:W217" si="654">CONCATENATE(A216, " = &amp;", B216,";")</f>
         <v>Pos_ErrorMsg_Line_1 = &amp;Pos_ErrorMsg_Line_1_Normal;</v>
       </c>
     </row>
@@ -23569,11 +23569,11 @@
         <v>299</v>
       </c>
       <c r="B217" t="str">
-        <f t="shared" si="642"/>
+        <f t="shared" si="639"/>
         <v>Pos_ErrorMsg_Line_2_Normal</v>
       </c>
       <c r="C217" s="26">
-        <f t="shared" ref="C217" si="659">C216</f>
+        <f t="shared" ref="C217" si="655">C216</f>
         <v>160</v>
       </c>
       <c r="D217" s="26">
@@ -23581,79 +23581,79 @@
         <v>141</v>
       </c>
       <c r="E217" s="23">
-        <f t="shared" ref="E217:E218" si="660">E216</f>
+        <f t="shared" ref="E217:E218" si="656">E216</f>
         <v>0</v>
       </c>
       <c r="F217" s="26">
-        <f t="shared" ref="F217" si="661">J216</f>
+        <f t="shared" ref="F217" si="657">J216</f>
         <v>146</v>
       </c>
       <c r="G217" s="22">
-        <f t="shared" ref="G217:G218" si="662">G216</f>
+        <f t="shared" ref="G217:G218" si="658">G216</f>
         <v>320</v>
       </c>
       <c r="H217" s="50">
+        <f t="shared" si="640"/>
+        <v>38</v>
+      </c>
+      <c r="I217" s="26">
+        <f t="shared" si="641"/>
+        <v>320</v>
+      </c>
+      <c r="J217" s="26">
+        <f t="shared" si="642"/>
+        <v>184</v>
+      </c>
+      <c r="K217" t="str">
         <f t="shared" si="643"/>
+        <v>static const CooGUI_tds Pos_ErrorMsg_Line_2_Normal = {160,141,0,146,320,38,320,184};</v>
+      </c>
+      <c r="L217">
+        <f t="shared" si="644"/>
+        <v>160</v>
+      </c>
+      <c r="M217" s="52">
+        <f t="shared" si="624"/>
+        <v>165</v>
+      </c>
+      <c r="N217">
+        <f t="shared" si="645"/>
+        <v>0</v>
+      </c>
+      <c r="O217">
+        <f t="shared" si="646"/>
+        <v>146</v>
+      </c>
+      <c r="P217">
+        <f t="shared" si="647"/>
+        <v>320</v>
+      </c>
+      <c r="Q217">
+        <f t="shared" si="648"/>
         <v>38</v>
       </c>
-      <c r="I217" s="26">
-        <f t="shared" si="644"/>
+      <c r="R217" s="20">
+        <f t="shared" si="649"/>
         <v>320</v>
       </c>
-      <c r="J217" s="26">
-        <f t="shared" si="645"/>
+      <c r="S217" s="20">
+        <f t="shared" si="650"/>
         <v>184</v>
       </c>
-      <c r="K217" t="str">
-        <f t="shared" si="646"/>
-        <v>static const CooGUI_tds Pos_ErrorMsg_Line_2_Normal = {160,141,0,146,320,38,320,184};</v>
-      </c>
-      <c r="L217">
-        <f t="shared" si="647"/>
-        <v>160</v>
-      </c>
-      <c r="M217" s="52">
-        <f t="shared" si="648"/>
-        <v>165</v>
-      </c>
-      <c r="N217">
-        <f t="shared" si="649"/>
-        <v>0</v>
-      </c>
-      <c r="O217">
-        <f t="shared" si="650"/>
-        <v>146</v>
-      </c>
-      <c r="P217">
+      <c r="T217" t="str">
         <f t="shared" si="651"/>
-        <v>320</v>
-      </c>
-      <c r="Q217">
+        <v>static const CooGUI_tds Pos_ErrorMsg_Line_2_Flipped = {160,165,0,146,320,38,320,184};</v>
+      </c>
+      <c r="U217" t="str">
         <f t="shared" si="652"/>
-        <v>38</v>
-      </c>
-      <c r="R217" s="20">
+        <v>const CooGUI_tds* Pos_ErrorMsg_Line_2;</v>
+      </c>
+      <c r="V217">
         <f t="shared" si="653"/>
-        <v>320</v>
-      </c>
-      <c r="S217" s="20">
+        <v>11.875</v>
+      </c>
+      <c r="W217" t="str">
         <f t="shared" si="654"/>
-        <v>184</v>
-      </c>
-      <c r="T217" t="str">
-        <f t="shared" si="655"/>
-        <v>static const CooGUI_tds Pos_ErrorMsg_Line_2_Flipped = {160,165,0,146,320,38,320,184};</v>
-      </c>
-      <c r="U217" t="str">
-        <f t="shared" si="656"/>
-        <v>const CooGUI_tds* Pos_ErrorMsg_Line_2;</v>
-      </c>
-      <c r="V217">
-        <f t="shared" si="657"/>
-        <v>11.875</v>
-      </c>
-      <c r="W217" t="str">
-        <f t="shared" si="658"/>
         <v>Pos_ErrorMsg_Line_2 = &amp;Pos_ErrorMsg_Line_2_Normal;</v>
       </c>
     </row>
@@ -23662,91 +23662,91 @@
         <v>300</v>
       </c>
       <c r="B218" t="str">
-        <f t="shared" ref="B218" si="663">CONCATENATE(A218, "_Normal")</f>
+        <f t="shared" ref="B218" si="659">CONCATENATE(A218, "_Normal")</f>
         <v>Pos_ErrorMsg_Line_3_Normal</v>
       </c>
       <c r="C218" s="26">
-        <f t="shared" ref="C218" si="664">C217</f>
+        <f t="shared" ref="C218" si="660">C217</f>
         <v>160</v>
       </c>
       <c r="D218" s="26">
-        <f t="shared" ref="D218" si="665">F218 - 5</f>
+        <f t="shared" ref="D218" si="661">F218 - 5</f>
         <v>179</v>
       </c>
       <c r="E218" s="23">
-        <f t="shared" si="660"/>
+        <f t="shared" si="656"/>
         <v>0</v>
       </c>
       <c r="F218" s="26">
-        <f t="shared" ref="F218" si="666">J217</f>
+        <f t="shared" ref="F218" si="662">J217</f>
         <v>184</v>
       </c>
       <c r="G218" s="22">
-        <f t="shared" si="662"/>
+        <f t="shared" si="658"/>
         <v>320</v>
       </c>
       <c r="H218" s="50">
-        <f t="shared" ref="H218" si="667">H217</f>
+        <f t="shared" ref="H218" si="663">H217</f>
         <v>38</v>
       </c>
       <c r="I218" s="26">
-        <f t="shared" ref="I218" si="668">E218+G218</f>
+        <f t="shared" ref="I218" si="664">E218+G218</f>
         <v>320</v>
       </c>
       <c r="J218" s="26">
-        <f t="shared" ref="J218" si="669">F218+H218</f>
+        <f t="shared" ref="J218" si="665">F218+H218</f>
         <v>222</v>
       </c>
       <c r="K218" t="str">
-        <f t="shared" ref="K218" si="670">CONCATENATE("static const CooGUI_tds ",A218, "_Normal = {", C218, ",", D218, ",", E218, ",", F218, ",",G218, ",", H218,",",  I218, ",", J218, "};")</f>
+        <f t="shared" ref="K218" si="666">CONCATENATE("static const CooGUI_tds ",A218, "_Normal = {", C218, ",", D218, ",", E218, ",", F218, ",",G218, ",", H218,",",  I218, ",", J218, "};")</f>
         <v>static const CooGUI_tds Pos_ErrorMsg_Line_3_Normal = {160,179,0,184,320,38,320,222};</v>
       </c>
       <c r="L218">
-        <f t="shared" ref="L218" si="671">C218</f>
+        <f t="shared" ref="L218" si="667">C218</f>
         <v>160</v>
       </c>
       <c r="M218" s="52">
-        <f t="shared" ref="M218" si="672">D218 + $D$1</f>
+        <f t="shared" si="624"/>
         <v>203</v>
       </c>
       <c r="N218">
-        <f t="shared" ref="N218" si="673">E218</f>
+        <f t="shared" ref="N218" si="668">E218</f>
         <v>0</v>
       </c>
       <c r="O218">
-        <f t="shared" ref="O218" si="674">F218</f>
+        <f t="shared" ref="O218" si="669">F218</f>
         <v>184</v>
       </c>
       <c r="P218">
-        <f t="shared" ref="P218" si="675">G218</f>
+        <f t="shared" ref="P218" si="670">G218</f>
         <v>320</v>
       </c>
       <c r="Q218">
-        <f t="shared" ref="Q218" si="676">H218</f>
+        <f t="shared" ref="Q218" si="671">H218</f>
         <v>38</v>
       </c>
       <c r="R218" s="20">
-        <f t="shared" ref="R218" si="677">N218+P218</f>
+        <f t="shared" ref="R218" si="672">N218+P218</f>
         <v>320</v>
       </c>
       <c r="S218" s="20">
-        <f t="shared" ref="S218" si="678">O218+Q218</f>
+        <f t="shared" ref="S218" si="673">O218+Q218</f>
         <v>222</v>
       </c>
       <c r="T218" t="str">
-        <f t="shared" ref="T218" si="679">CONCATENATE("static const CooGUI_tds ",A218, "_Flipped = {", L218, ",", M218, ",", N218, ",", O218, ",",P218, ",", Q218,",",  R218, ",", S218, "};")</f>
+        <f t="shared" ref="T218" si="674">CONCATENATE("static const CooGUI_tds ",A218, "_Flipped = {", L218, ",", M218, ",", N218, ",", O218, ",",P218, ",", Q218,",",  R218, ",", S218, "};")</f>
         <v>static const CooGUI_tds Pos_ErrorMsg_Line_3_Flipped = {160,203,0,184,320,38,320,222};</v>
       </c>
       <c r="U218" t="str">
-        <f t="shared" ref="U218" si="680">CONCATENATE("const CooGUI_tds* ",A218, ";")</f>
+        <f t="shared" ref="U218" si="675">CONCATENATE("const CooGUI_tds* ",A218, ";")</f>
         <v>const CooGUI_tds* Pos_ErrorMsg_Line_3;</v>
       </c>
       <c r="V218">
-        <f t="shared" ref="V218" si="681">(G218*H218)/1024</f>
+        <f t="shared" ref="V218" si="676">(G218*H218)/1024</f>
         <v>11.875</v>
       </c>
       <c r="W218" t="str">
-        <f t="shared" ref="W218" si="682">CONCATENATE(A218, " = &amp;", B218,";")</f>
+        <f t="shared" ref="W218" si="677">CONCATENATE(A218, " = &amp;", B218,";")</f>
         <v>Pos_ErrorMsg_Line_3 = &amp;Pos_ErrorMsg_Line_3_Normal;</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[Surface mode] - Update input sheet Required to generate Coordinator config
</commit_message>
<xml_diff>
--- a/UserInterface/Scripts/DSX_CoordinationClear.xlsx
+++ b/UserInterface/Scripts/DSX_CoordinationClear.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ducth\Downloads\DSX_Projects_T6_ALL\UserInterface\Scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCA8849C-929B-4FBA-A336-88E5D965D75F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03C95161-1E87-4C07-90F4-4A756B9919E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3853,9 +3853,9 @@
   <dimension ref="A1:W218"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A199" zoomScale="103" zoomScaleNormal="103" workbookViewId="0">
-      <pane ySplit="6290" topLeftCell="A209" activePane="bottomLeft"/>
+      <pane ySplit="6290" topLeftCell="A205" activePane="bottomLeft"/>
       <selection activeCell="H215" sqref="H215"/>
-      <selection pane="bottomLeft" activeCell="A231" sqref="A231"/>
+      <selection pane="bottomLeft" activeCell="N224" sqref="N224"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -18407,7 +18407,7 @@
         <v>120</v>
       </c>
       <c r="M160" s="52">
-        <f t="shared" ref="M160:M173" si="282">D160 + $D$1</f>
+        <f t="shared" ref="M160:M166" si="282">D160 + $D$1</f>
         <v>121</v>
       </c>
       <c r="N160">
@@ -19699,7 +19699,7 @@
         <v>85</v>
       </c>
       <c r="O174">
-        <f t="shared" ref="O174:O189" si="308">F174</f>
+        <f>F174</f>
         <v>115</v>
       </c>
       <c r="P174">
@@ -19740,7 +19740,7 @@
         <v>181</v>
       </c>
       <c r="B175" t="str">
-        <f t="shared" ref="B175:B189" si="309">CONCATENATE(A175, "_Normal")</f>
+        <f t="shared" ref="B175:B189" si="308">CONCATENATE(A175, "_Normal")</f>
         <v>Pos_Bluetooth_PasscodeValue_Normal</v>
       </c>
       <c r="C175" s="22">
@@ -19766,19 +19766,19 @@
         <v>60</v>
       </c>
       <c r="I175" s="20">
-        <f t="shared" ref="I175:I189" si="310">E175+G175</f>
+        <f t="shared" ref="I175:I189" si="309">E175+G175</f>
         <v>235</v>
       </c>
       <c r="J175" s="20">
-        <f t="shared" ref="J175:J189" si="311">F175+H175</f>
+        <f t="shared" ref="J175:J189" si="310">F175+H175</f>
         <v>200</v>
       </c>
       <c r="K175" t="str">
-        <f t="shared" ref="K175:K189" si="312">CONCATENATE("static const CooGUI_tds ",A175, "_Normal = {", C175, ",", D175, ",", E175, ",", F175, ",",G175, ",", H175,",",  I175, ",", J175, "};")</f>
+        <f t="shared" ref="K175:K189" si="311">CONCATENATE("static const CooGUI_tds ",A175, "_Normal = {", C175, ",", D175, ",", E175, ",", F175, ",",G175, ",", H175,",",  I175, ",", J175, "};")</f>
         <v>static const CooGUI_tds Pos_Bluetooth_PasscodeValue_Normal = {160,140,85,140,150,60,235,200};</v>
       </c>
       <c r="L175">
-        <f t="shared" ref="L175:L189" si="313">C175</f>
+        <f t="shared" ref="L175:L189" si="312">C175</f>
         <v>160</v>
       </c>
       <c r="M175" s="52">
@@ -19786,7 +19786,7 @@
         <v>140</v>
       </c>
       <c r="N175">
-        <f t="shared" ref="N175:N189" si="314">E175</f>
+        <f t="shared" ref="N175:N189" si="313">E175</f>
         <v>85</v>
       </c>
       <c r="O175">
@@ -19798,31 +19798,31 @@
         <v>150</v>
       </c>
       <c r="Q175">
-        <f t="shared" ref="Q175:Q189" si="315">H175</f>
+        <f t="shared" ref="Q175:Q189" si="314">H175</f>
         <v>60</v>
       </c>
       <c r="R175" s="20">
-        <f t="shared" ref="R175:R189" si="316">N175+P175</f>
+        <f t="shared" ref="R175:R189" si="315">N175+P175</f>
         <v>235</v>
       </c>
       <c r="S175" s="20">
-        <f t="shared" ref="S175:S189" si="317">O175+Q175</f>
+        <f t="shared" ref="S175:S189" si="316">O175+Q175</f>
         <v>200</v>
       </c>
       <c r="T175" t="str">
-        <f t="shared" ref="T175:T189" si="318">CONCATENATE("static const CooGUI_tds ",A175, "_Flipped = {", L175, ",", M175, ",", N175, ",", O175, ",",P175, ",", Q175,",",  R175, ",", S175, "};")</f>
+        <f t="shared" ref="T175:T189" si="317">CONCATENATE("static const CooGUI_tds ",A175, "_Flipped = {", L175, ",", M175, ",", N175, ",", O175, ",",P175, ",", Q175,",",  R175, ",", S175, "};")</f>
         <v>static const CooGUI_tds Pos_Bluetooth_PasscodeValue_Flipped = {160,140,85,140,150,60,235,200};</v>
       </c>
       <c r="U175" t="str">
-        <f t="shared" ref="U175:U189" si="319">CONCATENATE("const CooGUI_tds* ",A175, ";")</f>
+        <f t="shared" ref="U175:U189" si="318">CONCATENATE("const CooGUI_tds* ",A175, ";")</f>
         <v>const CooGUI_tds* Pos_Bluetooth_PasscodeValue;</v>
       </c>
       <c r="V175">
-        <f t="shared" ref="V175:V189" si="320">(G175*H175)/1024</f>
+        <f t="shared" ref="V175:V189" si="319">(G175*H175)/1024</f>
         <v>8.7890625</v>
       </c>
       <c r="W175" t="str">
-        <f t="shared" ref="W175:W189" si="321">CONCATENATE(A175, " = &amp;", B175,";")</f>
+        <f t="shared" ref="W175:W189" si="320">CONCATENATE(A175, " = &amp;", B175,";")</f>
         <v>Pos_Bluetooth_PasscodeValue = &amp;Pos_Bluetooth_PasscodeValue_Normal;</v>
       </c>
     </row>
@@ -19831,7 +19831,7 @@
         <v>307</v>
       </c>
       <c r="B176" t="str">
-        <f t="shared" ref="B176" si="322">CONCATENATE(A176, "_Normal")</f>
+        <f t="shared" ref="B176" si="321">CONCATENATE(A176, "_Normal")</f>
         <v>Pos_Bluetooth_DownLoadData_01_Normal</v>
       </c>
       <c r="C176" s="22">
@@ -19843,7 +19843,7 @@
         <v>115</v>
       </c>
       <c r="E176" s="23">
-        <f t="shared" ref="E176" si="323">C176-G176/2</f>
+        <f t="shared" ref="E176" si="322">C176-G176/2</f>
         <v>0</v>
       </c>
       <c r="F176" s="23">
@@ -19857,19 +19857,19 @@
         <v>32</v>
       </c>
       <c r="I176" s="20">
-        <f t="shared" ref="I176" si="324">E176+G176</f>
+        <f t="shared" ref="I176" si="323">E176+G176</f>
         <v>320</v>
       </c>
       <c r="J176" s="20">
-        <f t="shared" ref="J176" si="325">F176+H176</f>
+        <f t="shared" ref="J176" si="324">F176+H176</f>
         <v>147</v>
       </c>
       <c r="K176" t="str">
-        <f t="shared" ref="K176" si="326">CONCATENATE("static const CooGUI_tds ",A176, "_Normal = {", C176, ",", D176, ",", E176, ",", F176, ",",G176, ",", H176,",",  I176, ",", J176, "};")</f>
+        <f t="shared" ref="K176" si="325">CONCATENATE("static const CooGUI_tds ",A176, "_Normal = {", C176, ",", D176, ",", E176, ",", F176, ",",G176, ",", H176,",",  I176, ",", J176, "};")</f>
         <v>static const CooGUI_tds Pos_Bluetooth_DownLoadData_01_Normal = {160,115,0,115,320,32,320,147};</v>
       </c>
       <c r="L176">
-        <f t="shared" ref="L176" si="327">C176</f>
+        <f t="shared" ref="L176" si="326">C176</f>
         <v>160</v>
       </c>
       <c r="M176" s="52">
@@ -19877,7 +19877,7 @@
         <v>115</v>
       </c>
       <c r="N176">
-        <f t="shared" ref="N176" si="328">E176</f>
+        <f t="shared" ref="N176" si="327">E176</f>
         <v>0</v>
       </c>
       <c r="O176">
@@ -19885,35 +19885,35 @@
         <v>115</v>
       </c>
       <c r="P176">
-        <f t="shared" ref="P176" si="329">G176</f>
+        <f t="shared" ref="P176" si="328">G176</f>
         <v>320</v>
       </c>
       <c r="Q176">
-        <f t="shared" ref="Q176" si="330">H176</f>
+        <f t="shared" ref="Q176" si="329">H176</f>
         <v>32</v>
       </c>
       <c r="R176" s="20">
-        <f t="shared" ref="R176" si="331">N176+P176</f>
+        <f t="shared" ref="R176" si="330">N176+P176</f>
         <v>320</v>
       </c>
       <c r="S176" s="20">
-        <f t="shared" ref="S176" si="332">O176+Q176</f>
+        <f t="shared" ref="S176" si="331">O176+Q176</f>
         <v>147</v>
       </c>
       <c r="T176" t="str">
-        <f t="shared" ref="T176" si="333">CONCATENATE("static const CooGUI_tds ",A176, "_Flipped = {", L176, ",", M176, ",", N176, ",", O176, ",",P176, ",", Q176,",",  R176, ",", S176, "};")</f>
+        <f t="shared" ref="T176" si="332">CONCATENATE("static const CooGUI_tds ",A176, "_Flipped = {", L176, ",", M176, ",", N176, ",", O176, ",",P176, ",", Q176,",",  R176, ",", S176, "};")</f>
         <v>static const CooGUI_tds Pos_Bluetooth_DownLoadData_01_Flipped = {160,115,0,115,320,32,320,147};</v>
       </c>
       <c r="U176" t="str">
-        <f t="shared" ref="U176" si="334">CONCATENATE("const CooGUI_tds* ",A176, ";")</f>
+        <f t="shared" ref="U176" si="333">CONCATENATE("const CooGUI_tds* ",A176, ";")</f>
         <v>const CooGUI_tds* Pos_Bluetooth_DownLoadData_01;</v>
       </c>
       <c r="V176">
-        <f t="shared" ref="V176" si="335">(G176*H176)/1024</f>
+        <f t="shared" ref="V176" si="334">(G176*H176)/1024</f>
         <v>10</v>
       </c>
       <c r="W176" t="str">
-        <f t="shared" ref="W176" si="336">CONCATENATE(A176, " = &amp;", B176,";")</f>
+        <f t="shared" ref="W176" si="335">CONCATENATE(A176, " = &amp;", B176,";")</f>
         <v>Pos_Bluetooth_DownLoadData_01 = &amp;Pos_Bluetooth_DownLoadData_01_Normal;</v>
       </c>
     </row>
@@ -19922,7 +19922,7 @@
         <v>308</v>
       </c>
       <c r="B177" t="str">
-        <f t="shared" ref="B177" si="337">CONCATENATE(A177, "_Normal")</f>
+        <f t="shared" ref="B177" si="336">CONCATENATE(A177, "_Normal")</f>
         <v>Pos_Bluetooth_DownLoadData_02_Normal</v>
       </c>
       <c r="C177" s="22">
@@ -19950,19 +19950,19 @@
         <v>32</v>
       </c>
       <c r="I177" s="20">
-        <f t="shared" ref="I177" si="338">E177+G177</f>
+        <f t="shared" ref="I177" si="337">E177+G177</f>
         <v>320</v>
       </c>
       <c r="J177" s="20">
-        <f t="shared" ref="J177" si="339">F177+H177</f>
+        <f t="shared" ref="J177" si="338">F177+H177</f>
         <v>179</v>
       </c>
       <c r="K177" t="str">
-        <f t="shared" ref="K177" si="340">CONCATENATE("static const CooGUI_tds ",A177, "_Normal = {", C177, ",", D177, ",", E177, ",", F177, ",",G177, ",", H177,",",  I177, ",", J177, "};")</f>
+        <f t="shared" ref="K177" si="339">CONCATENATE("static const CooGUI_tds ",A177, "_Normal = {", C177, ",", D177, ",", E177, ",", F177, ",",G177, ",", H177,",",  I177, ",", J177, "};")</f>
         <v>static const CooGUI_tds Pos_Bluetooth_DownLoadData_02_Normal = {160,147,0,147,320,32,320,179};</v>
       </c>
       <c r="L177">
-        <f t="shared" ref="L177" si="341">C177</f>
+        <f t="shared" ref="L177" si="340">C177</f>
         <v>160</v>
       </c>
       <c r="M177" s="52">
@@ -19970,43 +19970,43 @@
         <v>147</v>
       </c>
       <c r="N177">
-        <f t="shared" ref="N177" si="342">E177</f>
+        <f t="shared" ref="N177" si="341">E177</f>
         <v>0</v>
       </c>
       <c r="O177">
-        <f t="shared" ref="O177" si="343">F177</f>
+        <f t="shared" ref="O177" si="342">F177</f>
         <v>147</v>
       </c>
       <c r="P177">
-        <f t="shared" ref="P177" si="344">G177</f>
+        <f t="shared" ref="P177" si="343">G177</f>
         <v>320</v>
       </c>
       <c r="Q177">
-        <f t="shared" ref="Q177" si="345">H177</f>
+        <f t="shared" ref="Q177" si="344">H177</f>
         <v>32</v>
       </c>
       <c r="R177" s="20">
-        <f t="shared" ref="R177" si="346">N177+P177</f>
+        <f t="shared" ref="R177" si="345">N177+P177</f>
         <v>320</v>
       </c>
       <c r="S177" s="20">
-        <f t="shared" ref="S177" si="347">O177+Q177</f>
+        <f t="shared" ref="S177" si="346">O177+Q177</f>
         <v>179</v>
       </c>
       <c r="T177" t="str">
-        <f t="shared" ref="T177" si="348">CONCATENATE("static const CooGUI_tds ",A177, "_Flipped = {", L177, ",", M177, ",", N177, ",", O177, ",",P177, ",", Q177,",",  R177, ",", S177, "};")</f>
+        <f t="shared" ref="T177" si="347">CONCATENATE("static const CooGUI_tds ",A177, "_Flipped = {", L177, ",", M177, ",", N177, ",", O177, ",",P177, ",", Q177,",",  R177, ",", S177, "};")</f>
         <v>static const CooGUI_tds Pos_Bluetooth_DownLoadData_02_Flipped = {160,147,0,147,320,32,320,179};</v>
       </c>
       <c r="U177" t="str">
-        <f t="shared" ref="U177" si="349">CONCATENATE("const CooGUI_tds* ",A177, ";")</f>
+        <f t="shared" ref="U177" si="348">CONCATENATE("const CooGUI_tds* ",A177, ";")</f>
         <v>const CooGUI_tds* Pos_Bluetooth_DownLoadData_02;</v>
       </c>
       <c r="V177">
-        <f t="shared" ref="V177" si="350">(G177*H177)/1024</f>
+        <f t="shared" ref="V177" si="349">(G177*H177)/1024</f>
         <v>10</v>
       </c>
       <c r="W177" t="str">
-        <f t="shared" ref="W177" si="351">CONCATENATE(A177, " = &amp;", B177,";")</f>
+        <f t="shared" ref="W177" si="350">CONCATENATE(A177, " = &amp;", B177,";")</f>
         <v>Pos_Bluetooth_DownLoadData_02 = &amp;Pos_Bluetooth_DownLoadData_02_Normal;</v>
       </c>
     </row>
@@ -20015,7 +20015,7 @@
         <v>191</v>
       </c>
       <c r="B178" t="str">
-        <f t="shared" si="309"/>
+        <f t="shared" si="308"/>
         <v>Pos_Slates_Tittle_Normal</v>
       </c>
       <c r="C178" s="9">
@@ -20039,63 +20039,63 @@
         <v>23</v>
       </c>
       <c r="I178" s="20">
+        <f t="shared" si="309"/>
+        <v>320</v>
+      </c>
+      <c r="J178" s="20">
         <f t="shared" si="310"/>
-        <v>320</v>
-      </c>
-      <c r="J178" s="20">
+        <v>23</v>
+      </c>
+      <c r="K178" t="str">
         <f t="shared" si="311"/>
-        <v>23</v>
-      </c>
-      <c r="K178" t="str">
+        <v>static const CooGUI_tds Pos_Slates_Tittle_Normal = {180,0,180,0,140,23,320,23};</v>
+      </c>
+      <c r="L178">
         <f t="shared" si="312"/>
-        <v>static const CooGUI_tds Pos_Slates_Tittle_Normal = {180,0,180,0,140,23,320,23};</v>
-      </c>
-      <c r="L178">
+        <v>180</v>
+      </c>
+      <c r="M178" s="52">
+        <f t="shared" ref="M178:M189" si="351">D178 + $D$1</f>
+        <v>24</v>
+      </c>
+      <c r="N178">
         <f t="shared" si="313"/>
         <v>180</v>
       </c>
-      <c r="M178" s="52">
-        <f t="shared" ref="M174:M189" si="352">D178 + $D$1</f>
-        <v>24</v>
-      </c>
-      <c r="N178">
+      <c r="O178">
+        <f t="shared" ref="O174:O189" si="352">F178</f>
+        <v>0</v>
+      </c>
+      <c r="P178">
+        <f t="shared" ref="P178:P189" si="353">G178</f>
+        <v>140</v>
+      </c>
+      <c r="Q178">
         <f t="shared" si="314"/>
-        <v>180</v>
-      </c>
-      <c r="O178">
-        <f t="shared" si="308"/>
-        <v>0</v>
-      </c>
-      <c r="P178">
-        <f t="shared" ref="P175:P189" si="353">G178</f>
-        <v>140</v>
-      </c>
-      <c r="Q178">
+        <v>23</v>
+      </c>
+      <c r="R178" s="20">
         <f t="shared" si="315"/>
+        <v>320</v>
+      </c>
+      <c r="S178" s="20">
+        <f t="shared" si="316"/>
         <v>23</v>
       </c>
-      <c r="R178" s="20">
-        <f t="shared" si="316"/>
-        <v>320</v>
-      </c>
-      <c r="S178" s="20">
+      <c r="T178" t="str">
         <f t="shared" si="317"/>
-        <v>23</v>
-      </c>
-      <c r="T178" t="str">
+        <v>static const CooGUI_tds Pos_Slates_Tittle_Flipped = {180,24,180,0,140,23,320,23};</v>
+      </c>
+      <c r="U178" t="str">
         <f t="shared" si="318"/>
-        <v>static const CooGUI_tds Pos_Slates_Tittle_Flipped = {180,24,180,0,140,23,320,23};</v>
-      </c>
-      <c r="U178" t="str">
+        <v>const CooGUI_tds* Pos_Slates_Tittle;</v>
+      </c>
+      <c r="V178">
         <f t="shared" si="319"/>
-        <v>const CooGUI_tds* Pos_Slates_Tittle;</v>
-      </c>
-      <c r="V178">
+        <v>3.14453125</v>
+      </c>
+      <c r="W178" t="str">
         <f t="shared" si="320"/>
-        <v>3.14453125</v>
-      </c>
-      <c r="W178" t="str">
-        <f t="shared" si="321"/>
         <v>Pos_Slates_Tittle = &amp;Pos_Slates_Tittle_Normal;</v>
       </c>
     </row>
@@ -20104,7 +20104,7 @@
         <v>203</v>
       </c>
       <c r="B179" t="str">
-        <f t="shared" si="309"/>
+        <f t="shared" si="308"/>
         <v>Pos_SurfClearToUpdate_1_Normal</v>
       </c>
       <c r="C179" s="23">
@@ -20127,31 +20127,31 @@
         <v>90</v>
       </c>
       <c r="I179" s="20">
+        <f t="shared" si="309"/>
+        <v>285</v>
+      </c>
+      <c r="J179" s="20">
         <f t="shared" si="310"/>
-        <v>285</v>
-      </c>
-      <c r="J179" s="20">
+        <v>210</v>
+      </c>
+      <c r="K179" t="str">
         <f t="shared" si="311"/>
-        <v>210</v>
-      </c>
-      <c r="K179" t="str">
+        <v>static const CooGUI_tds Pos_SurfClearToUpdate_1_Normal = {0,0,25,120,260,90,285,210};</v>
+      </c>
+      <c r="L179">
         <f t="shared" si="312"/>
-        <v>static const CooGUI_tds Pos_SurfClearToUpdate_1_Normal = {0,0,25,120,260,90,285,210};</v>
-      </c>
-      <c r="L179">
+        <v>0</v>
+      </c>
+      <c r="M179" s="52">
+        <f t="shared" si="351"/>
+        <v>24</v>
+      </c>
+      <c r="N179">
         <f t="shared" si="313"/>
-        <v>0</v>
-      </c>
-      <c r="M179" s="52">
+        <v>25</v>
+      </c>
+      <c r="O179">
         <f t="shared" si="352"/>
-        <v>24</v>
-      </c>
-      <c r="N179">
-        <f t="shared" si="314"/>
-        <v>25</v>
-      </c>
-      <c r="O179">
-        <f t="shared" si="308"/>
         <v>120</v>
       </c>
       <c r="P179">
@@ -20159,31 +20159,31 @@
         <v>260</v>
       </c>
       <c r="Q179">
+        <f t="shared" si="314"/>
+        <v>90</v>
+      </c>
+      <c r="R179" s="20">
         <f t="shared" si="315"/>
-        <v>90</v>
-      </c>
-      <c r="R179" s="20">
+        <v>285</v>
+      </c>
+      <c r="S179" s="20">
         <f t="shared" si="316"/>
-        <v>285</v>
-      </c>
-      <c r="S179" s="20">
+        <v>210</v>
+      </c>
+      <c r="T179" t="str">
         <f t="shared" si="317"/>
-        <v>210</v>
-      </c>
-      <c r="T179" t="str">
+        <v>static const CooGUI_tds Pos_SurfClearToUpdate_1_Flipped = {0,24,25,120,260,90,285,210};</v>
+      </c>
+      <c r="U179" t="str">
         <f t="shared" si="318"/>
-        <v>static const CooGUI_tds Pos_SurfClearToUpdate_1_Flipped = {0,24,25,120,260,90,285,210};</v>
-      </c>
-      <c r="U179" t="str">
+        <v>const CooGUI_tds* Pos_SurfClearToUpdate_1;</v>
+      </c>
+      <c r="V179">
         <f t="shared" si="319"/>
-        <v>const CooGUI_tds* Pos_SurfClearToUpdate_1;</v>
-      </c>
-      <c r="V179">
+        <v>22.8515625</v>
+      </c>
+      <c r="W179" t="str">
         <f t="shared" si="320"/>
-        <v>22.8515625</v>
-      </c>
-      <c r="W179" t="str">
-        <f t="shared" si="321"/>
         <v>Pos_SurfClearToUpdate_1 = &amp;Pos_SurfClearToUpdate_1_Normal;</v>
       </c>
     </row>
@@ -20192,7 +20192,7 @@
         <v>204</v>
       </c>
       <c r="B180" t="str">
-        <f t="shared" si="309"/>
+        <f t="shared" si="308"/>
         <v>Pos_SurfClearToUpdate_2_Normal</v>
       </c>
       <c r="C180" s="23">
@@ -20215,31 +20215,31 @@
         <v>30</v>
       </c>
       <c r="I180" s="20">
+        <f t="shared" si="309"/>
+        <v>320</v>
+      </c>
+      <c r="J180" s="20">
         <f t="shared" si="310"/>
-        <v>320</v>
-      </c>
-      <c r="J180" s="20">
+        <v>240</v>
+      </c>
+      <c r="K180" t="str">
         <f t="shared" si="311"/>
-        <v>240</v>
-      </c>
-      <c r="K180" t="str">
+        <v>static const CooGUI_tds Pos_SurfClearToUpdate_2_Normal = {0,0,0,210,320,30,320,240};</v>
+      </c>
+      <c r="L180">
         <f t="shared" si="312"/>
-        <v>static const CooGUI_tds Pos_SurfClearToUpdate_2_Normal = {0,0,0,210,320,30,320,240};</v>
-      </c>
-      <c r="L180">
+        <v>0</v>
+      </c>
+      <c r="M180" s="52">
+        <f t="shared" si="351"/>
+        <v>24</v>
+      </c>
+      <c r="N180">
         <f t="shared" si="313"/>
         <v>0</v>
       </c>
-      <c r="M180" s="52">
+      <c r="O180">
         <f t="shared" si="352"/>
-        <v>24</v>
-      </c>
-      <c r="N180">
-        <f t="shared" si="314"/>
-        <v>0</v>
-      </c>
-      <c r="O180">
-        <f t="shared" si="308"/>
         <v>210</v>
       </c>
       <c r="P180">
@@ -20247,31 +20247,31 @@
         <v>320</v>
       </c>
       <c r="Q180">
+        <f t="shared" si="314"/>
+        <v>30</v>
+      </c>
+      <c r="R180" s="20">
         <f t="shared" si="315"/>
-        <v>30</v>
-      </c>
-      <c r="R180" s="20">
+        <v>320</v>
+      </c>
+      <c r="S180" s="20">
         <f t="shared" si="316"/>
-        <v>320</v>
-      </c>
-      <c r="S180" s="20">
+        <v>240</v>
+      </c>
+      <c r="T180" t="str">
         <f t="shared" si="317"/>
-        <v>240</v>
-      </c>
-      <c r="T180" t="str">
+        <v>static const CooGUI_tds Pos_SurfClearToUpdate_2_Flipped = {0,24,0,210,320,30,320,240};</v>
+      </c>
+      <c r="U180" t="str">
         <f t="shared" si="318"/>
-        <v>static const CooGUI_tds Pos_SurfClearToUpdate_2_Flipped = {0,24,0,210,320,30,320,240};</v>
-      </c>
-      <c r="U180" t="str">
+        <v>const CooGUI_tds* Pos_SurfClearToUpdate_2;</v>
+      </c>
+      <c r="V180">
         <f t="shared" si="319"/>
-        <v>const CooGUI_tds* Pos_SurfClearToUpdate_2;</v>
-      </c>
-      <c r="V180">
+        <v>9.375</v>
+      </c>
+      <c r="W180" t="str">
         <f t="shared" si="320"/>
-        <v>9.375</v>
-      </c>
-      <c r="W180" t="str">
-        <f t="shared" si="321"/>
         <v>Pos_SurfClearToUpdate_2 = &amp;Pos_SurfClearToUpdate_2_Normal;</v>
       </c>
     </row>
@@ -20641,7 +20641,7 @@
         <v>214</v>
       </c>
       <c r="B185" t="str">
-        <f t="shared" si="309"/>
+        <f t="shared" si="308"/>
         <v>Pos_DiveMenu_DecoStop_PO2_Tittle_Normal</v>
       </c>
       <c r="C185" s="26">
@@ -20666,31 +20666,31 @@
         <v>20</v>
       </c>
       <c r="I185" s="20">
+        <f t="shared" si="309"/>
+        <v>320</v>
+      </c>
+      <c r="J185" s="20">
         <f t="shared" si="310"/>
-        <v>320</v>
-      </c>
-      <c r="J185" s="20">
+        <v>20</v>
+      </c>
+      <c r="K185" t="str">
         <f t="shared" si="311"/>
-        <v>20</v>
-      </c>
-      <c r="K185" t="str">
+        <v>static const CooGUI_tds Pos_DiveMenu_DecoStop_PO2_Tittle_Normal = {160,0,0,0,320,20,320,20};</v>
+      </c>
+      <c r="L185">
         <f t="shared" si="312"/>
-        <v>static const CooGUI_tds Pos_DiveMenu_DecoStop_PO2_Tittle_Normal = {160,0,0,0,320,20,320,20};</v>
-      </c>
-      <c r="L185">
+        <v>160</v>
+      </c>
+      <c r="M185" s="52">
+        <f t="shared" si="351"/>
+        <v>24</v>
+      </c>
+      <c r="N185">
         <f t="shared" si="313"/>
-        <v>160</v>
-      </c>
-      <c r="M185" s="52">
+        <v>0</v>
+      </c>
+      <c r="O185">
         <f t="shared" si="352"/>
-        <v>24</v>
-      </c>
-      <c r="N185">
-        <f t="shared" si="314"/>
-        <v>0</v>
-      </c>
-      <c r="O185">
-        <f t="shared" si="308"/>
         <v>0</v>
       </c>
       <c r="P185">
@@ -20698,31 +20698,31 @@
         <v>320</v>
       </c>
       <c r="Q185">
+        <f t="shared" si="314"/>
+        <v>20</v>
+      </c>
+      <c r="R185" s="20">
         <f t="shared" si="315"/>
+        <v>320</v>
+      </c>
+      <c r="S185" s="20">
+        <f t="shared" si="316"/>
         <v>20</v>
       </c>
-      <c r="R185" s="20">
-        <f t="shared" si="316"/>
-        <v>320</v>
-      </c>
-      <c r="S185" s="20">
+      <c r="T185" t="str">
         <f t="shared" si="317"/>
-        <v>20</v>
-      </c>
-      <c r="T185" t="str">
+        <v>static const CooGUI_tds Pos_DiveMenu_DecoStop_PO2_Tittle_Flipped = {160,24,0,0,320,20,320,20};</v>
+      </c>
+      <c r="U185" t="str">
         <f t="shared" si="318"/>
-        <v>static const CooGUI_tds Pos_DiveMenu_DecoStop_PO2_Tittle_Flipped = {160,24,0,0,320,20,320,20};</v>
-      </c>
-      <c r="U185" t="str">
+        <v>const CooGUI_tds* Pos_DiveMenu_DecoStop_PO2_Tittle;</v>
+      </c>
+      <c r="V185">
         <f t="shared" si="319"/>
-        <v>const CooGUI_tds* Pos_DiveMenu_DecoStop_PO2_Tittle;</v>
-      </c>
-      <c r="V185">
+        <v>6.25</v>
+      </c>
+      <c r="W185" t="str">
         <f t="shared" si="320"/>
-        <v>6.25</v>
-      </c>
-      <c r="W185" t="str">
-        <f t="shared" si="321"/>
         <v>Pos_DiveMenu_DecoStop_PO2_Tittle = &amp;Pos_DiveMenu_DecoStop_PO2_Tittle_Normal;</v>
       </c>
     </row>
@@ -20731,7 +20731,7 @@
         <v>215</v>
       </c>
       <c r="B186" t="str">
-        <f t="shared" si="309"/>
+        <f t="shared" si="308"/>
         <v>Pos_DiveMenu_DecoStop_PO2_Value_Normal</v>
       </c>
       <c r="C186" s="20">
@@ -20758,31 +20758,31 @@
         <v>40</v>
       </c>
       <c r="I186" s="20">
+        <f t="shared" si="309"/>
+        <v>320</v>
+      </c>
+      <c r="J186" s="20">
         <f t="shared" si="310"/>
-        <v>320</v>
-      </c>
-      <c r="J186" s="20">
+        <v>60</v>
+      </c>
+      <c r="K186" t="str">
         <f t="shared" si="311"/>
-        <v>60</v>
-      </c>
-      <c r="K186" t="str">
+        <v>static const CooGUI_tds Pos_DiveMenu_DecoStop_PO2_Value_Normal = {160,14,0,20,320,40,320,60};</v>
+      </c>
+      <c r="L186">
         <f t="shared" si="312"/>
-        <v>static const CooGUI_tds Pos_DiveMenu_DecoStop_PO2_Value_Normal = {160,14,0,20,320,40,320,60};</v>
-      </c>
-      <c r="L186">
+        <v>160</v>
+      </c>
+      <c r="M186" s="52">
+        <f t="shared" si="351"/>
+        <v>38</v>
+      </c>
+      <c r="N186">
         <f t="shared" si="313"/>
-        <v>160</v>
-      </c>
-      <c r="M186" s="52">
+        <v>0</v>
+      </c>
+      <c r="O186">
         <f t="shared" si="352"/>
-        <v>38</v>
-      </c>
-      <c r="N186">
-        <f t="shared" si="314"/>
-        <v>0</v>
-      </c>
-      <c r="O186">
-        <f t="shared" si="308"/>
         <v>20</v>
       </c>
       <c r="P186">
@@ -20790,31 +20790,31 @@
         <v>320</v>
       </c>
       <c r="Q186">
+        <f t="shared" si="314"/>
+        <v>40</v>
+      </c>
+      <c r="R186" s="20">
         <f t="shared" si="315"/>
-        <v>40</v>
-      </c>
-      <c r="R186" s="20">
+        <v>320</v>
+      </c>
+      <c r="S186" s="20">
         <f t="shared" si="316"/>
-        <v>320</v>
-      </c>
-      <c r="S186" s="20">
+        <v>60</v>
+      </c>
+      <c r="T186" t="str">
         <f t="shared" si="317"/>
-        <v>60</v>
-      </c>
-      <c r="T186" t="str">
+        <v>static const CooGUI_tds Pos_DiveMenu_DecoStop_PO2_Value_Flipped = {160,38,0,20,320,40,320,60};</v>
+      </c>
+      <c r="U186" t="str">
         <f t="shared" si="318"/>
-        <v>static const CooGUI_tds Pos_DiveMenu_DecoStop_PO2_Value_Flipped = {160,38,0,20,320,40,320,60};</v>
-      </c>
-      <c r="U186" t="str">
+        <v>const CooGUI_tds* Pos_DiveMenu_DecoStop_PO2_Value;</v>
+      </c>
+      <c r="V186">
         <f t="shared" si="319"/>
-        <v>const CooGUI_tds* Pos_DiveMenu_DecoStop_PO2_Value;</v>
-      </c>
-      <c r="V186">
+        <v>12.5</v>
+      </c>
+      <c r="W186" t="str">
         <f t="shared" si="320"/>
-        <v>12.5</v>
-      </c>
-      <c r="W186" t="str">
-        <f t="shared" si="321"/>
         <v>Pos_DiveMenu_DecoStop_PO2_Value = &amp;Pos_DiveMenu_DecoStop_PO2_Value_Normal;</v>
       </c>
     </row>
@@ -20823,7 +20823,7 @@
         <v>216</v>
       </c>
       <c r="B187" t="str">
-        <f t="shared" si="309"/>
+        <f t="shared" si="308"/>
         <v>Pos_DiveMenu_DecoStop_List_Normal</v>
       </c>
       <c r="C187" s="9">
@@ -20848,31 +20848,31 @@
         <v>26</v>
       </c>
       <c r="I187" s="20">
+        <f t="shared" si="309"/>
+        <v>320</v>
+      </c>
+      <c r="J187" s="20">
         <f t="shared" si="310"/>
-        <v>320</v>
-      </c>
-      <c r="J187" s="20">
+        <v>86</v>
+      </c>
+      <c r="K187" t="str">
         <f t="shared" si="311"/>
-        <v>86</v>
-      </c>
-      <c r="K187" t="str">
+        <v>static const CooGUI_tds Pos_DiveMenu_DecoStop_List_Normal = {0,60,0,60,320,26,320,86};</v>
+      </c>
+      <c r="L187">
         <f t="shared" si="312"/>
-        <v>static const CooGUI_tds Pos_DiveMenu_DecoStop_List_Normal = {0,60,0,60,320,26,320,86};</v>
-      </c>
-      <c r="L187">
+        <v>0</v>
+      </c>
+      <c r="M187" s="52">
+        <f t="shared" si="351"/>
+        <v>84</v>
+      </c>
+      <c r="N187">
         <f t="shared" si="313"/>
         <v>0</v>
       </c>
-      <c r="M187" s="52">
+      <c r="O187">
         <f t="shared" si="352"/>
-        <v>84</v>
-      </c>
-      <c r="N187">
-        <f t="shared" si="314"/>
-        <v>0</v>
-      </c>
-      <c r="O187">
-        <f t="shared" si="308"/>
         <v>60</v>
       </c>
       <c r="P187">
@@ -20880,31 +20880,31 @@
         <v>320</v>
       </c>
       <c r="Q187">
+        <f t="shared" si="314"/>
+        <v>26</v>
+      </c>
+      <c r="R187" s="20">
         <f t="shared" si="315"/>
-        <v>26</v>
-      </c>
-      <c r="R187" s="20">
+        <v>320</v>
+      </c>
+      <c r="S187" s="20">
         <f t="shared" si="316"/>
-        <v>320</v>
-      </c>
-      <c r="S187" s="20">
+        <v>86</v>
+      </c>
+      <c r="T187" t="str">
         <f t="shared" si="317"/>
-        <v>86</v>
-      </c>
-      <c r="T187" t="str">
+        <v>static const CooGUI_tds Pos_DiveMenu_DecoStop_List_Flipped = {0,84,0,60,320,26,320,86};</v>
+      </c>
+      <c r="U187" t="str">
         <f t="shared" si="318"/>
-        <v>static const CooGUI_tds Pos_DiveMenu_DecoStop_List_Flipped = {0,84,0,60,320,26,320,86};</v>
-      </c>
-      <c r="U187" t="str">
+        <v>const CooGUI_tds* Pos_DiveMenu_DecoStop_List;</v>
+      </c>
+      <c r="V187">
         <f t="shared" si="319"/>
-        <v>const CooGUI_tds* Pos_DiveMenu_DecoStop_List;</v>
-      </c>
-      <c r="V187">
+        <v>8.125</v>
+      </c>
+      <c r="W187" t="str">
         <f t="shared" si="320"/>
-        <v>8.125</v>
-      </c>
-      <c r="W187" t="str">
-        <f t="shared" si="321"/>
         <v>Pos_DiveMenu_DecoStop_List = &amp;Pos_DiveMenu_DecoStop_List_Normal;</v>
       </c>
     </row>
@@ -20913,7 +20913,7 @@
         <v>220</v>
       </c>
       <c r="B188" t="str">
-        <f t="shared" si="309"/>
+        <f t="shared" si="308"/>
         <v>Pos_DiveMenu_DecoStop_NODECO_Normal</v>
       </c>
       <c r="C188" s="35">
@@ -20939,31 +20939,31 @@
         <v>54</v>
       </c>
       <c r="I188" s="20">
+        <f t="shared" si="309"/>
+        <v>260</v>
+      </c>
+      <c r="J188" s="20">
         <f t="shared" si="310"/>
-        <v>260</v>
-      </c>
-      <c r="J188" s="20">
+        <v>164</v>
+      </c>
+      <c r="K188" t="str">
         <f t="shared" si="311"/>
-        <v>164</v>
-      </c>
-      <c r="K188" t="str">
+        <v>static const CooGUI_tds Pos_DiveMenu_DecoStop_NODECO_Normal = {160,100,60,110,200,54,260,164};</v>
+      </c>
+      <c r="L188">
         <f t="shared" si="312"/>
-        <v>static const CooGUI_tds Pos_DiveMenu_DecoStop_NODECO_Normal = {160,100,60,110,200,54,260,164};</v>
-      </c>
-      <c r="L188">
+        <v>160</v>
+      </c>
+      <c r="M188" s="52">
+        <f t="shared" si="351"/>
+        <v>124</v>
+      </c>
+      <c r="N188">
         <f t="shared" si="313"/>
-        <v>160</v>
-      </c>
-      <c r="M188" s="52">
+        <v>60</v>
+      </c>
+      <c r="O188">
         <f t="shared" si="352"/>
-        <v>124</v>
-      </c>
-      <c r="N188">
-        <f t="shared" si="314"/>
-        <v>60</v>
-      </c>
-      <c r="O188">
-        <f t="shared" si="308"/>
         <v>110</v>
       </c>
       <c r="P188">
@@ -20971,31 +20971,31 @@
         <v>200</v>
       </c>
       <c r="Q188">
+        <f t="shared" si="314"/>
+        <v>54</v>
+      </c>
+      <c r="R188" s="20">
         <f t="shared" si="315"/>
-        <v>54</v>
-      </c>
-      <c r="R188" s="20">
+        <v>260</v>
+      </c>
+      <c r="S188" s="20">
         <f t="shared" si="316"/>
-        <v>260</v>
-      </c>
-      <c r="S188" s="20">
+        <v>164</v>
+      </c>
+      <c r="T188" t="str">
         <f t="shared" si="317"/>
-        <v>164</v>
-      </c>
-      <c r="T188" t="str">
+        <v>static const CooGUI_tds Pos_DiveMenu_DecoStop_NODECO_Flipped = {160,124,60,110,200,54,260,164};</v>
+      </c>
+      <c r="U188" t="str">
         <f t="shared" si="318"/>
-        <v>static const CooGUI_tds Pos_DiveMenu_DecoStop_NODECO_Flipped = {160,124,60,110,200,54,260,164};</v>
-      </c>
-      <c r="U188" t="str">
+        <v>const CooGUI_tds* Pos_DiveMenu_DecoStop_NODECO;</v>
+      </c>
+      <c r="V188">
         <f t="shared" si="319"/>
-        <v>const CooGUI_tds* Pos_DiveMenu_DecoStop_NODECO;</v>
-      </c>
-      <c r="V188">
+        <v>10.546875</v>
+      </c>
+      <c r="W188" t="str">
         <f t="shared" si="320"/>
-        <v>10.546875</v>
-      </c>
-      <c r="W188" t="str">
-        <f t="shared" si="321"/>
         <v>Pos_DiveMenu_DecoStop_NODECO = &amp;Pos_DiveMenu_DecoStop_NODECO_Normal;</v>
       </c>
     </row>
@@ -21004,7 +21004,7 @@
         <v>301</v>
       </c>
       <c r="B189" t="str">
-        <f t="shared" si="309"/>
+        <f t="shared" si="308"/>
         <v>Pos_ALARM_BottomInOneLine_Normal</v>
       </c>
       <c r="C189" s="23">
@@ -21030,31 +21030,31 @@
         <v>60</v>
       </c>
       <c r="I189" s="20">
+        <f t="shared" si="309"/>
+        <v>295</v>
+      </c>
+      <c r="J189" s="20">
         <f t="shared" si="310"/>
-        <v>295</v>
-      </c>
-      <c r="J189" s="20">
+        <v>240</v>
+      </c>
+      <c r="K189" t="str">
         <f t="shared" si="311"/>
-        <v>240</v>
-      </c>
-      <c r="K189" t="str">
+        <v>static const CooGUI_tds Pos_ALARM_BottomInOneLine_Normal = {160,200,25,180,270,60,295,240};</v>
+      </c>
+      <c r="L189">
         <f t="shared" si="312"/>
-        <v>static const CooGUI_tds Pos_ALARM_BottomInOneLine_Normal = {160,200,25,180,270,60,295,240};</v>
-      </c>
-      <c r="L189">
+        <v>160</v>
+      </c>
+      <c r="M189" s="52">
+        <f t="shared" si="351"/>
+        <v>224</v>
+      </c>
+      <c r="N189">
         <f t="shared" si="313"/>
-        <v>160</v>
-      </c>
-      <c r="M189" s="52">
+        <v>25</v>
+      </c>
+      <c r="O189">
         <f t="shared" si="352"/>
-        <v>224</v>
-      </c>
-      <c r="N189">
-        <f t="shared" si="314"/>
-        <v>25</v>
-      </c>
-      <c r="O189">
-        <f t="shared" si="308"/>
         <v>180</v>
       </c>
       <c r="P189">
@@ -21062,31 +21062,31 @@
         <v>270</v>
       </c>
       <c r="Q189">
+        <f t="shared" si="314"/>
+        <v>60</v>
+      </c>
+      <c r="R189" s="20">
         <f t="shared" si="315"/>
-        <v>60</v>
-      </c>
-      <c r="R189" s="20">
+        <v>295</v>
+      </c>
+      <c r="S189" s="20">
         <f t="shared" si="316"/>
-        <v>295</v>
-      </c>
-      <c r="S189" s="20">
+        <v>240</v>
+      </c>
+      <c r="T189" t="str">
         <f t="shared" si="317"/>
-        <v>240</v>
-      </c>
-      <c r="T189" t="str">
+        <v>static const CooGUI_tds Pos_ALARM_BottomInOneLine_Flipped = {160,224,25,180,270,60,295,240};</v>
+      </c>
+      <c r="U189" t="str">
         <f t="shared" si="318"/>
-        <v>static const CooGUI_tds Pos_ALARM_BottomInOneLine_Flipped = {160,224,25,180,270,60,295,240};</v>
-      </c>
-      <c r="U189" t="str">
+        <v>const CooGUI_tds* Pos_ALARM_BottomInOneLine;</v>
+      </c>
+      <c r="V189">
         <f t="shared" si="319"/>
-        <v>const CooGUI_tds* Pos_ALARM_BottomInOneLine;</v>
-      </c>
-      <c r="V189">
+        <v>15.8203125</v>
+      </c>
+      <c r="W189" t="str">
         <f t="shared" si="320"/>
-        <v>15.8203125</v>
-      </c>
-      <c r="W189" t="str">
-        <f t="shared" si="321"/>
         <v>Pos_ALARM_BottomInOneLine = &amp;Pos_ALARM_BottomInOneLine_Normal;</v>
       </c>
     </row>
@@ -23338,7 +23338,7 @@
         <v>160</v>
       </c>
       <c r="M214" s="52">
-        <f t="shared" ref="M213:M218" si="624">D214 + $D$1</f>
+        <f t="shared" ref="M214:M218" si="624">D214 + $D$1</f>
         <v>234</v>
       </c>
       <c r="N214">
@@ -23427,47 +23427,47 @@
         <v>160</v>
       </c>
       <c r="M215" s="52">
-        <f t="shared" si="624"/>
-        <v>89</v>
+        <f>D215</f>
+        <v>65</v>
       </c>
       <c r="N215">
         <f t="shared" ref="N215" si="629">E215</f>
         <v>0</v>
       </c>
       <c r="O215">
-        <f t="shared" ref="O215" si="630">F215</f>
+        <f>F215</f>
         <v>70</v>
       </c>
       <c r="P215">
-        <f t="shared" ref="P215" si="631">G215</f>
+        <f t="shared" ref="P215" si="630">G215</f>
         <v>320</v>
       </c>
       <c r="Q215">
-        <f t="shared" ref="Q215" si="632">H215</f>
+        <f t="shared" ref="Q215" si="631">H215</f>
         <v>38</v>
       </c>
       <c r="R215" s="20">
-        <f t="shared" ref="R215" si="633">N215+P215</f>
+        <f t="shared" ref="R215" si="632">N215+P215</f>
         <v>320</v>
       </c>
       <c r="S215" s="20">
-        <f t="shared" ref="S215" si="634">O215+Q215</f>
+        <f t="shared" ref="S215" si="633">O215+Q215</f>
         <v>108</v>
       </c>
       <c r="T215" t="str">
-        <f t="shared" ref="T215" si="635">CONCATENATE("static const CooGUI_tds ",A215, "_Flipped = {", L215, ",", M215, ",", N215, ",", O215, ",",P215, ",", Q215,",",  R215, ",", S215, "};")</f>
-        <v>static const CooGUI_tds Pos_ErrorMsg_Line_0_Flipped = {160,89,0,70,320,38,320,108};</v>
+        <f t="shared" ref="T215" si="634">CONCATENATE("static const CooGUI_tds ",A215, "_Flipped = {", L215, ",", M215, ",", N215, ",", O215, ",",P215, ",", Q215,",",  R215, ",", S215, "};")</f>
+        <v>static const CooGUI_tds Pos_ErrorMsg_Line_0_Flipped = {160,65,0,70,320,38,320,108};</v>
       </c>
       <c r="U215" t="str">
-        <f t="shared" ref="U215" si="636">CONCATENATE("const CooGUI_tds* ",A215, ";")</f>
+        <f t="shared" ref="U215" si="635">CONCATENATE("const CooGUI_tds* ",A215, ";")</f>
         <v>const CooGUI_tds* Pos_ErrorMsg_Line_0;</v>
       </c>
       <c r="V215">
-        <f t="shared" ref="V215" si="637">(G215*H215)/1024</f>
+        <f t="shared" ref="V215" si="636">(G215*H215)/1024</f>
         <v>11.875</v>
       </c>
       <c r="W215" t="str">
-        <f t="shared" ref="W215" si="638">CONCATENATE(A215, " = &amp;", B215,";")</f>
+        <f t="shared" ref="W215" si="637">CONCATENATE(A215, " = &amp;", B215,";")</f>
         <v>Pos_ErrorMsg_Line_0 = &amp;Pos_ErrorMsg_Line_0_Normal;</v>
       </c>
     </row>
@@ -23476,7 +23476,7 @@
         <v>298</v>
       </c>
       <c r="B216" t="str">
-        <f t="shared" ref="B216:B217" si="639">CONCATENATE(A216, "_Normal")</f>
+        <f t="shared" ref="B216:B217" si="638">CONCATENATE(A216, "_Normal")</f>
         <v>Pos_ErrorMsg_Line_1_Normal</v>
       </c>
       <c r="C216" s="26">
@@ -23500,28 +23500,28 @@
         <v>320</v>
       </c>
       <c r="H216" s="50">
-        <f t="shared" ref="H216:H217" si="640">H215</f>
+        <f t="shared" ref="H216:H217" si="639">H215</f>
         <v>38</v>
       </c>
       <c r="I216" s="26">
-        <f t="shared" ref="I216:I217" si="641">E216+G216</f>
+        <f t="shared" ref="I216:I217" si="640">E216+G216</f>
         <v>320</v>
       </c>
       <c r="J216" s="26">
-        <f t="shared" ref="J216:J217" si="642">F216+H216</f>
+        <f t="shared" ref="J216:J217" si="641">F216+H216</f>
         <v>146</v>
       </c>
       <c r="K216" t="str">
-        <f t="shared" ref="K216:K217" si="643">CONCATENATE("static const CooGUI_tds ",A216, "_Normal = {", C216, ",", D216, ",", E216, ",", F216, ",",G216, ",", H216,",",  I216, ",", J216, "};")</f>
+        <f t="shared" ref="K216:K217" si="642">CONCATENATE("static const CooGUI_tds ",A216, "_Normal = {", C216, ",", D216, ",", E216, ",", F216, ",",G216, ",", H216,",",  I216, ",", J216, "};")</f>
         <v>static const CooGUI_tds Pos_ErrorMsg_Line_1_Normal = {160,103,0,108,320,38,320,146};</v>
       </c>
       <c r="L216">
-        <f t="shared" ref="L216:L217" si="644">C216</f>
+        <f t="shared" ref="L216:L217" si="643">C216</f>
         <v>160</v>
       </c>
       <c r="M216" s="52">
-        <f t="shared" si="624"/>
-        <v>127</v>
+        <f t="shared" ref="M216:M218" si="644">D216</f>
+        <v>103</v>
       </c>
       <c r="N216">
         <f t="shared" ref="N216:N217" si="645">E216</f>
@@ -23549,7 +23549,7 @@
       </c>
       <c r="T216" t="str">
         <f t="shared" ref="T216:T217" si="651">CONCATENATE("static const CooGUI_tds ",A216, "_Flipped = {", L216, ",", M216, ",", N216, ",", O216, ",",P216, ",", Q216,",",  R216, ",", S216, "};")</f>
-        <v>static const CooGUI_tds Pos_ErrorMsg_Line_1_Flipped = {160,127,0,108,320,38,320,146};</v>
+        <v>static const CooGUI_tds Pos_ErrorMsg_Line_1_Flipped = {160,103,0,108,320,38,320,146};</v>
       </c>
       <c r="U216" t="str">
         <f t="shared" ref="U216:U217" si="652">CONCATENATE("const CooGUI_tds* ",A216, ";")</f>
@@ -23569,7 +23569,7 @@
         <v>299</v>
       </c>
       <c r="B217" t="str">
-        <f t="shared" si="639"/>
+        <f t="shared" si="638"/>
         <v>Pos_ErrorMsg_Line_2_Normal</v>
       </c>
       <c r="C217" s="26">
@@ -23593,28 +23593,28 @@
         <v>320</v>
       </c>
       <c r="H217" s="50">
+        <f t="shared" si="639"/>
+        <v>38</v>
+      </c>
+      <c r="I217" s="26">
         <f t="shared" si="640"/>
-        <v>38</v>
-      </c>
-      <c r="I217" s="26">
+        <v>320</v>
+      </c>
+      <c r="J217" s="26">
         <f t="shared" si="641"/>
-        <v>320</v>
-      </c>
-      <c r="J217" s="26">
+        <v>184</v>
+      </c>
+      <c r="K217" t="str">
         <f t="shared" si="642"/>
-        <v>184</v>
-      </c>
-      <c r="K217" t="str">
+        <v>static const CooGUI_tds Pos_ErrorMsg_Line_2_Normal = {160,141,0,146,320,38,320,184};</v>
+      </c>
+      <c r="L217">
         <f t="shared" si="643"/>
-        <v>static const CooGUI_tds Pos_ErrorMsg_Line_2_Normal = {160,141,0,146,320,38,320,184};</v>
-      </c>
-      <c r="L217">
+        <v>160</v>
+      </c>
+      <c r="M217" s="52">
         <f t="shared" si="644"/>
-        <v>160</v>
-      </c>
-      <c r="M217" s="52">
-        <f t="shared" si="624"/>
-        <v>165</v>
+        <v>141</v>
       </c>
       <c r="N217">
         <f t="shared" si="645"/>
@@ -23642,7 +23642,7 @@
       </c>
       <c r="T217" t="str">
         <f t="shared" si="651"/>
-        <v>static const CooGUI_tds Pos_ErrorMsg_Line_2_Flipped = {160,165,0,146,320,38,320,184};</v>
+        <v>static const CooGUI_tds Pos_ErrorMsg_Line_2_Flipped = {160,141,0,146,320,38,320,184};</v>
       </c>
       <c r="U217" t="str">
         <f t="shared" si="652"/>
@@ -23706,8 +23706,8 @@
         <v>160</v>
       </c>
       <c r="M218" s="52">
-        <f t="shared" si="624"/>
-        <v>203</v>
+        <f t="shared" si="644"/>
+        <v>179</v>
       </c>
       <c r="N218">
         <f t="shared" ref="N218" si="668">E218</f>
@@ -23735,7 +23735,7 @@
       </c>
       <c r="T218" t="str">
         <f t="shared" ref="T218" si="674">CONCATENATE("static const CooGUI_tds ",A218, "_Flipped = {", L218, ",", M218, ",", N218, ",", O218, ",",P218, ",", Q218,",",  R218, ",", S218, "};")</f>
-        <v>static const CooGUI_tds Pos_ErrorMsg_Line_3_Flipped = {160,203,0,184,320,38,320,222};</v>
+        <v>static const CooGUI_tds Pos_ErrorMsg_Line_3_Flipped = {160,179,0,184,320,38,320,222};</v>
       </c>
       <c r="U218" t="str">
         <f t="shared" ref="U218" si="675">CONCATENATE("const CooGUI_tds* ",A218, ";")</f>

</xml_diff>